<commit_message>
Wizard activities and conditions, Spell Combination
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Documents/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="598" documentId="13_ncr:4000b_{E48AABDC-DD04-4615-8145-6641F89B4174}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B161FE1F-436B-47E3-8D2B-2CDE07B7D28D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B287601-E85E-484D-A717-8764212CCAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">activities!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">activities!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="708">
   <si>
     <t>name</t>
   </si>
@@ -2171,6 +2171,64 @@
   </si>
   <si>
     <t>You’ve learned how to cast many of your spells without speaking the words of power you would normally need to provide. If the next action you use is Casting a Spell that has a verbal component and at least one other component, you can remove the verbal component. This makes the spell quieter and allows you to cast it in areas where sound can’t carry. However, the spell still has visual manifestations, so this doesn’t make the spell any less obvious to someone who sees you casting it. When you use Silent Spell, you can choose to gain the benefits of Conceal Spell, and you don’t need to attempt a Deception check because the spell has no verbal components.</t>
+  </si>
+  <si>
+    <t>Bond Conservation</t>
+  </si>
+  <si>
+    <t>Overwhelming Energy</t>
+  </si>
+  <si>
+    <t>Quickened Casting</t>
+  </si>
+  <si>
+    <t>Magic Sense</t>
+  </si>
+  <si>
+    <t>Effortless Concentration</t>
+  </si>
+  <si>
+    <t>Spell Tinker</t>
+  </si>
+  <si>
+    <t>The last action you used was Drain Bonded Item.</t>
+  </si>
+  <si>
+    <t>By carefully manipulating the arcane energies stored in your bonded item as you drain it, you can conserve just enough power to cast another, slightly weaker spell. If the next action you use is to Cast a Spell using the energy from Drain Bonded Item, you gain an extra use of Drain Bonded Item. You must use this extra use of Drain Bonded Item before the end of your next turn or you lose it, and you can use this additional use only to cast a spell 2 or more levels lower than the first spell cast with Drain Bonded Item.</t>
+  </si>
+  <si>
+    <t>You alter your spells to overcome resistances. If the next action you use is to Cast a Spell, the spell ignores an amount of the target’s resistance to acid, cold, electricity, fire, or sonic damage equal to your level. This applies to all damage the spell deals, including persistent damage and damage caused by an ongoing effect of the spell, such as the wall created by wall of fire. A creature’s immunities are unaffected.</t>
+  </si>
+  <si>
+    <t>If your next action is to cast a cantrip or a spell that is at least 2 levels lower than the highest level spell you can cast, reduce the number of actions to cast it by 1 (minimum 1 action).</t>
+  </si>
+  <si>
+    <t>This can only be used on a cantrip or spell from the class matching the one you gained this feat from.</t>
+  </si>
+  <si>
+    <t>You have a literal sixth sense for ambient magic in your vicinity. You can sense the presence of magic auras as though you were always using a 1st-level detect magic spell. This detects magic in your field of vision only. When you Seek, you gain the benefits of a 3rd-level detect magic spell on things you see (in addition to the normal benefits of Seeking). You can turn this sense off and on with a free action at the start or the end of your turn.</t>
+  </si>
+  <si>
+    <t>Detection</t>
+  </si>
+  <si>
+    <t>Divination</t>
+  </si>
+  <si>
+    <t>Your turn begins or ends.</t>
+  </si>
+  <si>
+    <t>You maintain a spell with hardly a thought. You immediately gain the effects of the Sustain a Spell action, allowing you to extend the duration of one of your active class spells.</t>
+  </si>
+  <si>
+    <t>Your turn begins.</t>
+  </si>
+  <si>
+    <t>You’ve learned to alter choices you make when casting spells on yourself. After casting a spell on only yourself that offers several choices of effect (such as resist energy, spell immunity, or a polymorph spell that offers several potential forms), you can alter the choice you made when Casting the Spell (for instance, choosing a different type of damage for resist energy). However, your tinkering weakens the spell’s integrity, reducing its remaining duration by half.
+You can’t use this feat if the benefits of the spell have already been used up or if the effects of the first choice would persist in any way after switching (for instance, if one of the choices was to create a consumable item you already used, or to heal you), or if the feat would create an effect more powerful than that offered by the base spell. The GM is the final arbiter of what Spell Tinker can be applied to.</t>
+  </si>
+  <si>
+    <t>For spells where the chosen effect makes a mechanical difference, you can select the alternative condition from the conditions menu and set the duration appropriately before removing the original condition.</t>
   </si>
 </sst>
 </file>
@@ -2654,7 +2712,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="35"/>
@@ -2662,6 +2720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="35" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2707,27 +2766,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3118,16 +3157,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M208"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3138,68 +3179,94 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>529</v>
+      </c>
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>663</v>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>689</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2" t="s">
-        <v>673</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="H2"/>
+        <v>695</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2" s="1" t="s">
+        <v>696</v>
+      </c>
       <c r="I2"/>
-      <c r="J2"/>
+      <c r="J2">
+        <v>15</v>
+      </c>
       <c r="K2" t="s">
-        <v>675</v>
+        <v>689</v>
       </c>
       <c r="L2" t="s">
-        <v>310</v>
-      </c>
-      <c r="M2" t="s">
+        <v>689</v>
+      </c>
+      <c r="M2"/>
+      <c r="N2" t="s">
+        <v>147</v>
+      </c>
+      <c r="O2" t="s">
+        <v>320</v>
+      </c>
+      <c r="P2" t="s">
         <v>311</v>
       </c>
+      <c r="Q2"/>
+      <c r="R2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>664</v>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>690</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -3208,3206 +3275,193 @@
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3"/>
-      <c r="G3" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="H3"/>
+      <c r="G3"/>
+      <c r="H3" s="1" t="s">
+        <v>697</v>
+      </c>
       <c r="I3"/>
       <c r="J3"/>
-      <c r="K3" t="s">
-        <v>144</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3" t="s">
+        <v>319</v>
+      </c>
+      <c r="O3" t="s">
         <v>147</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>320</v>
       </c>
+      <c r="Q3" t="s">
+        <v>321</v>
+      </c>
+      <c r="R3" t="s">
+        <v>311</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>665</v>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>691</v>
       </c>
       <c r="B4" t="s">
         <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>677</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>679</v>
+        <v>179</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4">
+        <v>144000</v>
       </c>
       <c r="F4"/>
-      <c r="G4" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
+      <c r="G4"/>
+      <c r="H4" t="s">
+        <v>698</v>
       </c>
       <c r="I4" t="s">
-        <v>665</v>
-      </c>
-      <c r="J4" t="s">
-        <v>665</v>
-      </c>
-      <c r="K4" t="s">
+        <v>699</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4" t="s">
+        <v>323</v>
+      </c>
+      <c r="O4" t="s">
+        <v>144</v>
+      </c>
+      <c r="P4" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q4" t="s">
         <v>321</v>
       </c>
-      <c r="L4" t="s">
+      <c r="R4" t="s">
         <v>311</v>
       </c>
-      <c r="M4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>666</v>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>692</v>
       </c>
       <c r="B5" t="s">
         <v>124</v>
       </c>
-      <c r="C5" t="s">
-        <v>677</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>681</v>
-      </c>
+      <c r="C5"/>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5"/>
       <c r="F5"/>
-      <c r="G5" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5" t="s">
-        <v>666</v>
-      </c>
-      <c r="J5" t="s">
-        <v>666</v>
+      <c r="G5" t="s">
+        <v>703</v>
+      </c>
+      <c r="H5" t="s">
+        <v>700</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5">
+        <v>-1</v>
       </c>
       <c r="K5" t="s">
+        <v>692</v>
+      </c>
+      <c r="L5" t="s">
+        <v>692</v>
+      </c>
+      <c r="M5"/>
+      <c r="N5" t="s">
+        <v>701</v>
+      </c>
+      <c r="O5" t="s">
+        <v>702</v>
+      </c>
+      <c r="P5" t="s">
         <v>321</v>
       </c>
-      <c r="L5" t="s">
+      <c r="Q5" t="s">
         <v>311</v>
       </c>
-      <c r="M5"/>
+      <c r="R5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>667</v>
-      </c>
-      <c r="B6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" t="s">
-        <v>677</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>682</v>
-      </c>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
       <c r="F6"/>
-      <c r="G6" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6" t="s">
-        <v>667</v>
-      </c>
-      <c r="J6" t="s">
-        <v>667</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="G6" t="s">
+        <v>705</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6" t="s">
+        <v>323</v>
+      </c>
+      <c r="O6" t="s">
+        <v>319</v>
+      </c>
+      <c r="P6" t="s">
         <v>321</v>
       </c>
-      <c r="L6" t="s">
+      <c r="Q6" t="s">
         <v>311</v>
       </c>
-      <c r="M6"/>
+      <c r="R6"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>668</v>
-      </c>
-      <c r="B7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" t="s">
-        <v>677</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>684</v>
-      </c>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
       <c r="F7"/>
-      <c r="G7" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>668</v>
-      </c>
-      <c r="J7" t="s">
-        <v>668</v>
-      </c>
-      <c r="K7" t="s">
-        <v>321</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="G7"/>
+      <c r="H7" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7" t="s">
+        <v>707</v>
+      </c>
+      <c r="N7" t="s">
+        <v>144</v>
+      </c>
+      <c r="O7" t="s">
         <v>311</v>
       </c>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>669</v>
-      </c>
-      <c r="B8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" t="s">
-        <v>677</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>686</v>
-      </c>
-      <c r="F8"/>
-      <c r="G8" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-      <c r="I8" t="s">
-        <v>669</v>
-      </c>
-      <c r="J8" t="s">
-        <v>669</v>
-      </c>
-      <c r="K8" t="s">
-        <v>321</v>
-      </c>
-      <c r="L8" t="s">
-        <v>311</v>
-      </c>
-      <c r="M8"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>670</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9" t="s">
-        <v>144</v>
-      </c>
-      <c r="L9" t="s">
-        <v>320</v>
-      </c>
-      <c r="M9" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
-      <c r="J27"/>
-      <c r="K27"/>
-      <c r="L27"/>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="G42"/>
-      <c r="H42"/>
-      <c r="I42"/>
-      <c r="J42"/>
-      <c r="K42"/>
-      <c r="L42"/>
-      <c r="M42"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
-      <c r="I43"/>
-      <c r="J43"/>
-      <c r="K43"/>
-      <c r="L43"/>
-      <c r="M43"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="K44"/>
-      <c r="L44"/>
-      <c r="M44"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-      <c r="D45"/>
-      <c r="E45"/>
-      <c r="F45"/>
-      <c r="G45"/>
-      <c r="H45"/>
-      <c r="I45"/>
-      <c r="J45"/>
-      <c r="K45"/>
-      <c r="L45"/>
-      <c r="M45"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="M46"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-      <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
-      <c r="M47"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
-      <c r="M48"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
-      <c r="F49"/>
-      <c r="G49"/>
-      <c r="H49"/>
-      <c r="I49"/>
-      <c r="J49"/>
-      <c r="K49"/>
-      <c r="L49"/>
-      <c r="M49"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
-      <c r="G50"/>
-      <c r="H50"/>
-      <c r="I50"/>
-      <c r="J50"/>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-      <c r="B51"/>
-      <c r="C51"/>
-      <c r="D51"/>
-      <c r="E51"/>
-      <c r="F51"/>
-      <c r="G51"/>
-      <c r="H51"/>
-      <c r="I51"/>
-      <c r="J51"/>
-      <c r="K51"/>
-      <c r="L51"/>
-      <c r="M51"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52"/>
-      <c r="B52"/>
-      <c r="C52"/>
-      <c r="D52"/>
-      <c r="E52"/>
-      <c r="F52"/>
-      <c r="G52"/>
-      <c r="H52"/>
-      <c r="I52"/>
-      <c r="J52"/>
-      <c r="K52"/>
-      <c r="L52"/>
-      <c r="M52"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53"/>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-      <c r="F53"/>
-      <c r="G53"/>
-      <c r="H53"/>
-      <c r="I53"/>
-      <c r="J53"/>
-      <c r="K53"/>
-      <c r="L53"/>
-      <c r="M53"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-      <c r="F54"/>
-      <c r="G54"/>
-      <c r="H54"/>
-      <c r="I54"/>
-      <c r="J54"/>
-      <c r="K54"/>
-      <c r="L54"/>
-      <c r="M54"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55"/>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
-      <c r="J55"/>
-      <c r="K55"/>
-      <c r="L55"/>
-      <c r="M55"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
-      <c r="J56"/>
-      <c r="K56"/>
-      <c r="L56"/>
-      <c r="M56"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57"/>
-      <c r="B57"/>
-      <c r="C57"/>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
-      <c r="G57"/>
-      <c r="H57"/>
-      <c r="I57"/>
-      <c r="J57"/>
-      <c r="K57"/>
-      <c r="L57"/>
-      <c r="M57"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58"/>
-      <c r="D58"/>
-      <c r="E58"/>
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
-      <c r="J58"/>
-      <c r="K58"/>
-      <c r="L58"/>
-      <c r="M58"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59"/>
-      <c r="D59"/>
-      <c r="E59"/>
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
-      <c r="J59"/>
-      <c r="K59"/>
-      <c r="L59"/>
-      <c r="M59"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
-      <c r="J60"/>
-      <c r="K60"/>
-      <c r="L60"/>
-      <c r="M60"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
-      <c r="J61"/>
-      <c r="K61"/>
-      <c r="L61"/>
-      <c r="M61"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
-      <c r="J62"/>
-      <c r="K62"/>
-      <c r="L62"/>
-      <c r="M62"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-      <c r="I63"/>
-      <c r="J63"/>
-      <c r="K63"/>
-      <c r="L63"/>
-      <c r="M63"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="D64"/>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64"/>
-      <c r="I64"/>
-      <c r="J64"/>
-      <c r="K64"/>
-      <c r="L64"/>
-      <c r="M64"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-      <c r="G65"/>
-      <c r="H65"/>
-      <c r="I65"/>
-      <c r="J65"/>
-      <c r="K65"/>
-      <c r="L65"/>
-      <c r="M65"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-      <c r="I66"/>
-      <c r="J66"/>
-      <c r="K66"/>
-      <c r="L66"/>
-      <c r="M66"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="D67"/>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
-      <c r="I67"/>
-      <c r="J67"/>
-      <c r="K67"/>
-      <c r="L67"/>
-      <c r="M67"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="D68"/>
-      <c r="E68"/>
-      <c r="F68"/>
-      <c r="G68"/>
-      <c r="H68"/>
-      <c r="I68"/>
-      <c r="J68"/>
-      <c r="K68"/>
-      <c r="L68"/>
-      <c r="M68"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
-      <c r="D69"/>
-      <c r="E69"/>
-      <c r="F69"/>
-      <c r="G69"/>
-      <c r="H69"/>
-      <c r="I69"/>
-      <c r="J69"/>
-      <c r="K69"/>
-      <c r="L69"/>
-      <c r="M69"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="D70"/>
-      <c r="E70"/>
-      <c r="F70"/>
-      <c r="G70"/>
-      <c r="H70"/>
-      <c r="I70"/>
-      <c r="J70"/>
-      <c r="K70"/>
-      <c r="L70"/>
-      <c r="M70"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71"/>
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71"/>
-      <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71"/>
-      <c r="I71"/>
-      <c r="J71"/>
-      <c r="K71"/>
-      <c r="L71"/>
-      <c r="M71"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72"/>
-      <c r="B72"/>
-      <c r="C72"/>
-      <c r="D72"/>
-      <c r="E72"/>
-      <c r="F72"/>
-      <c r="G72"/>
-      <c r="H72"/>
-      <c r="I72"/>
-      <c r="J72"/>
-      <c r="K72"/>
-      <c r="L72"/>
-      <c r="M72"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73"/>
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="D73"/>
-      <c r="E73"/>
-      <c r="F73"/>
-      <c r="G73"/>
-      <c r="H73"/>
-      <c r="I73"/>
-      <c r="J73"/>
-      <c r="K73"/>
-      <c r="L73"/>
-      <c r="M73"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74"/>
-      <c r="B74"/>
-      <c r="C74"/>
-      <c r="D74"/>
-      <c r="E74"/>
-      <c r="F74"/>
-      <c r="G74"/>
-      <c r="H74"/>
-      <c r="I74"/>
-      <c r="J74"/>
-      <c r="K74"/>
-      <c r="L74"/>
-      <c r="M74"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75"/>
-      <c r="B75"/>
-      <c r="C75"/>
-      <c r="D75"/>
-      <c r="E75"/>
-      <c r="F75"/>
-      <c r="G75"/>
-      <c r="H75"/>
-      <c r="I75"/>
-      <c r="J75"/>
-      <c r="K75"/>
-      <c r="L75"/>
-      <c r="M75"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76"/>
-      <c r="B76"/>
-      <c r="C76"/>
-      <c r="D76"/>
-      <c r="E76"/>
-      <c r="F76"/>
-      <c r="G76"/>
-      <c r="H76"/>
-      <c r="I76"/>
-      <c r="J76"/>
-      <c r="K76"/>
-      <c r="L76"/>
-      <c r="M76"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77"/>
-      <c r="B77"/>
-      <c r="C77"/>
-      <c r="D77"/>
-      <c r="E77"/>
-      <c r="F77"/>
-      <c r="G77"/>
-      <c r="H77"/>
-      <c r="I77"/>
-      <c r="J77"/>
-      <c r="K77"/>
-      <c r="L77"/>
-      <c r="M77"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78"/>
-      <c r="B78"/>
-      <c r="C78"/>
-      <c r="D78"/>
-      <c r="E78"/>
-      <c r="F78"/>
-      <c r="G78"/>
-      <c r="H78"/>
-      <c r="I78"/>
-      <c r="J78"/>
-      <c r="K78"/>
-      <c r="L78"/>
-      <c r="M78"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79"/>
-      <c r="B79"/>
-      <c r="C79"/>
-      <c r="D79"/>
-      <c r="E79"/>
-      <c r="F79"/>
-      <c r="G79"/>
-      <c r="H79"/>
-      <c r="I79"/>
-      <c r="J79"/>
-      <c r="K79"/>
-      <c r="L79"/>
-      <c r="M79"/>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80"/>
-      <c r="B80"/>
-      <c r="C80"/>
-      <c r="D80"/>
-      <c r="E80"/>
-      <c r="F80"/>
-      <c r="G80"/>
-      <c r="H80"/>
-      <c r="I80"/>
-      <c r="J80"/>
-      <c r="K80"/>
-      <c r="L80"/>
-      <c r="M80"/>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81"/>
-      <c r="B81"/>
-      <c r="C81"/>
-      <c r="D81"/>
-      <c r="E81"/>
-      <c r="F81"/>
-      <c r="G81"/>
-      <c r="H81"/>
-      <c r="I81"/>
-      <c r="J81"/>
-      <c r="K81"/>
-      <c r="L81"/>
-      <c r="M81"/>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82"/>
-      <c r="B82"/>
-      <c r="C82"/>
-      <c r="D82"/>
-      <c r="E82"/>
-      <c r="F82"/>
-      <c r="G82"/>
-      <c r="H82"/>
-      <c r="I82"/>
-      <c r="J82"/>
-      <c r="K82"/>
-      <c r="L82"/>
-      <c r="M82"/>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A83"/>
-      <c r="B83"/>
-      <c r="C83"/>
-      <c r="D83"/>
-      <c r="E83"/>
-      <c r="F83"/>
-      <c r="G83"/>
-      <c r="H83"/>
-      <c r="I83"/>
-      <c r="J83"/>
-      <c r="K83"/>
-      <c r="L83"/>
-      <c r="M83"/>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A84"/>
-      <c r="B84"/>
-      <c r="C84"/>
-      <c r="D84"/>
-      <c r="E84"/>
-      <c r="F84"/>
-      <c r="G84"/>
-      <c r="H84"/>
-      <c r="I84"/>
-      <c r="J84"/>
-      <c r="K84"/>
-      <c r="L84"/>
-      <c r="M84"/>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A85"/>
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85"/>
-      <c r="E85"/>
-      <c r="F85"/>
-      <c r="G85"/>
-      <c r="H85"/>
-      <c r="I85"/>
-      <c r="J85"/>
-      <c r="K85"/>
-      <c r="L85"/>
-      <c r="M85"/>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86"/>
-      <c r="B86"/>
-      <c r="C86"/>
-      <c r="D86"/>
-      <c r="E86"/>
-      <c r="F86"/>
-      <c r="G86"/>
-      <c r="H86"/>
-      <c r="I86"/>
-      <c r="J86"/>
-      <c r="K86"/>
-      <c r="L86"/>
-      <c r="M86"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87"/>
-      <c r="B87"/>
-      <c r="C87"/>
-      <c r="D87"/>
-      <c r="E87"/>
-      <c r="F87"/>
-      <c r="G87"/>
-      <c r="H87"/>
-      <c r="I87"/>
-      <c r="J87"/>
-      <c r="K87"/>
-      <c r="L87"/>
-      <c r="M87"/>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88"/>
-      <c r="B88"/>
-      <c r="C88"/>
-      <c r="D88"/>
-      <c r="E88"/>
-      <c r="F88"/>
-      <c r="G88"/>
-      <c r="H88"/>
-      <c r="I88"/>
-      <c r="J88"/>
-      <c r="K88"/>
-      <c r="L88"/>
-      <c r="M88"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89"/>
-      <c r="B89"/>
-      <c r="C89"/>
-      <c r="D89"/>
-      <c r="E89"/>
-      <c r="F89"/>
-      <c r="G89"/>
-      <c r="H89"/>
-      <c r="I89"/>
-      <c r="J89"/>
-      <c r="K89"/>
-      <c r="L89"/>
-      <c r="M89"/>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90"/>
-      <c r="B90"/>
-      <c r="C90"/>
-      <c r="D90"/>
-      <c r="E90"/>
-      <c r="F90"/>
-      <c r="G90"/>
-      <c r="H90"/>
-      <c r="I90"/>
-      <c r="J90"/>
-      <c r="K90"/>
-      <c r="L90"/>
-      <c r="M90"/>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91"/>
-      <c r="B91"/>
-      <c r="C91"/>
-      <c r="D91"/>
-      <c r="E91"/>
-      <c r="F91"/>
-      <c r="G91"/>
-      <c r="H91"/>
-      <c r="I91"/>
-      <c r="J91"/>
-      <c r="K91"/>
-      <c r="L91"/>
-      <c r="M91"/>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A92"/>
-      <c r="B92"/>
-      <c r="C92"/>
-      <c r="D92"/>
-      <c r="E92"/>
-      <c r="F92"/>
-      <c r="G92"/>
-      <c r="H92"/>
-      <c r="I92"/>
-      <c r="J92"/>
-      <c r="K92"/>
-      <c r="L92"/>
-      <c r="M92"/>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93"/>
-      <c r="B93"/>
-      <c r="C93"/>
-      <c r="D93"/>
-      <c r="E93"/>
-      <c r="F93"/>
-      <c r="G93"/>
-      <c r="H93"/>
-      <c r="I93"/>
-      <c r="J93"/>
-      <c r="K93"/>
-      <c r="L93"/>
-      <c r="M93"/>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94"/>
-      <c r="B94"/>
-      <c r="C94"/>
-      <c r="D94"/>
-      <c r="E94"/>
-      <c r="F94"/>
-      <c r="G94"/>
-      <c r="H94"/>
-      <c r="I94"/>
-      <c r="J94"/>
-      <c r="K94"/>
-      <c r="L94"/>
-      <c r="M94"/>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A95"/>
-      <c r="B95"/>
-      <c r="C95"/>
-      <c r="D95"/>
-      <c r="E95"/>
-      <c r="F95"/>
-      <c r="G95"/>
-      <c r="H95"/>
-      <c r="I95"/>
-      <c r="J95"/>
-      <c r="K95"/>
-      <c r="L95"/>
-      <c r="M95"/>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96"/>
-      <c r="B96"/>
-      <c r="C96"/>
-      <c r="D96"/>
-      <c r="E96"/>
-      <c r="F96"/>
-      <c r="G96"/>
-      <c r="H96"/>
-      <c r="I96"/>
-      <c r="J96"/>
-      <c r="K96"/>
-      <c r="L96"/>
-      <c r="M96"/>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A97"/>
-      <c r="B97"/>
-      <c r="C97"/>
-      <c r="D97"/>
-      <c r="E97"/>
-      <c r="F97"/>
-      <c r="G97"/>
-      <c r="H97"/>
-      <c r="I97"/>
-      <c r="J97"/>
-      <c r="K97"/>
-      <c r="L97"/>
-      <c r="M97"/>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A98"/>
-      <c r="B98"/>
-      <c r="C98"/>
-      <c r="D98"/>
-      <c r="E98"/>
-      <c r="F98"/>
-      <c r="G98"/>
-      <c r="H98"/>
-      <c r="I98"/>
-      <c r="J98"/>
-      <c r="K98"/>
-      <c r="L98"/>
-      <c r="M98"/>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A99"/>
-      <c r="B99"/>
-      <c r="C99"/>
-      <c r="D99"/>
-      <c r="E99"/>
-      <c r="F99"/>
-      <c r="G99"/>
-      <c r="H99"/>
-      <c r="I99"/>
-      <c r="J99"/>
-      <c r="K99"/>
-      <c r="L99"/>
-      <c r="M99"/>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="C100"/>
-      <c r="D100"/>
-      <c r="E100"/>
-      <c r="F100"/>
-      <c r="G100"/>
-      <c r="H100"/>
-      <c r="I100"/>
-      <c r="J100"/>
-      <c r="K100"/>
-      <c r="L100"/>
-      <c r="M100"/>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="C101"/>
-      <c r="D101"/>
-      <c r="E101"/>
-      <c r="F101"/>
-      <c r="G101"/>
-      <c r="H101"/>
-      <c r="I101"/>
-      <c r="J101"/>
-      <c r="K101"/>
-      <c r="L101"/>
-      <c r="M101"/>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102"/>
-      <c r="D102"/>
-      <c r="E102"/>
-      <c r="F102"/>
-      <c r="G102"/>
-      <c r="H102"/>
-      <c r="I102"/>
-      <c r="J102"/>
-      <c r="K102"/>
-      <c r="L102"/>
-      <c r="M102"/>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
-      <c r="D103"/>
-      <c r="E103"/>
-      <c r="F103"/>
-      <c r="G103"/>
-      <c r="H103"/>
-      <c r="I103"/>
-      <c r="J103"/>
-      <c r="K103"/>
-      <c r="L103"/>
-      <c r="M103"/>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104"/>
-      <c r="D104"/>
-      <c r="E104"/>
-      <c r="F104"/>
-      <c r="G104"/>
-      <c r="H104"/>
-      <c r="I104"/>
-      <c r="J104"/>
-      <c r="K104"/>
-      <c r="L104"/>
-      <c r="M104"/>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="C105"/>
-      <c r="D105"/>
-      <c r="E105"/>
-      <c r="F105"/>
-      <c r="G105"/>
-      <c r="H105"/>
-      <c r="I105"/>
-      <c r="J105"/>
-      <c r="K105"/>
-      <c r="L105"/>
-      <c r="M105"/>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A106"/>
-      <c r="B106"/>
-      <c r="C106"/>
-      <c r="D106"/>
-      <c r="E106"/>
-      <c r="F106"/>
-      <c r="G106"/>
-      <c r="H106"/>
-      <c r="I106"/>
-      <c r="J106"/>
-      <c r="K106"/>
-      <c r="L106"/>
-      <c r="M106"/>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A107"/>
-      <c r="B107"/>
-      <c r="C107"/>
-      <c r="D107"/>
-      <c r="E107"/>
-      <c r="F107"/>
-      <c r="G107"/>
-      <c r="H107"/>
-      <c r="I107"/>
-      <c r="J107"/>
-      <c r="K107"/>
-      <c r="L107"/>
-      <c r="M107"/>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A108"/>
-      <c r="B108"/>
-      <c r="C108"/>
-      <c r="D108"/>
-      <c r="E108"/>
-      <c r="F108"/>
-      <c r="G108"/>
-      <c r="H108"/>
-      <c r="I108"/>
-      <c r="J108"/>
-      <c r="K108"/>
-      <c r="L108"/>
-      <c r="M108"/>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A109"/>
-      <c r="B109"/>
-      <c r="C109"/>
-      <c r="D109"/>
-      <c r="E109"/>
-      <c r="F109"/>
-      <c r="G109"/>
-      <c r="H109"/>
-      <c r="I109"/>
-      <c r="J109"/>
-      <c r="K109"/>
-      <c r="L109"/>
-      <c r="M109"/>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A110"/>
-      <c r="B110"/>
-      <c r="C110"/>
-      <c r="D110"/>
-      <c r="E110"/>
-      <c r="F110"/>
-      <c r="G110"/>
-      <c r="H110"/>
-      <c r="I110"/>
-      <c r="J110"/>
-      <c r="K110"/>
-      <c r="L110"/>
-      <c r="M110"/>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A111"/>
-      <c r="B111"/>
-      <c r="C111"/>
-      <c r="D111"/>
-      <c r="E111"/>
-      <c r="F111"/>
-      <c r="G111"/>
-      <c r="H111"/>
-      <c r="I111"/>
-      <c r="J111"/>
-      <c r="K111"/>
-      <c r="L111"/>
-      <c r="M111"/>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A112"/>
-      <c r="B112"/>
-      <c r="C112"/>
-      <c r="D112"/>
-      <c r="E112"/>
-      <c r="F112"/>
-      <c r="G112"/>
-      <c r="H112"/>
-      <c r="I112"/>
-      <c r="J112"/>
-      <c r="K112"/>
-      <c r="L112"/>
-      <c r="M112"/>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A113"/>
-      <c r="B113"/>
-      <c r="C113"/>
-      <c r="D113"/>
-      <c r="E113"/>
-      <c r="F113"/>
-      <c r="G113"/>
-      <c r="H113"/>
-      <c r="I113"/>
-      <c r="J113"/>
-      <c r="K113"/>
-      <c r="L113"/>
-      <c r="M113"/>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A114"/>
-      <c r="B114"/>
-      <c r="C114"/>
-      <c r="D114"/>
-      <c r="E114"/>
-      <c r="F114"/>
-      <c r="G114"/>
-      <c r="H114"/>
-      <c r="I114"/>
-      <c r="J114"/>
-      <c r="K114"/>
-      <c r="L114"/>
-      <c r="M114"/>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A115"/>
-      <c r="B115"/>
-      <c r="C115"/>
-      <c r="D115"/>
-      <c r="E115"/>
-      <c r="F115"/>
-      <c r="G115"/>
-      <c r="H115"/>
-      <c r="I115"/>
-      <c r="J115"/>
-      <c r="K115"/>
-      <c r="L115"/>
-      <c r="M115"/>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A116"/>
-      <c r="B116"/>
-      <c r="C116"/>
-      <c r="D116"/>
-      <c r="E116"/>
-      <c r="F116"/>
-      <c r="G116"/>
-      <c r="H116"/>
-      <c r="I116"/>
-      <c r="J116"/>
-      <c r="K116"/>
-      <c r="L116"/>
-      <c r="M116"/>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A117"/>
-      <c r="B117"/>
-      <c r="C117"/>
-      <c r="D117"/>
-      <c r="E117"/>
-      <c r="F117"/>
-      <c r="G117"/>
-      <c r="H117"/>
-      <c r="I117"/>
-      <c r="J117"/>
-      <c r="K117"/>
-      <c r="L117"/>
-      <c r="M117"/>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A118"/>
-      <c r="B118"/>
-      <c r="C118"/>
-      <c r="D118"/>
-      <c r="E118"/>
-      <c r="F118"/>
-      <c r="G118"/>
-      <c r="H118"/>
-      <c r="I118"/>
-      <c r="J118"/>
-      <c r="K118"/>
-      <c r="L118"/>
-      <c r="M118"/>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A119"/>
-      <c r="B119"/>
-      <c r="C119"/>
-      <c r="D119"/>
-      <c r="E119"/>
-      <c r="F119"/>
-      <c r="G119"/>
-      <c r="H119"/>
-      <c r="I119"/>
-      <c r="J119"/>
-      <c r="K119"/>
-      <c r="L119"/>
-      <c r="M119"/>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A120"/>
-      <c r="B120"/>
-      <c r="C120"/>
-      <c r="D120"/>
-      <c r="E120"/>
-      <c r="F120"/>
-      <c r="G120"/>
-      <c r="H120"/>
-      <c r="I120"/>
-      <c r="J120"/>
-      <c r="K120"/>
-      <c r="L120"/>
-      <c r="M120"/>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A121"/>
-      <c r="B121"/>
-      <c r="C121"/>
-      <c r="D121"/>
-      <c r="E121"/>
-      <c r="F121"/>
-      <c r="G121"/>
-      <c r="H121"/>
-      <c r="I121"/>
-      <c r="J121"/>
-      <c r="K121"/>
-      <c r="L121"/>
-      <c r="M121"/>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A122"/>
-      <c r="B122"/>
-      <c r="C122"/>
-      <c r="D122"/>
-      <c r="E122"/>
-      <c r="F122"/>
-      <c r="G122"/>
-      <c r="H122"/>
-      <c r="I122"/>
-      <c r="J122"/>
-      <c r="K122"/>
-      <c r="L122"/>
-      <c r="M122"/>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A123"/>
-      <c r="B123"/>
-      <c r="C123"/>
-      <c r="D123"/>
-      <c r="E123"/>
-      <c r="F123"/>
-      <c r="G123"/>
-      <c r="H123"/>
-      <c r="I123"/>
-      <c r="J123"/>
-      <c r="K123"/>
-      <c r="L123"/>
-      <c r="M123"/>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A124"/>
-      <c r="B124"/>
-      <c r="C124"/>
-      <c r="D124"/>
-      <c r="E124"/>
-      <c r="F124"/>
-      <c r="G124"/>
-      <c r="H124"/>
-      <c r="I124"/>
-      <c r="J124"/>
-      <c r="K124"/>
-      <c r="L124"/>
-      <c r="M124"/>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A125"/>
-      <c r="B125"/>
-      <c r="C125"/>
-      <c r="D125"/>
-      <c r="E125"/>
-      <c r="F125"/>
-      <c r="G125"/>
-      <c r="H125"/>
-      <c r="I125"/>
-      <c r="J125"/>
-      <c r="K125"/>
-      <c r="L125"/>
-      <c r="M125"/>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A126"/>
-      <c r="B126"/>
-      <c r="C126"/>
-      <c r="D126"/>
-      <c r="E126"/>
-      <c r="F126"/>
-      <c r="G126"/>
-      <c r="H126"/>
-      <c r="I126"/>
-      <c r="J126"/>
-      <c r="K126"/>
-      <c r="L126"/>
-      <c r="M126"/>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A127"/>
-      <c r="B127"/>
-      <c r="C127"/>
-      <c r="D127"/>
-      <c r="E127"/>
-      <c r="F127"/>
-      <c r="G127"/>
-      <c r="H127"/>
-      <c r="I127"/>
-      <c r="J127"/>
-      <c r="K127"/>
-      <c r="L127"/>
-      <c r="M127"/>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A128"/>
-      <c r="B128"/>
-      <c r="C128"/>
-      <c r="D128"/>
-      <c r="E128"/>
-      <c r="F128"/>
-      <c r="G128"/>
-      <c r="H128"/>
-      <c r="I128"/>
-      <c r="J128"/>
-      <c r="K128"/>
-      <c r="L128"/>
-      <c r="M128"/>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A129"/>
-      <c r="B129"/>
-      <c r="C129"/>
-      <c r="D129"/>
-      <c r="E129"/>
-      <c r="F129"/>
-      <c r="G129"/>
-      <c r="H129"/>
-      <c r="I129"/>
-      <c r="J129"/>
-      <c r="K129"/>
-      <c r="L129"/>
-      <c r="M129"/>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A130"/>
-      <c r="B130"/>
-      <c r="C130"/>
-      <c r="D130"/>
-      <c r="E130"/>
-      <c r="F130"/>
-      <c r="G130"/>
-      <c r="H130"/>
-      <c r="I130"/>
-      <c r="J130"/>
-      <c r="K130"/>
-      <c r="L130"/>
-      <c r="M130"/>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A131"/>
-      <c r="B131"/>
-      <c r="C131"/>
-      <c r="D131"/>
-      <c r="E131"/>
-      <c r="F131"/>
-      <c r="G131"/>
-      <c r="H131"/>
-      <c r="I131"/>
-      <c r="J131"/>
-      <c r="K131"/>
-      <c r="L131"/>
-      <c r="M131"/>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A132"/>
-      <c r="B132"/>
-      <c r="C132"/>
-      <c r="D132"/>
-      <c r="E132"/>
-      <c r="F132"/>
-      <c r="G132"/>
-      <c r="H132"/>
-      <c r="I132"/>
-      <c r="J132"/>
-      <c r="K132"/>
-      <c r="L132"/>
-      <c r="M132"/>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A133"/>
-      <c r="B133"/>
-      <c r="C133"/>
-      <c r="D133"/>
-      <c r="E133"/>
-      <c r="F133"/>
-      <c r="G133"/>
-      <c r="H133"/>
-      <c r="I133"/>
-      <c r="J133"/>
-      <c r="K133"/>
-      <c r="L133"/>
-      <c r="M133"/>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A134"/>
-      <c r="B134"/>
-      <c r="C134"/>
-      <c r="D134"/>
-      <c r="E134"/>
-      <c r="F134"/>
-      <c r="G134"/>
-      <c r="H134"/>
-      <c r="I134"/>
-      <c r="J134"/>
-      <c r="K134"/>
-      <c r="L134"/>
-      <c r="M134"/>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A135"/>
-      <c r="B135"/>
-      <c r="C135"/>
-      <c r="D135"/>
-      <c r="E135"/>
-      <c r="F135"/>
-      <c r="G135"/>
-      <c r="H135"/>
-      <c r="I135"/>
-      <c r="J135"/>
-      <c r="K135"/>
-      <c r="L135"/>
-      <c r="M135"/>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A136"/>
-      <c r="B136"/>
-      <c r="C136"/>
-      <c r="D136"/>
-      <c r="E136"/>
-      <c r="F136"/>
-      <c r="G136"/>
-      <c r="H136"/>
-      <c r="I136"/>
-      <c r="J136"/>
-      <c r="K136"/>
-      <c r="L136"/>
-      <c r="M136"/>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A137"/>
-      <c r="B137"/>
-      <c r="C137"/>
-      <c r="D137"/>
-      <c r="E137"/>
-      <c r="F137"/>
-      <c r="G137"/>
-      <c r="H137"/>
-      <c r="I137"/>
-      <c r="J137"/>
-      <c r="K137"/>
-      <c r="L137"/>
-      <c r="M137"/>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A138"/>
-      <c r="B138"/>
-      <c r="C138"/>
-      <c r="D138"/>
-      <c r="E138"/>
-      <c r="F138"/>
-      <c r="G138"/>
-      <c r="H138"/>
-      <c r="I138"/>
-      <c r="J138"/>
-      <c r="K138"/>
-      <c r="L138"/>
-      <c r="M138"/>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A139"/>
-      <c r="B139"/>
-      <c r="C139"/>
-      <c r="D139"/>
-      <c r="E139"/>
-      <c r="F139"/>
-      <c r="G139"/>
-      <c r="H139"/>
-      <c r="I139"/>
-      <c r="J139"/>
-      <c r="K139"/>
-      <c r="L139"/>
-      <c r="M139"/>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A140"/>
-      <c r="B140"/>
-      <c r="C140"/>
-      <c r="D140"/>
-      <c r="E140"/>
-      <c r="F140"/>
-      <c r="G140"/>
-      <c r="H140"/>
-      <c r="I140"/>
-      <c r="J140"/>
-      <c r="K140"/>
-      <c r="L140"/>
-      <c r="M140"/>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A141"/>
-      <c r="B141"/>
-      <c r="C141"/>
-      <c r="D141"/>
-      <c r="E141"/>
-      <c r="F141"/>
-      <c r="G141"/>
-      <c r="H141"/>
-      <c r="I141"/>
-      <c r="J141"/>
-      <c r="K141"/>
-      <c r="L141"/>
-      <c r="M141"/>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A142"/>
-      <c r="B142"/>
-      <c r="C142"/>
-      <c r="D142"/>
-      <c r="E142"/>
-      <c r="F142"/>
-      <c r="G142"/>
-      <c r="H142"/>
-      <c r="I142"/>
-      <c r="J142"/>
-      <c r="K142"/>
-      <c r="L142"/>
-      <c r="M142"/>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A143"/>
-      <c r="B143"/>
-      <c r="C143"/>
-      <c r="D143"/>
-      <c r="E143"/>
-      <c r="F143"/>
-      <c r="G143"/>
-      <c r="H143"/>
-      <c r="I143"/>
-      <c r="J143"/>
-      <c r="K143"/>
-      <c r="L143"/>
-      <c r="M143"/>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A144"/>
-      <c r="B144"/>
-      <c r="C144"/>
-      <c r="D144"/>
-      <c r="E144"/>
-      <c r="F144"/>
-      <c r="G144"/>
-      <c r="H144"/>
-      <c r="I144"/>
-      <c r="J144"/>
-      <c r="K144"/>
-      <c r="L144"/>
-      <c r="M144"/>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A145"/>
-      <c r="B145"/>
-      <c r="C145"/>
-      <c r="D145"/>
-      <c r="E145"/>
-      <c r="F145"/>
-      <c r="G145"/>
-      <c r="H145"/>
-      <c r="I145"/>
-      <c r="J145"/>
-      <c r="K145"/>
-      <c r="L145"/>
-      <c r="M145"/>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A146"/>
-      <c r="B146"/>
-      <c r="C146"/>
-      <c r="D146"/>
-      <c r="E146"/>
-      <c r="F146"/>
-      <c r="G146"/>
-      <c r="H146"/>
-      <c r="I146"/>
-      <c r="J146"/>
-      <c r="K146"/>
-      <c r="L146"/>
-      <c r="M146"/>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A147"/>
-      <c r="B147"/>
-      <c r="C147"/>
-      <c r="D147"/>
-      <c r="E147"/>
-      <c r="F147"/>
-      <c r="G147"/>
-      <c r="H147"/>
-      <c r="I147"/>
-      <c r="J147"/>
-      <c r="K147"/>
-      <c r="L147"/>
-      <c r="M147"/>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A148"/>
-      <c r="B148"/>
-      <c r="C148"/>
-      <c r="D148"/>
-      <c r="E148"/>
-      <c r="F148"/>
-      <c r="G148"/>
-      <c r="H148"/>
-      <c r="I148"/>
-      <c r="J148"/>
-      <c r="K148"/>
-      <c r="L148"/>
-      <c r="M148"/>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A149"/>
-      <c r="B149"/>
-      <c r="C149"/>
-      <c r="D149"/>
-      <c r="E149"/>
-      <c r="F149"/>
-      <c r="G149"/>
-      <c r="H149"/>
-      <c r="I149"/>
-      <c r="J149"/>
-      <c r="K149"/>
-      <c r="L149"/>
-      <c r="M149"/>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A150"/>
-      <c r="B150"/>
-      <c r="C150"/>
-      <c r="D150"/>
-      <c r="E150"/>
-      <c r="F150"/>
-      <c r="G150"/>
-      <c r="H150"/>
-      <c r="I150"/>
-      <c r="J150"/>
-      <c r="K150"/>
-      <c r="L150"/>
-      <c r="M150"/>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A151"/>
-      <c r="B151"/>
-      <c r="C151"/>
-      <c r="D151"/>
-      <c r="E151"/>
-      <c r="F151"/>
-      <c r="G151"/>
-      <c r="H151"/>
-      <c r="I151"/>
-      <c r="J151"/>
-      <c r="K151"/>
-      <c r="L151"/>
-      <c r="M151"/>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A152"/>
-      <c r="B152"/>
-      <c r="C152"/>
-      <c r="D152"/>
-      <c r="E152"/>
-      <c r="F152"/>
-      <c r="G152"/>
-      <c r="H152"/>
-      <c r="I152"/>
-      <c r="J152"/>
-      <c r="K152"/>
-      <c r="L152"/>
-      <c r="M152"/>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A153"/>
-      <c r="B153"/>
-      <c r="C153"/>
-      <c r="D153"/>
-      <c r="E153"/>
-      <c r="F153"/>
-      <c r="G153"/>
-      <c r="H153"/>
-      <c r="I153"/>
-      <c r="J153"/>
-      <c r="K153"/>
-      <c r="L153"/>
-      <c r="M153"/>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A154"/>
-      <c r="B154"/>
-      <c r="C154"/>
-      <c r="D154"/>
-      <c r="E154"/>
-      <c r="F154"/>
-      <c r="G154"/>
-      <c r="H154"/>
-      <c r="I154"/>
-      <c r="J154"/>
-      <c r="K154"/>
-      <c r="L154"/>
-      <c r="M154"/>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A155"/>
-      <c r="B155"/>
-      <c r="C155"/>
-      <c r="D155"/>
-      <c r="E155"/>
-      <c r="F155"/>
-      <c r="G155"/>
-      <c r="H155"/>
-      <c r="I155"/>
-      <c r="J155"/>
-      <c r="K155"/>
-      <c r="L155"/>
-      <c r="M155"/>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A156"/>
-      <c r="B156"/>
-      <c r="C156"/>
-      <c r="D156"/>
-      <c r="E156"/>
-      <c r="F156"/>
-      <c r="G156"/>
-      <c r="H156"/>
-      <c r="I156"/>
-      <c r="J156"/>
-      <c r="K156"/>
-      <c r="L156"/>
-      <c r="M156"/>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A157"/>
-      <c r="B157"/>
-      <c r="C157"/>
-      <c r="D157"/>
-      <c r="E157"/>
-      <c r="F157"/>
-      <c r="G157"/>
-      <c r="H157"/>
-      <c r="I157"/>
-      <c r="J157"/>
-      <c r="K157"/>
-      <c r="L157"/>
-      <c r="M157"/>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A158"/>
-      <c r="B158"/>
-      <c r="C158"/>
-      <c r="D158"/>
-      <c r="E158"/>
-      <c r="F158"/>
-      <c r="G158"/>
-      <c r="H158"/>
-      <c r="I158"/>
-      <c r="J158"/>
-      <c r="K158"/>
-      <c r="L158"/>
-      <c r="M158"/>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A159"/>
-      <c r="B159"/>
-      <c r="C159"/>
-      <c r="D159"/>
-      <c r="E159"/>
-      <c r="F159"/>
-      <c r="G159"/>
-      <c r="H159"/>
-      <c r="I159"/>
-      <c r="J159"/>
-      <c r="K159"/>
-      <c r="L159"/>
-      <c r="M159"/>
-    </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A160"/>
-      <c r="B160"/>
-      <c r="C160"/>
-      <c r="D160"/>
-      <c r="E160"/>
-      <c r="F160"/>
-      <c r="G160"/>
-      <c r="H160"/>
-      <c r="I160"/>
-      <c r="J160"/>
-      <c r="K160"/>
-      <c r="L160"/>
-      <c r="M160"/>
-    </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A161"/>
-      <c r="B161"/>
-      <c r="C161"/>
-      <c r="D161"/>
-      <c r="E161"/>
-      <c r="F161"/>
-      <c r="G161"/>
-      <c r="H161"/>
-      <c r="I161"/>
-      <c r="J161"/>
-      <c r="K161"/>
-      <c r="L161"/>
-      <c r="M161"/>
-    </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A162"/>
-      <c r="B162"/>
-      <c r="C162"/>
-      <c r="D162"/>
-      <c r="E162"/>
-      <c r="F162"/>
-      <c r="G162"/>
-      <c r="H162"/>
-      <c r="I162"/>
-      <c r="J162"/>
-      <c r="K162"/>
-      <c r="L162"/>
-      <c r="M162"/>
-    </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A163"/>
-      <c r="B163"/>
-      <c r="C163"/>
-      <c r="D163"/>
-      <c r="E163"/>
-      <c r="F163"/>
-      <c r="G163"/>
-      <c r="H163"/>
-      <c r="I163"/>
-      <c r="J163"/>
-      <c r="K163"/>
-      <c r="L163"/>
-      <c r="M163"/>
-    </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A164"/>
-      <c r="B164"/>
-      <c r="C164"/>
-      <c r="D164"/>
-      <c r="E164"/>
-      <c r="F164"/>
-      <c r="G164"/>
-      <c r="H164"/>
-      <c r="I164"/>
-      <c r="J164"/>
-      <c r="K164"/>
-      <c r="L164"/>
-      <c r="M164"/>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A165"/>
-      <c r="B165"/>
-      <c r="C165"/>
-      <c r="D165"/>
-      <c r="E165"/>
-      <c r="F165"/>
-      <c r="G165"/>
-      <c r="H165"/>
-      <c r="I165"/>
-      <c r="J165"/>
-      <c r="K165"/>
-      <c r="L165"/>
-      <c r="M165"/>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A166"/>
-      <c r="B166"/>
-      <c r="C166"/>
-      <c r="D166"/>
-      <c r="E166"/>
-      <c r="F166"/>
-      <c r="G166"/>
-      <c r="H166"/>
-      <c r="I166"/>
-      <c r="J166"/>
-      <c r="K166"/>
-      <c r="L166"/>
-      <c r="M166"/>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A167"/>
-      <c r="B167"/>
-      <c r="C167"/>
-      <c r="D167"/>
-      <c r="E167"/>
-      <c r="F167"/>
-      <c r="G167"/>
-      <c r="H167"/>
-      <c r="I167"/>
-      <c r="J167"/>
-      <c r="K167"/>
-      <c r="L167"/>
-      <c r="M167"/>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A168"/>
-      <c r="B168"/>
-      <c r="C168"/>
-      <c r="D168"/>
-      <c r="E168"/>
-      <c r="F168"/>
-      <c r="G168"/>
-      <c r="H168"/>
-      <c r="I168"/>
-      <c r="J168"/>
-      <c r="K168"/>
-      <c r="L168"/>
-      <c r="M168"/>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A169"/>
-      <c r="B169"/>
-      <c r="C169"/>
-      <c r="D169"/>
-      <c r="E169"/>
-      <c r="F169"/>
-      <c r="G169"/>
-      <c r="H169"/>
-      <c r="I169"/>
-      <c r="J169"/>
-      <c r="K169"/>
-      <c r="L169"/>
-      <c r="M169"/>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A170"/>
-      <c r="B170"/>
-      <c r="C170"/>
-      <c r="D170"/>
-      <c r="E170"/>
-      <c r="F170"/>
-      <c r="G170"/>
-      <c r="H170"/>
-      <c r="I170"/>
-      <c r="J170"/>
-      <c r="K170"/>
-      <c r="L170"/>
-      <c r="M170"/>
-    </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A171"/>
-      <c r="B171"/>
-      <c r="C171"/>
-      <c r="D171"/>
-      <c r="E171"/>
-      <c r="F171"/>
-      <c r="G171"/>
-      <c r="H171"/>
-      <c r="I171"/>
-      <c r="J171"/>
-      <c r="K171"/>
-      <c r="L171"/>
-      <c r="M171"/>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A172"/>
-      <c r="B172"/>
-      <c r="C172"/>
-      <c r="D172"/>
-      <c r="E172"/>
-      <c r="F172"/>
-      <c r="G172"/>
-      <c r="H172"/>
-      <c r="I172"/>
-      <c r="J172"/>
-      <c r="K172"/>
-      <c r="L172"/>
-      <c r="M172"/>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A173"/>
-      <c r="B173"/>
-      <c r="C173"/>
-      <c r="D173"/>
-      <c r="E173"/>
-      <c r="F173"/>
-      <c r="G173"/>
-      <c r="H173"/>
-      <c r="I173"/>
-      <c r="J173"/>
-      <c r="K173"/>
-      <c r="L173"/>
-      <c r="M173"/>
-    </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A174"/>
-      <c r="B174"/>
-      <c r="C174"/>
-      <c r="D174"/>
-      <c r="E174"/>
-      <c r="F174"/>
-      <c r="G174"/>
-      <c r="H174"/>
-      <c r="I174"/>
-      <c r="J174"/>
-      <c r="K174"/>
-      <c r="L174"/>
-      <c r="M174"/>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A175"/>
-      <c r="B175"/>
-      <c r="C175"/>
-      <c r="D175"/>
-      <c r="E175"/>
-      <c r="F175"/>
-      <c r="G175"/>
-      <c r="H175"/>
-      <c r="I175"/>
-      <c r="J175"/>
-      <c r="K175"/>
-      <c r="L175"/>
-      <c r="M175"/>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A176"/>
-      <c r="B176"/>
-      <c r="C176"/>
-      <c r="D176"/>
-      <c r="E176"/>
-      <c r="F176"/>
-      <c r="G176"/>
-      <c r="H176"/>
-      <c r="I176"/>
-      <c r="J176"/>
-      <c r="K176"/>
-      <c r="L176"/>
-      <c r="M176"/>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A177"/>
-      <c r="B177"/>
-      <c r="C177"/>
-      <c r="D177"/>
-      <c r="E177"/>
-      <c r="F177"/>
-      <c r="G177"/>
-      <c r="H177"/>
-      <c r="I177"/>
-      <c r="J177"/>
-      <c r="K177"/>
-      <c r="L177"/>
-      <c r="M177"/>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A178"/>
-      <c r="B178"/>
-      <c r="C178"/>
-      <c r="D178"/>
-      <c r="E178"/>
-      <c r="F178"/>
-      <c r="G178"/>
-      <c r="H178"/>
-      <c r="I178"/>
-      <c r="J178"/>
-      <c r="K178"/>
-      <c r="L178"/>
-      <c r="M178"/>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A179" s="2"/>
-      <c r="B179"/>
-      <c r="C179"/>
-      <c r="D179"/>
-      <c r="E179"/>
-      <c r="F179"/>
-      <c r="H179"/>
-      <c r="I179"/>
-      <c r="J179"/>
-      <c r="K179"/>
-      <c r="L179"/>
-      <c r="M179"/>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A180" s="2"/>
-      <c r="B180"/>
-      <c r="C180"/>
-      <c r="D180"/>
-      <c r="E180"/>
-      <c r="F180"/>
-      <c r="H180"/>
-      <c r="I180"/>
-      <c r="J180"/>
-      <c r="K180"/>
-      <c r="L180"/>
-      <c r="M180"/>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A181" s="2"/>
-      <c r="B181"/>
-      <c r="C181"/>
-      <c r="D181"/>
-      <c r="E181"/>
-      <c r="F181"/>
-      <c r="H181"/>
-      <c r="I181"/>
-      <c r="J181"/>
-      <c r="K181"/>
-      <c r="L181"/>
-      <c r="M181"/>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A182" s="2"/>
-      <c r="B182"/>
-      <c r="C182"/>
-      <c r="D182"/>
-      <c r="E182"/>
-      <c r="F182"/>
-      <c r="H182"/>
-      <c r="I182"/>
-      <c r="J182"/>
-      <c r="K182"/>
-      <c r="L182"/>
-      <c r="M182"/>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A183" s="2"/>
-      <c r="B183"/>
-      <c r="C183"/>
-      <c r="D183"/>
-      <c r="E183"/>
-      <c r="F183"/>
-      <c r="H183"/>
-      <c r="I183"/>
-      <c r="J183"/>
-      <c r="K183"/>
-      <c r="L183"/>
-      <c r="M183"/>
-    </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A184" s="2"/>
-      <c r="B184"/>
-      <c r="C184"/>
-      <c r="D184"/>
-      <c r="E184"/>
-      <c r="F184"/>
-      <c r="H184"/>
-      <c r="I184"/>
-      <c r="J184"/>
-      <c r="K184"/>
-      <c r="L184"/>
-      <c r="M184"/>
-    </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A185" s="2"/>
-      <c r="B185"/>
-      <c r="C185"/>
-      <c r="D185"/>
-      <c r="E185"/>
-      <c r="F185"/>
-      <c r="H185"/>
-      <c r="I185"/>
-      <c r="J185"/>
-      <c r="K185"/>
-      <c r="L185"/>
-      <c r="M185"/>
-    </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A186" s="2"/>
-      <c r="B186"/>
-      <c r="C186"/>
-      <c r="D186"/>
-      <c r="E186"/>
-      <c r="F186"/>
-      <c r="H186"/>
-      <c r="I186"/>
-      <c r="J186"/>
-      <c r="K186"/>
-      <c r="L186"/>
-      <c r="M186"/>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A187" s="2"/>
-      <c r="B187"/>
-      <c r="C187"/>
-      <c r="D187"/>
-      <c r="E187"/>
-      <c r="F187"/>
-      <c r="H187"/>
-      <c r="I187"/>
-      <c r="J187"/>
-      <c r="K187"/>
-      <c r="L187"/>
-      <c r="M187"/>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A188" s="2"/>
-      <c r="B188"/>
-      <c r="C188"/>
-      <c r="D188"/>
-      <c r="E188"/>
-      <c r="F188"/>
-      <c r="H188"/>
-      <c r="I188"/>
-      <c r="J188"/>
-      <c r="K188"/>
-      <c r="L188"/>
-      <c r="M188"/>
-    </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A189" s="2"/>
-      <c r="B189"/>
-      <c r="C189"/>
-      <c r="D189"/>
-      <c r="E189"/>
-      <c r="F189"/>
-      <c r="H189"/>
-      <c r="I189"/>
-      <c r="J189"/>
-      <c r="K189"/>
-      <c r="L189"/>
-      <c r="M189"/>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A190" s="2"/>
-      <c r="B190"/>
-      <c r="C190"/>
-      <c r="D190"/>
-      <c r="E190"/>
-      <c r="F190"/>
-      <c r="H190"/>
-      <c r="I190"/>
-      <c r="J190"/>
-      <c r="K190"/>
-      <c r="L190"/>
-      <c r="M190"/>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A191" s="2"/>
-      <c r="B191"/>
-      <c r="C191"/>
-      <c r="D191"/>
-      <c r="E191"/>
-      <c r="F191"/>
-      <c r="H191"/>
-      <c r="I191"/>
-      <c r="J191"/>
-      <c r="K191"/>
-      <c r="L191"/>
-      <c r="M191"/>
-    </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A192" s="2"/>
-      <c r="B192"/>
-      <c r="C192"/>
-      <c r="D192"/>
-      <c r="E192"/>
-      <c r="F192"/>
-      <c r="H192"/>
-      <c r="I192"/>
-      <c r="J192"/>
-      <c r="K192"/>
-      <c r="L192"/>
-      <c r="M192"/>
-    </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A193" s="2"/>
-      <c r="B193"/>
-      <c r="C193"/>
-      <c r="D193"/>
-      <c r="E193"/>
-      <c r="F193"/>
-      <c r="G193"/>
-      <c r="H193"/>
-      <c r="I193"/>
-      <c r="J193"/>
-      <c r="K193"/>
-      <c r="L193"/>
-      <c r="M193"/>
-    </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A194" s="2"/>
-      <c r="B194"/>
-      <c r="C194"/>
-      <c r="D194"/>
-      <c r="E194"/>
-      <c r="F194"/>
-      <c r="H194"/>
-      <c r="I194"/>
-      <c r="J194"/>
-      <c r="K194"/>
-      <c r="L194"/>
-      <c r="M194"/>
-    </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A195" s="2"/>
-      <c r="B195"/>
-      <c r="C195"/>
-      <c r="D195"/>
-      <c r="E195"/>
-      <c r="F195"/>
-      <c r="H195"/>
-      <c r="I195"/>
-      <c r="J195"/>
-      <c r="K195"/>
-      <c r="L195"/>
-      <c r="M195"/>
-    </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A196" s="2"/>
-      <c r="B196"/>
-      <c r="C196"/>
-      <c r="D196"/>
-      <c r="E196"/>
-      <c r="F196"/>
-      <c r="H196"/>
-      <c r="I196"/>
-      <c r="J196"/>
-      <c r="K196"/>
-      <c r="L196"/>
-      <c r="M196"/>
-    </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A197" s="2"/>
-      <c r="B197"/>
-      <c r="C197"/>
-      <c r="D197"/>
-      <c r="E197"/>
-      <c r="F197"/>
-      <c r="H197"/>
-      <c r="I197"/>
-      <c r="J197"/>
-      <c r="K197"/>
-      <c r="L197"/>
-      <c r="M197"/>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A198" s="2"/>
-      <c r="B198"/>
-      <c r="C198"/>
-      <c r="D198"/>
-      <c r="E198"/>
-      <c r="F198"/>
-      <c r="H198"/>
-      <c r="I198"/>
-      <c r="J198"/>
-      <c r="K198"/>
-      <c r="L198"/>
-      <c r="M198"/>
-    </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A199" s="2"/>
-      <c r="B199"/>
-      <c r="C199"/>
-      <c r="D199"/>
-      <c r="E199"/>
-      <c r="F199"/>
-      <c r="H199"/>
-      <c r="I199"/>
-      <c r="J199"/>
-      <c r="K199"/>
-      <c r="L199"/>
-      <c r="M199"/>
-    </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A200" s="2"/>
-      <c r="B200"/>
-      <c r="C200"/>
-      <c r="D200"/>
-      <c r="E200"/>
-      <c r="F200"/>
-      <c r="H200"/>
-      <c r="I200"/>
-      <c r="J200"/>
-      <c r="K200"/>
-      <c r="L200"/>
-      <c r="M200"/>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A201" s="2"/>
-      <c r="B201"/>
-      <c r="C201"/>
-      <c r="D201"/>
-      <c r="E201"/>
-      <c r="F201"/>
-      <c r="H201"/>
-      <c r="I201"/>
-      <c r="J201"/>
-      <c r="K201"/>
-      <c r="L201"/>
-      <c r="M201"/>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A202" s="2"/>
-      <c r="B202"/>
-      <c r="C202"/>
-      <c r="D202"/>
-      <c r="E202"/>
-      <c r="F202"/>
-      <c r="H202"/>
-      <c r="I202"/>
-      <c r="J202"/>
-      <c r="K202"/>
-      <c r="L202"/>
-      <c r="M202"/>
-    </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A203" s="2"/>
-      <c r="B203"/>
-      <c r="C203"/>
-      <c r="D203"/>
-      <c r="E203"/>
-      <c r="F203"/>
-      <c r="H203"/>
-      <c r="I203"/>
-      <c r="J203"/>
-      <c r="K203"/>
-      <c r="L203"/>
-      <c r="M203"/>
-    </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A204" s="2"/>
-      <c r="B204"/>
-      <c r="C204"/>
-      <c r="D204"/>
-      <c r="E204"/>
-      <c r="F204"/>
-      <c r="H204"/>
-      <c r="I204"/>
-      <c r="J204"/>
-      <c r="K204"/>
-      <c r="L204"/>
-      <c r="M204"/>
-    </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A205" s="2"/>
-      <c r="B205"/>
-      <c r="C205"/>
-      <c r="D205"/>
-      <c r="E205"/>
-      <c r="F205"/>
-      <c r="H205"/>
-      <c r="I205"/>
-      <c r="J205"/>
-      <c r="K205"/>
-      <c r="L205"/>
-      <c r="M205"/>
-    </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A206" s="2"/>
-      <c r="B206"/>
-      <c r="C206"/>
-      <c r="D206"/>
-      <c r="E206"/>
-      <c r="F206"/>
-      <c r="H206"/>
-      <c r="I206"/>
-      <c r="J206"/>
-      <c r="K206"/>
-      <c r="L206"/>
-      <c r="M206"/>
-    </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A207" s="2"/>
-      <c r="B207"/>
-      <c r="C207"/>
-      <c r="D207"/>
-      <c r="E207"/>
-      <c r="F207"/>
-      <c r="H207"/>
-      <c r="I207"/>
-      <c r="J207"/>
-      <c r="K207"/>
-      <c r="L207"/>
-      <c r="M207"/>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A208" s="2"/>
-      <c r="B208"/>
-      <c r="C208"/>
-      <c r="D208"/>
-      <c r="E208"/>
-      <c r="F208"/>
-      <c r="H208"/>
-      <c r="I208"/>
-      <c r="J208"/>
-      <c r="K208"/>
-      <c r="L208"/>
-      <c r="M208"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{0A576EDF-D255-4C28-A615-1A8736202A92}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="B1:M125">
-    <sortCondition ref="B1:M1"/>
+  <autoFilter ref="A1:I1" xr:uid="{0A576EDF-D255-4C28-A615-1A8736202A92}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="B1:I1">
+    <sortCondition ref="B1:I1"/>
   </sortState>
-  <conditionalFormatting sqref="A1 A10:A178">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:A208">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+  <conditionalFormatting sqref="L2">
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A9">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I8">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="5" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6415,22 +3469,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:HI33"/>
+  <dimension ref="A1:HO33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="HB2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="HH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="HD6" sqref="HD6"/>
+      <selection pane="bottomRight" activeCell="HM10" sqref="HM10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="217" width="27.42578125" customWidth="1"/>
+    <col min="2" max="223" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7082,8 +4136,26 @@
       <c r="HI1" t="s">
         <v>670</v>
       </c>
+      <c r="HJ1" s="5" t="s">
+        <v>689</v>
+      </c>
+      <c r="HK1" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="HL1" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="HM1" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="HN1" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="HO1" s="5" t="s">
+        <v>694</v>
+      </c>
     </row>
-    <row r="2" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7708,8 +4780,20 @@
       <c r="HI2" t="s">
         <v>33</v>
       </c>
+      <c r="HJ2" t="s">
+        <v>33</v>
+      </c>
+      <c r="HK2" t="s">
+        <v>33</v>
+      </c>
+      <c r="HL2" t="s">
+        <v>124</v>
+      </c>
+      <c r="HM2" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="3" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -7717,7 +4801,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -7775,8 +4859,11 @@
       <c r="HH4" t="s">
         <v>677</v>
       </c>
+      <c r="HL4" t="s">
+        <v>179</v>
+      </c>
     </row>
-    <row r="5" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -7784,7 +4871,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -7893,8 +4980,11 @@
       <c r="GO6" t="b">
         <v>1</v>
       </c>
+      <c r="HM6" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -7955,8 +5045,11 @@
       <c r="HH7">
         <v>10</v>
       </c>
+      <c r="HL7">
+        <v>144000</v>
+      </c>
     </row>
-    <row r="8" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -8176,8 +5269,11 @@
       <c r="HH8" t="s">
         <v>686</v>
       </c>
+      <c r="HJ8" t="s">
+        <v>695</v>
+      </c>
     </row>
-    <row r="9" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -8271,8 +5367,14 @@
       <c r="HB9" t="s">
         <v>673</v>
       </c>
+      <c r="HM9" t="s">
+        <v>703</v>
+      </c>
+      <c r="HN9" t="s">
+        <v>705</v>
+      </c>
     </row>
-    <row r="10" spans="1:217" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:223" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -8924,8 +6026,26 @@
       <c r="HI10" s="1" t="s">
         <v>688</v>
       </c>
+      <c r="HJ10" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="HK10" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="HL10" t="s">
+        <v>698</v>
+      </c>
+      <c r="HM10" t="s">
+        <v>700</v>
+      </c>
+      <c r="HN10" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="HO10" s="1" t="s">
+        <v>706</v>
+      </c>
     </row>
-    <row r="11" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>529</v>
       </c>
@@ -8936,8 +6056,11 @@
         <v>563</v>
       </c>
       <c r="GW11" s="4"/>
+      <c r="HL11" t="s">
+        <v>699</v>
+      </c>
     </row>
-    <row r="12" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -8981,7 +6104,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -9031,7 +6154,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="14" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -9099,7 +6222,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="15" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -9140,7 +6263,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="16" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -9166,7 +6289,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="17" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -9216,7 +6339,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="18" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -9224,7 +6347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -9375,8 +6498,14 @@
       <c r="HH19">
         <v>5</v>
       </c>
+      <c r="HJ19">
+        <v>15</v>
+      </c>
+      <c r="HM19">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="20" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -9560,8 +6689,14 @@
       <c r="HH20" t="s">
         <v>669</v>
       </c>
+      <c r="HJ20" t="s">
+        <v>689</v>
+      </c>
+      <c r="HM20" t="s">
+        <v>692</v>
+      </c>
     </row>
-    <row r="21" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -9745,8 +6880,14 @@
       <c r="HH21" t="s">
         <v>669</v>
       </c>
+      <c r="HJ21" t="s">
+        <v>689</v>
+      </c>
+      <c r="HM21" t="s">
+        <v>692</v>
+      </c>
     </row>
-    <row r="22" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -9775,7 +6916,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -9804,7 +6945,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -9949,8 +7090,11 @@
       <c r="HA24" t="s">
         <v>671</v>
       </c>
+      <c r="HO24" t="s">
+        <v>707</v>
+      </c>
     </row>
-    <row r="25" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -9973,7 +7117,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="26" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -9996,7 +7140,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="27" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -10615,8 +7759,26 @@
       <c r="HI27" t="s">
         <v>144</v>
       </c>
+      <c r="HJ27" t="s">
+        <v>147</v>
+      </c>
+      <c r="HK27" t="s">
+        <v>319</v>
+      </c>
+      <c r="HL27" t="s">
+        <v>323</v>
+      </c>
+      <c r="HM27" t="s">
+        <v>701</v>
+      </c>
+      <c r="HN27" t="s">
+        <v>323</v>
+      </c>
+      <c r="HO27" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="28" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -11073,8 +8235,26 @@
       <c r="HI28" t="s">
         <v>320</v>
       </c>
+      <c r="HJ28" t="s">
+        <v>320</v>
+      </c>
+      <c r="HK28" t="s">
+        <v>147</v>
+      </c>
+      <c r="HL28" t="s">
+        <v>144</v>
+      </c>
+      <c r="HM28" t="s">
+        <v>702</v>
+      </c>
+      <c r="HN28" t="s">
+        <v>319</v>
+      </c>
+      <c r="HO28" t="s">
+        <v>311</v>
+      </c>
     </row>
-    <row r="29" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -11321,8 +8501,23 @@
       <c r="HI29" t="s">
         <v>311</v>
       </c>
+      <c r="HJ29" t="s">
+        <v>311</v>
+      </c>
+      <c r="HK29" t="s">
+        <v>320</v>
+      </c>
+      <c r="HL29" t="s">
+        <v>320</v>
+      </c>
+      <c r="HM29" t="s">
+        <v>321</v>
+      </c>
+      <c r="HN29" t="s">
+        <v>321</v>
+      </c>
     </row>
-    <row r="30" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -11506,8 +8701,20 @@
       <c r="HC30" t="s">
         <v>311</v>
       </c>
+      <c r="HK30" t="s">
+        <v>321</v>
+      </c>
+      <c r="HL30" t="s">
+        <v>321</v>
+      </c>
+      <c r="HM30" t="s">
+        <v>311</v>
+      </c>
+      <c r="HN30" t="s">
+        <v>311</v>
+      </c>
     </row>
-    <row r="31" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -11622,8 +8829,14 @@
       <c r="DH31" t="s">
         <v>340</v>
       </c>
+      <c r="HK31" t="s">
+        <v>311</v>
+      </c>
+      <c r="HL31" t="s">
+        <v>311</v>
+      </c>
     </row>
-    <row r="32" spans="1:217" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:223" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -11644,15 +8857,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:FV1">
-    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:GZ1">
-    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:HI1">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HE20:HH20">
+  <conditionalFormatting sqref="HE20:HH20 HJ20">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="HJ21">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tested and fixed Barbarian feats and archetype Adding activity source to onceEffects to improve temporary HP Adding parent conditionGain to new conditions to pass variables to sub-conditions Made turn state saveable and loadable Ticking time and resting are now blocked if an instant condition is active. Improved handling of missing traits Fixed missing Thrown weapon damage Fixed undefined available feats list
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{893E49E7-F8E0-4C28-AB2B-6487BFB0E13F}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6749EF7B-DE0A-4CC6-A48C-89C032E3DAAE}"/>
   <bookViews>
-    <workbookView xWindow="8535" yWindow="3075" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="630" windowWidth="19710" windowHeight="15570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4954" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4969" uniqueCount="1123">
   <si>
     <t>name</t>
   </si>
@@ -3472,6 +3472,54 @@
   </si>
   <si>
     <t>When struck by an enemy, you respond in turn. Make a melee Strike against the triggering creature. This Strike doesn't count toward your multiple attack penalty, and your multiple attack penalty doesn't apply to this Strike.</t>
+  </si>
+  <si>
+    <t>While this is activated, you can enter Rage without waiting.</t>
+  </si>
+  <si>
+    <t>!Has_Feat(Creature.type, 'Contagious Rage') ? 1 : 0</t>
+  </si>
+  <si>
+    <t>Share Rage Cooldown</t>
+  </si>
+  <si>
+    <t>Your ally can grant themselves the Share Rage condition for the remainder of your Rage duration.</t>
+  </si>
+  <si>
+    <t>hideChoices</t>
+  </si>
+  <si>
+    <t>gainConditions/0/choiceLocked</t>
+  </si>
+  <si>
+    <t>gainConditions/8/choiceLocked</t>
+  </si>
+  <si>
+    <t>gainConditions/7/choiceLocked</t>
+  </si>
+  <si>
+    <t>gainConditions/6/choiceLocked</t>
+  </si>
+  <si>
+    <t>gainConditions/5/choiceLocked</t>
+  </si>
+  <si>
+    <t>gainConditions/4/choiceLocked</t>
+  </si>
+  <si>
+    <t>gainConditions/3/choiceLocked</t>
+  </si>
+  <si>
+    <t>gainConditions/2/choiceLocked</t>
+  </si>
+  <si>
+    <t>gainConditions/1/choiceLocked</t>
+  </si>
+  <si>
+    <t>Dragon's Rage Breath Cooldown</t>
+  </si>
+  <si>
+    <t>Dragon Form</t>
   </si>
 </sst>
 </file>
@@ -4343,7 +4391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -38380,7 +38428,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A333">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38388,13 +38436,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:LU84"/>
+  <dimension ref="A1:LU93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="LR50" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="LM76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:LU84"/>
+      <selection pane="bottomRight" activeCell="LN93" sqref="LN93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40569,14 +40617,14 @@
       <c r="KM3" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="KS3" s="1" t="s">
-        <v>993</v>
+      <c r="KR3" s="1" t="s">
+        <v>1107</v>
       </c>
       <c r="KU3" s="1" t="s">
         <v>998</v>
       </c>
       <c r="LB3" s="1" t="s">
-        <v>1011</v>
+        <v>1110</v>
       </c>
       <c r="LT3" s="1" t="s">
         <v>1103</v>
@@ -42514,7 +42562,7 @@
         <v>1004</v>
       </c>
       <c r="LQ6" s="2" t="s">
-        <v>1043</v>
+        <v>159</v>
       </c>
       <c r="LU6" s="2" t="s">
         <v>317</v>
@@ -43634,7 +43682,7 @@
     </row>
     <row r="14" spans="1:333" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>1059</v>
+        <v>1111</v>
       </c>
       <c r="KZ14" s="1" t="b">
         <v>1</v>
@@ -45220,6 +45268,9 @@
       <c r="KZ27" s="7" t="s">
         <v>1063</v>
       </c>
+      <c r="LB27" s="7" t="s">
+        <v>1108</v>
+      </c>
     </row>
     <row r="28" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -45228,9 +45279,6 @@
       <c r="AM28" s="4">
         <v>1</v>
       </c>
-      <c r="KS28" s="4">
-        <v>-1</v>
-      </c>
       <c r="LT28" s="4">
         <v>2</v>
       </c>
@@ -45245,626 +45293,317 @@
     </row>
     <row r="30" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="D30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="E30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="F30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="G30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="H30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="N30" s="4">
-        <v>10</v>
-      </c>
-      <c r="R30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="T30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="AA30" s="4">
-        <v>10</v>
-      </c>
-      <c r="AJ30" s="4">
-        <v>-2</v>
-      </c>
-      <c r="AN30" s="4">
-        <v>10</v>
-      </c>
-      <c r="AO30" s="4">
-        <v>10</v>
-      </c>
-      <c r="AP30" s="4">
-        <v>10</v>
-      </c>
-      <c r="AS30" s="4">
-        <v>100</v>
-      </c>
-      <c r="AT30" s="4">
-        <v>200</v>
-      </c>
-      <c r="AU30" s="4">
-        <v>500</v>
-      </c>
-      <c r="BD30" s="4">
-        <v>1000</v>
-      </c>
-      <c r="BP30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="BT30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="BW30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="DJ30" s="4">
-        <v>0</v>
-      </c>
-      <c r="DK30" s="4">
-        <v>0</v>
-      </c>
-      <c r="DL30" s="4">
-        <v>0</v>
-      </c>
-      <c r="DM30" s="4">
-        <v>0</v>
-      </c>
-      <c r="DN30" s="4">
-        <v>0</v>
-      </c>
-      <c r="DO30" s="4">
-        <v>0</v>
-      </c>
-      <c r="DP30" s="4">
-        <v>0</v>
-      </c>
-      <c r="DQ30" s="4">
-        <v>0</v>
-      </c>
-      <c r="DS30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="DU30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="ED30" s="4">
-        <v>10</v>
-      </c>
-      <c r="EM30" s="4">
-        <v>10</v>
-      </c>
-      <c r="EO30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="EU30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="EW30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FC30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FG30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FI30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FJ30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FR30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FS30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FT30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FY30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="FZ30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GA30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GB30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GC30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GD30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GE30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GF30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GG30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GP30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GX30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GY30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="GZ30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="HB30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="HQ30" s="4">
-        <v>5</v>
-      </c>
-      <c r="HR30" s="4">
-        <v>5</v>
-      </c>
-      <c r="HS30" s="4">
-        <v>5</v>
-      </c>
-      <c r="HT30" s="4">
-        <v>5</v>
-      </c>
-      <c r="HU30" s="4">
-        <v>5</v>
-      </c>
-      <c r="HW30" s="4">
-        <v>15</v>
-      </c>
-      <c r="HZ30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="IT30" s="4">
-        <v>10</v>
-      </c>
-      <c r="IV30" s="4">
-        <v>100</v>
-      </c>
-      <c r="IW30" s="4">
-        <v>0</v>
-      </c>
-      <c r="JA30" s="4">
-        <v>100</v>
-      </c>
-      <c r="JB30" s="4">
-        <v>100</v>
-      </c>
-      <c r="JO30" s="4">
-        <v>100</v>
-      </c>
-      <c r="JT30" s="4">
-        <v>0</v>
-      </c>
-      <c r="JW30" s="4">
-        <v>1</v>
-      </c>
-      <c r="JX30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="JY30" s="4">
-        <v>1</v>
-      </c>
-      <c r="JZ30" s="4">
-        <v>6000</v>
-      </c>
-      <c r="KA30" s="4">
-        <v>1</v>
-      </c>
-      <c r="KB30" s="4">
-        <v>15</v>
-      </c>
-      <c r="KD30" s="4">
-        <v>3000</v>
-      </c>
-      <c r="KE30" s="4">
-        <v>1</v>
-      </c>
-      <c r="KH30" s="4">
-        <v>15</v>
-      </c>
-      <c r="KI30" s="4">
-        <v>1008000</v>
-      </c>
-      <c r="KJ30" s="4">
-        <v>100</v>
-      </c>
-      <c r="KK30" s="4">
-        <v>10</v>
-      </c>
-      <c r="KL30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="KM30" s="4">
-        <v>100</v>
-      </c>
-      <c r="KO30" s="4">
-        <v>5</v>
-      </c>
-      <c r="KP30" s="4">
-        <v>1</v>
-      </c>
-      <c r="KT30" s="4">
-        <v>1</v>
-      </c>
-      <c r="KW30" s="4">
-        <v>6000</v>
-      </c>
-      <c r="KX30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="KY30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LD30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LH30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LL30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LN30" s="4">
-        <v>100</v>
-      </c>
-      <c r="LO30" s="4">
-        <v>40</v>
-      </c>
-      <c r="LP30" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LQ30" s="4">
+        <v>1112</v>
+      </c>
+      <c r="KZ30" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="N31" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="R31" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="T31" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA31" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ31" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM31" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN31" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AO31" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="AP31" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="AS31" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="AT31" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="AU31" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="BD31" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="BP31" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="BT31" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="BW31" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="DJ31" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="DK31" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="DL31" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="DM31" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="DN31" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="DO31" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="DP31" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="DQ31" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="DS31" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="DU31" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="ED31" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="EM31" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="EO31" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="EU31" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="EW31" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="FC31" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="FG31" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="FI31" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="FJ31" s="4" t="s">
-        <v>553</v>
-      </c>
-      <c r="FR31" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="FS31" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="FT31" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="FY31" s="4" t="s">
-        <v>594</v>
-      </c>
-      <c r="FZ31" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="GA31" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="GB31" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="GC31" s="4" t="s">
-        <v>606</v>
-      </c>
-      <c r="GD31" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="GE31" s="4" t="s">
-        <v>612</v>
-      </c>
-      <c r="GF31" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="GG31" s="4" t="s">
-        <v>618</v>
-      </c>
-      <c r="GP31" s="4" t="s">
-        <v>641</v>
-      </c>
-      <c r="GX31" s="4" t="s">
-        <v>659</v>
-      </c>
-      <c r="GY31" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="GZ31" s="4" t="s">
-        <v>663</v>
-      </c>
-      <c r="HB31" s="4" t="s">
-        <v>668</v>
-      </c>
-      <c r="HQ31" s="4" t="s">
-        <v>702</v>
-      </c>
-      <c r="HR31" s="4" t="s">
-        <v>706</v>
-      </c>
-      <c r="HS31" s="4" t="s">
-        <v>709</v>
-      </c>
-      <c r="HT31" s="4" t="s">
-        <v>712</v>
-      </c>
-      <c r="HU31" s="4" t="s">
-        <v>715</v>
-      </c>
-      <c r="HW31" s="4" t="s">
-        <v>720</v>
-      </c>
-      <c r="HZ31" s="4" t="s">
-        <v>729</v>
-      </c>
-      <c r="IT31" s="4" t="s">
-        <v>802</v>
-      </c>
-      <c r="IV31" s="4" t="s">
-        <v>809</v>
-      </c>
-      <c r="IW31" s="4" t="s">
-        <v>814</v>
-      </c>
-      <c r="JA31" s="4" t="s">
-        <v>827</v>
-      </c>
-      <c r="JB31" s="4" t="s">
-        <v>809</v>
-      </c>
-      <c r="JM31" s="4" t="s">
-        <v>867</v>
-      </c>
-      <c r="JO31" s="4" t="s">
-        <v>874</v>
-      </c>
-      <c r="JP31" s="4" t="s">
-        <v>879</v>
-      </c>
-      <c r="JT31" s="4" t="s">
-        <v>890</v>
-      </c>
-      <c r="JW31" s="4" t="s">
-        <v>898</v>
-      </c>
-      <c r="JX31" s="4" t="s">
-        <v>902</v>
-      </c>
-      <c r="JY31" s="4" t="s">
-        <v>904</v>
-      </c>
-      <c r="JZ31" s="4" t="s">
-        <v>907</v>
-      </c>
-      <c r="KA31" s="4" t="s">
-        <v>911</v>
-      </c>
-      <c r="KB31" s="4" t="s">
-        <v>914</v>
-      </c>
-      <c r="KD31" s="4" t="s">
-        <v>922</v>
-      </c>
-      <c r="KE31" s="4" t="s">
-        <v>925</v>
-      </c>
-      <c r="KH31" s="4" t="s">
-        <v>933</v>
-      </c>
-      <c r="KI31" s="4" t="s">
-        <v>937</v>
-      </c>
-      <c r="KJ31" s="4" t="s">
-        <v>941</v>
-      </c>
-      <c r="KK31" s="4" t="s">
-        <v>945</v>
-      </c>
-      <c r="KL31" s="4" t="s">
-        <v>947</v>
-      </c>
-      <c r="KM31" s="4" t="s">
-        <v>950</v>
-      </c>
-      <c r="KO31" s="4" t="s">
-        <v>986</v>
-      </c>
-      <c r="KP31" s="4" t="s">
-        <v>956</v>
-      </c>
-      <c r="KR31" s="4" t="s">
-        <v>958</v>
-      </c>
-      <c r="KS31" s="4" t="s">
-        <v>992</v>
-      </c>
-      <c r="KT31" s="4" t="s">
-        <v>994</v>
-      </c>
-      <c r="KW31" s="4" t="s">
-        <v>1001</v>
-      </c>
-      <c r="KX31" s="4" t="s">
-        <v>963</v>
-      </c>
-      <c r="KY31" s="4" t="s">
-        <v>964</v>
-      </c>
-      <c r="KZ31" s="4" t="s">
-        <v>965</v>
-      </c>
-      <c r="LD31" s="4" t="s">
-        <v>969</v>
-      </c>
-      <c r="LH31" s="4" t="s">
-        <v>1027</v>
-      </c>
-      <c r="LL31" s="4" t="s">
-        <v>977</v>
-      </c>
-      <c r="LN31" s="4" t="s">
-        <v>979</v>
-      </c>
-      <c r="LO31" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="LP31" s="4" t="s">
-        <v>980</v>
-      </c>
-      <c r="LQ31" s="4" t="s">
-        <v>981</v>
-      </c>
-      <c r="LT31" s="4" t="s">
-        <v>178</v>
+        <v>7</v>
+      </c>
+      <c r="C31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="G31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="H31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="N31" s="4">
+        <v>10</v>
+      </c>
+      <c r="R31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="T31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="AA31" s="4">
+        <v>10</v>
+      </c>
+      <c r="AJ31" s="4">
+        <v>-2</v>
+      </c>
+      <c r="AN31" s="4">
+        <v>10</v>
+      </c>
+      <c r="AO31" s="4">
+        <v>10</v>
+      </c>
+      <c r="AP31" s="4">
+        <v>10</v>
+      </c>
+      <c r="AS31" s="4">
+        <v>100</v>
+      </c>
+      <c r="AT31" s="4">
+        <v>200</v>
+      </c>
+      <c r="AU31" s="4">
+        <v>500</v>
+      </c>
+      <c r="BD31" s="4">
+        <v>1000</v>
+      </c>
+      <c r="BP31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="BT31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="BW31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="DJ31" s="4">
+        <v>0</v>
+      </c>
+      <c r="DK31" s="4">
+        <v>0</v>
+      </c>
+      <c r="DL31" s="4">
+        <v>0</v>
+      </c>
+      <c r="DM31" s="4">
+        <v>0</v>
+      </c>
+      <c r="DN31" s="4">
+        <v>0</v>
+      </c>
+      <c r="DO31" s="4">
+        <v>0</v>
+      </c>
+      <c r="DP31" s="4">
+        <v>0</v>
+      </c>
+      <c r="DQ31" s="4">
+        <v>0</v>
+      </c>
+      <c r="DS31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="DU31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="ED31" s="4">
+        <v>10</v>
+      </c>
+      <c r="EM31" s="4">
+        <v>10</v>
+      </c>
+      <c r="EO31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="EU31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="EW31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FC31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FG31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FI31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FJ31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FR31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FS31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FT31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FY31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="FZ31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GA31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GB31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GC31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GD31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GE31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GF31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GG31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GP31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GX31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GY31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="GZ31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="HB31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="HQ31" s="4">
+        <v>5</v>
+      </c>
+      <c r="HR31" s="4">
+        <v>5</v>
+      </c>
+      <c r="HS31" s="4">
+        <v>5</v>
+      </c>
+      <c r="HT31" s="4">
+        <v>5</v>
+      </c>
+      <c r="HU31" s="4">
+        <v>5</v>
+      </c>
+      <c r="HW31" s="4">
+        <v>15</v>
+      </c>
+      <c r="HZ31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="IT31" s="4">
+        <v>10</v>
+      </c>
+      <c r="IV31" s="4">
+        <v>100</v>
+      </c>
+      <c r="IW31" s="4">
+        <v>0</v>
+      </c>
+      <c r="JA31" s="4">
+        <v>100</v>
+      </c>
+      <c r="JB31" s="4">
+        <v>100</v>
+      </c>
+      <c r="JO31" s="4">
+        <v>100</v>
+      </c>
+      <c r="JT31" s="4">
+        <v>0</v>
+      </c>
+      <c r="JW31" s="4">
+        <v>1</v>
+      </c>
+      <c r="JX31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="JY31" s="4">
+        <v>1</v>
+      </c>
+      <c r="JZ31" s="4">
+        <v>6000</v>
+      </c>
+      <c r="KA31" s="4">
+        <v>1</v>
+      </c>
+      <c r="KB31" s="4">
+        <v>15</v>
+      </c>
+      <c r="KD31" s="4">
+        <v>3000</v>
+      </c>
+      <c r="KE31" s="4">
+        <v>1</v>
+      </c>
+      <c r="KH31" s="4">
+        <v>15</v>
+      </c>
+      <c r="KI31" s="4">
+        <v>1008000</v>
+      </c>
+      <c r="KJ31" s="4">
+        <v>100</v>
+      </c>
+      <c r="KK31" s="4">
+        <v>10</v>
+      </c>
+      <c r="KL31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="KM31" s="4">
+        <v>100</v>
+      </c>
+      <c r="KO31" s="4">
+        <v>5</v>
+      </c>
+      <c r="KP31" s="4">
+        <v>1</v>
+      </c>
+      <c r="KS31" s="4">
+        <v>0</v>
+      </c>
+      <c r="KT31" s="4">
+        <v>1</v>
+      </c>
+      <c r="KW31" s="4">
+        <v>6000</v>
+      </c>
+      <c r="KX31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="KY31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LD31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LH31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LL31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LN31" s="4">
+        <v>100</v>
+      </c>
+      <c r="LO31" s="4">
+        <v>40</v>
+      </c>
+      <c r="LP31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LQ31" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>55</v>
@@ -45896,8 +45635,11 @@
       <c r="AA32" s="4" t="s">
         <v>133</v>
       </c>
+      <c r="AJ32" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="AM32" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AN32" s="4" t="s">
         <v>182</v>
@@ -45917,6 +45659,9 @@
       <c r="AU32" s="4" t="s">
         <v>198</v>
       </c>
+      <c r="BD32" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="BP32" s="4" t="s">
         <v>295</v>
       </c>
@@ -45927,28 +45672,28 @@
         <v>317</v>
       </c>
       <c r="DJ32" s="4" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="DK32" s="4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="DL32" s="4" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="DM32" s="4" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="DN32" s="4" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="DO32" s="4" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="DP32" s="4" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="DQ32" s="4" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="DS32" s="4" t="s">
         <v>431</v>
@@ -45975,7 +45720,7 @@
         <v>534</v>
       </c>
       <c r="FG32" s="4" t="s">
-        <v>547</v>
+        <v>465</v>
       </c>
       <c r="FI32" s="4" t="s">
         <v>551</v>
@@ -45990,7 +45735,7 @@
         <v>577</v>
       </c>
       <c r="FT32" s="4" t="s">
-        <v>579</v>
+        <v>490</v>
       </c>
       <c r="FY32" s="4" t="s">
         <v>594</v>
@@ -46077,7 +45822,7 @@
         <v>874</v>
       </c>
       <c r="JP32" s="4" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="JT32" s="4" t="s">
         <v>890</v>
@@ -46140,7 +45885,7 @@
         <v>994</v>
       </c>
       <c r="KW32" s="4" t="s">
-        <v>962</v>
+        <v>1001</v>
       </c>
       <c r="KX32" s="4" t="s">
         <v>963</v>
@@ -46151,6 +45896,9 @@
       <c r="KZ32" s="4" t="s">
         <v>965</v>
       </c>
+      <c r="LB32" s="4" t="s">
+        <v>1109</v>
+      </c>
       <c r="LD32" s="4" t="s">
         <v>969</v>
       </c>
@@ -46164,7 +45912,7 @@
         <v>979</v>
       </c>
       <c r="LO32" s="4" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
       <c r="LP32" s="4" t="s">
         <v>980</v>
@@ -46173,219 +45921,537 @@
         <v>981</v>
       </c>
       <c r="LT32" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA33" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM33" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AN33" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AO33" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="AP33" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="AS33" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AT33" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AU33" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="BP33" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="BT33" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="BW33" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="DJ33" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="DK33" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="DL33" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="DM33" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="DN33" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="DO33" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="DP33" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="DQ33" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="DS33" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="DU33" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="ED33" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="EM33" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="EO33" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="EU33" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="EW33" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="FC33" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="FG33" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="FI33" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="FJ33" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="FR33" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="FS33" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="FT33" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="FY33" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="FZ33" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="GA33" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="GB33" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="GC33" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="GD33" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="GE33" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="GF33" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="GG33" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="GP33" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="GX33" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="GY33" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="GZ33" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="HB33" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="HQ33" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="HR33" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="HS33" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="HT33" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="HU33" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="HW33" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="HZ33" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="IT33" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="IV33" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="IW33" s="4" t="s">
+        <v>814</v>
+      </c>
+      <c r="JA33" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="JB33" s="4" t="s">
+        <v>809</v>
+      </c>
+      <c r="JM33" s="4" t="s">
+        <v>867</v>
+      </c>
+      <c r="JO33" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="JP33" s="4" t="s">
+        <v>877</v>
+      </c>
+      <c r="JT33" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="JW33" s="4" t="s">
+        <v>898</v>
+      </c>
+      <c r="JX33" s="4" t="s">
+        <v>902</v>
+      </c>
+      <c r="JY33" s="4" t="s">
+        <v>904</v>
+      </c>
+      <c r="JZ33" s="4" t="s">
+        <v>907</v>
+      </c>
+      <c r="KA33" s="4" t="s">
+        <v>911</v>
+      </c>
+      <c r="KB33" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="KD33" s="4" t="s">
+        <v>922</v>
+      </c>
+      <c r="KE33" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="KH33" s="4" t="s">
+        <v>933</v>
+      </c>
+      <c r="KI33" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="KJ33" s="4" t="s">
+        <v>941</v>
+      </c>
+      <c r="KK33" s="4" t="s">
+        <v>945</v>
+      </c>
+      <c r="KL33" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="KM33" s="4" t="s">
+        <v>950</v>
+      </c>
+      <c r="KO33" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="KP33" s="4" t="s">
+        <v>956</v>
+      </c>
+      <c r="KR33" s="4" t="s">
+        <v>958</v>
+      </c>
+      <c r="KS33" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="KT33" s="4" t="s">
+        <v>994</v>
+      </c>
+      <c r="KW33" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="KX33" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="KY33" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="KZ33" s="4" t="s">
+        <v>965</v>
+      </c>
+      <c r="LB33" s="4" t="s">
+        <v>967</v>
+      </c>
+      <c r="LD33" s="4" t="s">
+        <v>969</v>
+      </c>
+      <c r="LH33" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="LL33" s="4" t="s">
+        <v>977</v>
+      </c>
+      <c r="LN33" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="LO33" s="4" t="s">
+        <v>1101</v>
+      </c>
+      <c r="LP33" s="4" t="s">
+        <v>980</v>
+      </c>
+      <c r="LQ33" s="4" t="s">
+        <v>981</v>
+      </c>
+      <c r="LT33" s="4" t="s">
         <v>984</v>
       </c>
     </row>
-    <row r="33" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+    <row r="34" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AS33" s="7" t="s">
+      <c r="AS34" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="KZ33" s="7" t="s">
+      <c r="KZ34" s="7" t="s">
         <v>1062</v>
       </c>
     </row>
-    <row r="34" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>1060</v>
       </c>
-      <c r="KZ34" s="4" t="s">
+      <c r="KZ35" s="4" t="s">
         <v>1050</v>
       </c>
     </row>
-    <row r="35" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="36" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="KZ36" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AS35" s="4">
+      <c r="AS37" s="4">
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="38" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AS36" s="4" t="s">
+      <c r="AS38" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="JP36" s="4" t="s">
+      <c r="JP38" s="4" t="s">
         <v>881</v>
       </c>
-      <c r="KZ36" s="4" t="s">
+      <c r="KW38" s="4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="KZ38" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="37" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="39" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AS37" s="4" t="s">
+      <c r="AS39" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="JP37" s="4" t="s">
+      <c r="JP39" s="4" t="s">
         <v>877</v>
       </c>
-      <c r="KZ37" s="4" t="s">
+      <c r="KW39" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="KZ39" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="38" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="40" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="JP38" s="4">
+      <c r="JP40" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+    <row r="41" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AS39" s="7" t="s">
+      <c r="AS41" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="KZ39" s="7" t="s">
+      <c r="KZ41" s="7" t="s">
         <v>1061</v>
       </c>
     </row>
-    <row r="40" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+    <row r="42" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>1064</v>
       </c>
-      <c r="KZ40" s="4" t="s">
+      <c r="KZ42" s="4" t="s">
         <v>1051</v>
       </c>
     </row>
-    <row r="41" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+    <row r="43" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="KZ43" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AS41" s="4">
+      <c r="AS44" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="42" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="45" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AS42" s="4" t="s">
+      <c r="AS45" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="KZ42" s="4" t="s">
+      <c r="KZ45" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="43" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="46" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AS43" s="4" t="s">
+      <c r="AS46" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="KZ43" s="4" t="s">
+      <c r="KZ46" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="44" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+    <row r="47" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
         <v>1065</v>
       </c>
-      <c r="KZ44" s="7" t="s">
+      <c r="KZ47" s="7" t="s">
         <v>1095</v>
       </c>
     </row>
-    <row r="45" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+    <row r="48" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>1066</v>
       </c>
-      <c r="KZ45" s="4" t="s">
+      <c r="KZ48" s="4" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="46" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="47" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>1068</v>
-      </c>
-      <c r="KZ47" s="4" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="48" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>1069</v>
-      </c>
-      <c r="KZ48" s="4" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="49" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>1070</v>
-      </c>
-      <c r="KZ49" s="7" t="s">
-        <v>1096</v>
+    <row r="49" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="KZ49" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>1071</v>
-      </c>
-      <c r="KZ50" s="4" t="s">
-        <v>1054</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="51" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>1072</v>
+        <v>1068</v>
+      </c>
+      <c r="KZ51" s="4" t="s">
+        <v>965</v>
       </c>
     </row>
     <row r="52" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="KZ52" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="53" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>1074</v>
-      </c>
-      <c r="KZ53" s="4" t="s">
-        <v>965</v>
+    <row r="53" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>1070</v>
+      </c>
+      <c r="KZ53" s="7" t="s">
+        <v>1096</v>
       </c>
     </row>
-    <row r="54" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>1075</v>
-      </c>
-      <c r="KZ54" s="7" t="s">
-        <v>1097</v>
+    <row r="54" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="KZ54" s="4" t="s">
+        <v>1054</v>
       </c>
     </row>
     <row r="55" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>1076</v>
-      </c>
-      <c r="KZ55" s="4" t="s">
-        <v>1055</v>
+        <v>1117</v>
+      </c>
+      <c r="KZ55" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>1077</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="57" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>1078</v>
+        <v>1073</v>
       </c>
       <c r="KZ57" s="4" t="s">
         <v>965</v>
@@ -46393,7 +46459,7 @@
     </row>
     <row r="58" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>1079</v>
+        <v>1074</v>
       </c>
       <c r="KZ58" s="4" t="s">
         <v>965</v>
@@ -46401,275 +46467,350 @@
     </row>
     <row r="59" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>1080</v>
+        <v>1075</v>
       </c>
       <c r="KZ59" s="7" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="60" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>1081</v>
+        <v>1076</v>
       </c>
       <c r="KZ60" s="4" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="61" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>1082</v>
+        <v>1116</v>
+      </c>
+      <c r="KZ61" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>1083</v>
-      </c>
-      <c r="KZ62" s="4" t="s">
-        <v>965</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="63" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>1084</v>
+        <v>1078</v>
       </c>
       <c r="KZ63" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="64" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+    <row r="64" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="KZ64" s="4" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="65" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>1080</v>
+      </c>
+      <c r="KZ65" s="7" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="66" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="KZ66" s="4" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="67" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>1115</v>
+      </c>
+      <c r="KZ67" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="69" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>1083</v>
+      </c>
+      <c r="KZ69" s="4" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="70" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="KZ70" s="4" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="71" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
         <v>1085</v>
       </c>
-      <c r="KZ64" s="7" t="s">
+      <c r="KZ71" s="7" t="s">
         <v>1099</v>
       </c>
     </row>
-    <row r="65" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+    <row r="72" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>1086</v>
       </c>
-      <c r="KZ65" s="4" t="s">
+      <c r="KZ72" s="4" t="s">
         <v>1057</v>
       </c>
     </row>
-    <row r="66" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+    <row r="73" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="KZ73" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>1087</v>
       </c>
     </row>
-    <row r="67" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+    <row r="75" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>1088</v>
       </c>
-      <c r="KZ67" s="4" t="s">
+      <c r="KZ75" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="68" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+    <row r="76" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>1089</v>
       </c>
-      <c r="KZ68" s="4" t="s">
+      <c r="KZ76" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="69" spans="1:333" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+    <row r="77" spans="1:312" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
         <v>1090</v>
       </c>
-      <c r="KZ69" s="7" t="s">
+      <c r="KZ77" s="7" t="s">
         <v>1100</v>
       </c>
     </row>
-    <row r="70" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+    <row r="78" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>1091</v>
       </c>
-      <c r="KZ70" s="4" t="s">
+      <c r="KZ78" s="4" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="71" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+    <row r="79" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>1113</v>
+      </c>
+      <c r="KZ79" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:312" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>1092</v>
       </c>
     </row>
-    <row r="72" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+    <row r="81" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>1093</v>
       </c>
-      <c r="KZ72" s="4" t="s">
+      <c r="KZ81" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="73" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+    <row r="82" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>1094</v>
       </c>
-      <c r="KZ73" s="4" t="s">
+      <c r="KZ82" s="4" t="s">
         <v>965</v>
       </c>
     </row>
-    <row r="74" spans="1:333" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="83" spans="1:333" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AM74" s="5" t="s">
+      <c r="AM83" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="BN74" s="5" t="s">
+      <c r="BN83" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="DW74" s="5" t="s">
+      <c r="DW83" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="FJ74" s="5" t="s">
+      <c r="FJ83" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="KC74" s="5" t="s">
+      <c r="KC83" s="5" t="s">
         <v>921</v>
       </c>
-      <c r="LA74" s="5" t="s">
+      <c r="LA83" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="LT74" s="5" t="s">
+      <c r="LT83" s="5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="75" spans="1:333" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+    <row r="84" spans="1:333" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AM75" s="5" t="s">
+      <c r="AM84" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="BN75" s="5">
+      <c r="BN84" s="5">
         <v>1</v>
       </c>
-      <c r="DW75" s="5">
+      <c r="DW84" s="5">
         <v>1</v>
       </c>
-      <c r="FJ75" s="5">
+      <c r="FJ84" s="5">
         <v>1</v>
       </c>
-      <c r="KC75" s="5">
+      <c r="KC84" s="5">
         <v>4</v>
       </c>
-      <c r="LA75" s="5" t="s">
+      <c r="LA84" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="LT75" s="5" t="s">
+      <c r="LT84" s="5" t="s">
         <v>955</v>
       </c>
     </row>
-    <row r="76" spans="1:333" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="8" t="s">
+    <row r="85" spans="1:333" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="HZ76" s="8" t="s">
+      <c r="HZ85" s="8" t="s">
         <v>735</v>
       </c>
-      <c r="KD76" s="8" t="s">
+      <c r="KD85" s="8" t="s">
         <v>735</v>
       </c>
-      <c r="LU76" s="8" t="s">
+      <c r="LU85" s="8" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="77" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
+    <row r="86" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="HZ77" s="6">
+      <c r="HZ86" s="6">
         <v>1</v>
       </c>
-      <c r="KD77" s="6">
+      <c r="KD86" s="6">
         <v>2</v>
       </c>
-      <c r="LU77" s="6">
+      <c r="LU86" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
+    <row r="87" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="HZ78" s="6" t="s">
+      <c r="HZ87" s="6" t="s">
         <v>734</v>
       </c>
-      <c r="KD78" s="6" t="s">
+      <c r="KD87" s="6" t="s">
         <v>924</v>
       </c>
-      <c r="LU78" s="6" t="s">
+      <c r="LU87" s="6" t="s">
         <v>1046</v>
       </c>
     </row>
-    <row r="79" spans="1:333" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="8" t="s">
+    <row r="88" spans="1:333" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="HZ79" s="8" t="s">
+      <c r="HZ88" s="8" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="80" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+    <row r="89" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="HZ80" s="6">
+      <c r="HZ89" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:312" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
+    <row r="90" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="HZ81" s="6" t="s">
+      <c r="HZ90" s="6" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="82" spans="1:312" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="91" spans="1:333" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="KD82" s="1" t="s">
+      <c r="KD91" s="1" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="83" spans="1:312" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="92" spans="1:333" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="IV83" s="1">
+      <c r="IV92" s="1">
         <v>6</v>
       </c>
-      <c r="JZ83" s="1">
+      <c r="JZ92" s="1">
         <v>5</v>
       </c>
-      <c r="KZ83" s="1">
+      <c r="KZ92" s="1">
         <v>3</v>
       </c>
+      <c r="LN92" s="1">
+        <v>6</v>
+      </c>
     </row>
-    <row r="84" spans="1:312" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="93" spans="1:333" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="IV84" s="1" t="s">
+      <c r="IV93" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="JZ84" s="1" t="s">
+      <c r="JZ93" s="1" t="s">
         <v>910</v>
       </c>
-      <c r="KZ84" s="1" t="s">
+      <c r="KZ93" s="1" t="s">
         <v>1014</v>
+      </c>
+      <c r="LN93" s="1" t="s">
+        <v>1122</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A76:KN84">
-    <sortCondition ref="A76:A84"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A85:KN93">
+    <sortCondition ref="A85:A93"/>
   </sortState>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Built and tested some Druid orders, feats and spells Expanded condition choices to have feat requirements Active Spells now end when their condition ends Not-unlimited conditions are now exclusive even with different choices
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="328" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{82E42B4C-6527-4DA9-B0A6-0F5663D67C76}"/>
+  <xr:revisionPtr revIDLastSave="339" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{48F1FD75-90B0-417F-B0AD-D612A38DB7D3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4966" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4974" uniqueCount="1127">
   <si>
     <t>name</t>
   </si>
@@ -3526,6 +3526,12 @@
   </si>
   <si>
     <t>If needed, your ally can grant themselves the Guardian's Deflection condition to apply the bonus to AC.</t>
+  </si>
+  <si>
+    <t>Form Control</t>
+  </si>
+  <si>
+    <t>With additional care and effort, you can take on an alternate form for a longer period of time. If your next action is to cast wild shape, wild shape's spell level is 2 lower than normal (minimum 1st level), but you can remain transformed for up to 1 hour or the listed duration (whichever is longer). You can still Dismiss the form at any time, as permitted by the spell.</t>
   </si>
 </sst>
 </file>
@@ -38442,23 +38448,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:LS93"/>
+  <dimension ref="A1:LT93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="LQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN21" sqref="AN21"/>
+      <selection pane="bottomRight" activeCell="LT1" sqref="LT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="331" width="27.42578125" style="1" customWidth="1"/>
-    <col min="332" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="332" width="27.42578125" style="1" customWidth="1"/>
+    <col min="333" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:331" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:332" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -39452,8 +39458,11 @@
       <c r="LS1" t="s">
         <v>985</v>
       </c>
+      <c r="LT1" t="s">
+        <v>1125</v>
+      </c>
     </row>
-    <row r="2" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -40435,8 +40444,11 @@
       <c r="LS2" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="LT2" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="3" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -40627,7 +40639,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="4" spans="1:331" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -41567,8 +41579,11 @@
       <c r="LS4" s="2" t="s">
         <v>315</v>
       </c>
+      <c r="LT4" s="2" t="s">
+        <v>344</v>
+      </c>
     </row>
-    <row r="5" spans="1:331" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -42211,8 +42226,11 @@
       <c r="LS5" s="2" t="s">
         <v>152</v>
       </c>
+      <c r="LT5" s="2" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="6" spans="1:331" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -42564,8 +42582,11 @@
       <c r="LS6" s="2" t="s">
         <v>317</v>
       </c>
+      <c r="LT6" s="2" t="s">
+        <v>345</v>
+      </c>
     </row>
-    <row r="7" spans="1:331" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -42810,7 +42831,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="1:331" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -42956,7 +42977,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:331" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -42982,7 +43003,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="10" spans="1:331" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -42996,7 +43017,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="11" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -43301,7 +43322,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="12" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -43510,7 +43531,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="13" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -43683,7 +43704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1111</v>
       </c>
@@ -43691,7 +43712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -43702,7 +43723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -43710,7 +43731,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -43815,7 +43836,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="18" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -43928,7 +43949,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -43939,7 +43960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -43980,7 +44001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -44974,8 +44995,11 @@
       <c r="LS21" s="1" t="s">
         <v>1045</v>
       </c>
+      <c r="LT21" s="1" t="s">
+        <v>1126</v>
+      </c>
     </row>
-    <row r="22" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:332" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -44992,7 +45016,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="23" spans="1:331" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:332" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -45051,7 +45075,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="24" spans="1:331" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:332" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -45119,7 +45143,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="25" spans="1:331" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:332" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -45193,7 +45217,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="26" spans="1:331" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:332" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
@@ -45252,7 +45276,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="27" spans="1:331" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -45269,7 +45293,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="28" spans="1:331" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
@@ -45280,7 +45304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:331" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>1058</v>
       </c>
@@ -45288,7 +45312,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="30" spans="1:331" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>1112</v>
       </c>
@@ -45296,7 +45320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:331" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -45603,8 +45627,11 @@
       <c r="LO31" s="4">
         <v>1</v>
       </c>
+      <c r="LT31" s="4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="32" spans="1:331" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -45932,8 +45959,11 @@
       <c r="LR32" s="4" t="s">
         <v>178</v>
       </c>
+      <c r="LT32" s="4" t="s">
+        <v>1125</v>
+      </c>
     </row>
-    <row r="33" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>9</v>
       </c>
@@ -46255,8 +46285,11 @@
       <c r="LR33" s="4" t="s">
         <v>984</v>
       </c>
+      <c r="LT33" s="4" t="s">
+        <v>1125</v>
+      </c>
     </row>
-    <row r="34" spans="1:330" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
@@ -46267,7 +46300,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="35" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>1060</v>
       </c>
@@ -46275,7 +46308,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="36" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>1120</v>
       </c>
@@ -46283,7 +46316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>26</v>
       </c>
@@ -46291,7 +46324,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>27</v>
       </c>
@@ -46308,7 +46341,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="39" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>28</v>
       </c>
@@ -46325,7 +46358,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="40" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>47</v>
       </c>
@@ -46333,7 +46366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:330" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
@@ -46344,7 +46377,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="42" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>1064</v>
       </c>
@@ -46352,7 +46385,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="43" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>1119</v>
       </c>
@@ -46360,7 +46393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
@@ -46368,7 +46401,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>31</v>
       </c>
@@ -46379,7 +46412,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="46" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>32</v>
       </c>
@@ -46390,7 +46423,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="47" spans="1:330" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>1065</v>
       </c>
@@ -46398,7 +46431,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="48" spans="1:330" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>1066</v>
       </c>

</xml_diff>

<commit_message>
Implemented minimum level for spell conditions Implemented effect that disables spells or activities
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{48F1FD75-90B0-417F-B0AD-D612A38DB7D3}"/>
+  <xr:revisionPtr revIDLastSave="347" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{45CA69EC-FE95-444D-9641-18A22350E13B}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4974" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4975" uniqueCount="1129">
   <si>
     <t>name</t>
   </si>
@@ -3532,6 +3532,23 @@
   </si>
   <si>
     <t>With additional care and effort, you can take on an alternate form for a longer period of time. If your next action is to cast wild shape, wild shape's spell level is 2 lower than normal (minimum 1st level), but you can remain transformed for up to 1 hour or the listed duration (whichever is longer). You can still Dismiss the form at any time, as permitted by the spell.</t>
+  </si>
+  <si>
+    <t>The shape, damage, and damage type of your breath weapon depend on your specific dragon form (see below). A creature in the area attempts a basic save against your spell DC. This is a Reflex save unless stated otherwise in the special ability description for your specific dragon form. Once activated, your breath weapon can't be used again for 1d4 rounds. Your breath weapon has the trait corresponding to the type of damage it deals.
+On 8th spell level, you gain a +14 status bonus to the breath weapon's damage.
+&lt;strong&gt;Black&lt;/strong&gt; 60-foot line, 11d6 acid.
+&lt;strong&gt;Blue&lt;/strong&gt; 80-foot line, 6d12 electricity.
+&lt;strong&gt;Brass&lt;/strong&gt; 60-foot line, 15d4 fire.
+&lt;strong&gt;Bronze&lt;/strong&gt; 80-foot line, 6d12 electricity.
+&lt;strong&gt;Copper&lt;/strong&gt; 60-foot line, 10d6 acid.
+&lt;strong&gt;Gold&lt;/strong&gt; 30-foot cone, 6d10 fire.
+&lt;strong&gt;Green&lt;/strong&gt; 30-foot cone, 10d6 poison (Fortitude save instead of Reflex).
+&lt;strong&gt;Red&lt;/strong&gt; 30-foot cone, 10d6 fire.
+&lt;strong&gt;Silver&lt;/strong&gt; 30-foot cone, 8d8 cold.
+&lt;strong&gt;White&lt;/strong&gt; 30-foot cone, 10d6 cold.</t>
+  </si>
+  <si>
+    <t>After using the breath weapon, roll 1d4 and change the duration of the cooldown condition to the result.</t>
   </si>
 </sst>
 </file>
@@ -38451,10 +38468,10 @@
   <dimension ref="A1:LT93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="LQ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="LI2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="LT1" sqref="LT1"/>
+      <selection pane="bottomRight" activeCell="LM18" sqref="LM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40635,6 +40652,9 @@
       <c r="KZ3" s="1" t="s">
         <v>1110</v>
       </c>
+      <c r="LM3" s="1" t="s">
+        <v>1128</v>
+      </c>
       <c r="LR3" s="1" t="s">
         <v>1103</v>
       </c>
@@ -44975,7 +44995,7 @@
         <v>1036</v>
       </c>
       <c r="LM21" s="1" t="s">
-        <v>1102</v>
+        <v>1127</v>
       </c>
       <c r="LN21" s="1" t="s">
         <v>1039</v>

</xml_diff>

<commit_message>
Some more Druid feats (Excel only) Expanded hint activations to 5 from 3 Some hardcoding
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{45CA69EC-FE95-444D-9641-18A22350E13B}"/>
+  <xr:revisionPtr revIDLastSave="464" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8B8EB133-26DB-4A4B-9807-D15A77F2C4DD}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="1080" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4975" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5040" uniqueCount="1156">
   <si>
     <t>name</t>
   </si>
@@ -3549,6 +3549,92 @@
   </si>
   <si>
     <t>After using the breath weapon, roll 1d4 and change the duration of the cooldown condition to the result.</t>
+  </si>
+  <si>
+    <t>Shroud of Flame</t>
+  </si>
+  <si>
+    <t>Aura</t>
+  </si>
+  <si>
+    <t>Spine Rake</t>
+  </si>
+  <si>
+    <t>Storm Retribution</t>
+  </si>
+  <si>
+    <t>An opponent adjacent to you critically hits you with a melee weapon or melee unarmed attack.</t>
+  </si>
+  <si>
+    <t>You have at least 1 available Focus Point.</t>
+  </si>
+  <si>
+    <t>You lash out, directing a burst of storming fury toward a creature that has harmed you. You cast tempest surge on the triggering opponent and push that creature, moving it 5 feet away from you if it fails its Reflex save, or 10 feet if it critically fails. This movement is forced movement.</t>
+  </si>
+  <si>
+    <t>Tempest Surge</t>
+  </si>
+  <si>
+    <t>(Phoenix form only) You gain a 20 feet aura of fire that extends out from you. A creature that enters or ends its turn within the aura takes 2d6 fire damage (3d6 on 9th level monstrosity form). A creature can take this damage only once per turn. You can use a single action, which has the concentrate trait, to activate or deactivate this aura.</t>
+  </si>
+  <si>
+    <t>(Sea serpent form only) You extend your spines and Swim or Stride. Each creature you're adjacent to at any point during your movement takes 4d8+10 slashing damage (5d8+10 on 9th level monstrosity form) (basic Reflex against your spell DC).</t>
+  </si>
+  <si>
+    <t>Trample</t>
+  </si>
+  <si>
+    <t>(Kaiju form only) You move up to double your Speed and move through the spaces of Huge or smaller creatures, trampling each creature whose space you enter. A trampled creature takes foot damage with a basic Reflex save against your spell DC.</t>
+  </si>
+  <si>
+    <t>Healing Transformation</t>
+  </si>
+  <si>
+    <t>You can take advantage of shapechanging magic to close wounds and patch injuries. If your next action is to cast a non-cantrip polymorph spell that targets only one creature, your polymorph spell also restores 1d6 Hit Points per spell level to that creature. This is a healing effect.</t>
+  </si>
+  <si>
+    <t>Only use Form Control if your maximum spell level is at least 2 higher than the minimum spell level of your intended form. Wild shape will not have an effect otherwise.</t>
+  </si>
+  <si>
+    <t>Pesh Skin</t>
+  </si>
+  <si>
+    <t>Your plant form sprouts hundreds of spines, and your blood causes mild hallucinations in creatures exposed to it. Each time a creature touches you, hits you with an unarmed attack, or hits you with a melee weapon attack while adjacent to you, that creature takes 1d6 piercing damage. Increase the damage to 2d6 if the polymorph spell is 8th level or higher, or to 3d6 if it’s 10th level.
+When an adjacent creature damages you with piercing or slashing damage, it must succeed at a Fortitude save against your class DC or become stupefied 1 (or stupefied 2 on a critical failure) until the end of its next turn.
+These benefits last until you’re no longer polymorphed into a plant.</t>
+  </si>
+  <si>
+    <t>You are transformed into a plant by a polymorph spell.</t>
+  </si>
+  <si>
+    <t>You can change from a form that looks mostly like your old self into a tree or any other non-creature plant as a single action, which has the concentrate trait. This has the same effect as tree shape, except you can turn into any kind of non-creature plant and your AC is 30.</t>
+  </si>
+  <si>
+    <t>Tree Shape (Verdant Metamorphosis)</t>
+  </si>
+  <si>
+    <t>Verdant Metamorphosis: Tree Shape</t>
+  </si>
+  <si>
+    <t>Impaling Briars: Ensnare</t>
+  </si>
+  <si>
+    <t>Impaling Briars: Impede</t>
+  </si>
+  <si>
+    <t>Impaling Briars: Wall</t>
+  </si>
+  <si>
+    <t>Impaling Briars: Impale</t>
+  </si>
+  <si>
+    <t>The ground within the area transforms into a mass of dangerous briars that assault and impede your foes. The first time each round you Sustain the Spell, you can select one of the following effects to occur in the area.
+&lt;strong&gt;Ensnare&lt;/strong&gt; The briars clump around your foes, attempting to hold them in place. A foe within the area (or flying at most 20 feet above the area) must attempt a Reflex save. On a failure, it takes a -10-foot circumstance penalty to all Speeds for 1 round, and on a critical failure, it is immobilized for 1 round unless it Escapes.
+&lt;strong&gt;Impede&lt;/strong&gt; The briars twist and writhe, making the entire area difficult terrain.
+&lt;strong&gt;Wall&lt;/strong&gt; A wall of thorns appears in the area, lasting for 1 round. The wall is greater difficult terrain instead of difficult terrain.</t>
+  </si>
+  <si>
+    <t>Once per round, you can direct the briars to impale any target in the area (or flying up to 20 feet above the area) that you can see by using a single action, which has the concentrate and manipulate traits. Make a spell attack roll. On a success, the target takes 10d6 piercing damage and takes a -10-foot circumstance penalty to all Speeds for 1 round; on a critical success, the target is immobilized for 1 round unless it Escapes.</t>
   </si>
 </sst>
 </file>
@@ -4087,7 +4173,47 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -38457,7 +38583,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A333">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38465,23 +38591,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:LT93"/>
+  <dimension ref="A1:ME93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="LI2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="MA11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="LM18" sqref="LM18"/>
+      <selection pane="bottomRight" activeCell="MB32" sqref="MB32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="332" width="27.42578125" style="1" customWidth="1"/>
-    <col min="333" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="339" width="27.42578125" style="1" customWidth="1"/>
+    <col min="340" max="342" width="27.5703125" style="1" customWidth="1"/>
+    <col min="343" max="343" width="27.42578125" style="1" customWidth="1"/>
+    <col min="344" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:332" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:343" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -39478,8 +39606,41 @@
       <c r="LT1" t="s">
         <v>1125</v>
       </c>
+      <c r="LU1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="LV1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="LW1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="LX1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="LY1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="LZ1" t="s">
+        <v>1144</v>
+      </c>
+      <c r="MA1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="MB1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="MC1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="MD1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="ME1" t="s">
+        <v>1153</v>
+      </c>
     </row>
-    <row r="2" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -40464,8 +40625,32 @@
       <c r="LT2" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="LU2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="LV2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LW2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="LX2" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="LY2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LZ2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MA2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="ME2" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="3" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -40658,8 +40843,11 @@
       <c r="LR3" s="1" t="s">
         <v>1103</v>
       </c>
+      <c r="LT3" s="1" t="s">
+        <v>1143</v>
+      </c>
     </row>
-    <row r="4" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:343" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -41602,8 +41790,29 @@
       <c r="LT4" s="2" t="s">
         <v>344</v>
       </c>
+      <c r="LU4" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="LV4" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="LW4" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="LY4" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="LZ4" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="MA4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="ME4" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="5" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:343" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -42249,8 +42458,20 @@
       <c r="LT5" s="2" t="s">
         <v>152</v>
       </c>
+      <c r="LV5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="LY5" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="LZ5" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="ME5" s="2" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="6" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:343" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -42605,8 +42826,14 @@
       <c r="LT6" s="2" t="s">
         <v>345</v>
       </c>
+      <c r="LV6" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="LZ6" s="2" t="s">
+        <v>1026</v>
+      </c>
     </row>
-    <row r="7" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:343" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -42850,8 +43077,11 @@
       <c r="LO7" s="2" t="s">
         <v>317</v>
       </c>
+      <c r="LV7" s="2" t="s">
+        <v>189</v>
+      </c>
     </row>
-    <row r="8" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:343" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -42997,7 +43227,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:343" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -43023,7 +43253,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="10" spans="1:332" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:343" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -43037,7 +43267,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="11" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -43341,8 +43571,14 @@
       <c r="LN11" s="1" t="s">
         <v>1037</v>
       </c>
+      <c r="LU11" s="1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="LZ11" s="1" t="s">
+        <v>1146</v>
+      </c>
     </row>
-    <row r="12" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -43550,8 +43786,11 @@
       <c r="LR12" s="1" t="s">
         <v>1047</v>
       </c>
+      <c r="LU12" s="1" t="s">
+        <v>1133</v>
+      </c>
     </row>
-    <row r="13" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -43723,8 +43962,11 @@
       <c r="LO13" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="LV13" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1111</v>
       </c>
@@ -43732,7 +43974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -43743,7 +43985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -43751,7 +43993,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -43855,8 +44097,20 @@
       <c r="LS17" s="1" t="s">
         <v>799</v>
       </c>
+      <c r="MB17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="MC17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="MD17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="ME17" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="18" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -43968,8 +44222,20 @@
       <c r="LS18" s="1">
         <v>1000</v>
       </c>
+      <c r="MB18" s="1">
+        <v>10</v>
+      </c>
+      <c r="MC18" s="1">
+        <v>10</v>
+      </c>
+      <c r="MD18" s="1">
+        <v>10</v>
+      </c>
+      <c r="ME18" s="1">
+        <v>10</v>
+      </c>
     </row>
-    <row r="19" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -43980,7 +44246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -44021,7 +44287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -45018,8 +45284,41 @@
       <c r="LT21" s="1" t="s">
         <v>1126</v>
       </c>
+      <c r="LU21" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="LV21" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="LW21" s="1" t="s">
+        <v>1138</v>
+      </c>
+      <c r="LX21" s="1" t="s">
+        <v>1140</v>
+      </c>
+      <c r="LY21" s="1" t="s">
+        <v>1142</v>
+      </c>
+      <c r="LZ21" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="MA21" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="MB21" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="MC21" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="MD21" s="1" t="s">
+        <v>1154</v>
+      </c>
+      <c r="ME21" s="1" t="s">
+        <v>1155</v>
+      </c>
     </row>
-    <row r="22" spans="1:332" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:343" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -45036,7 +45335,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="23" spans="1:332" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:343" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -45095,7 +45394,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="24" spans="1:332" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:343" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -45163,7 +45462,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="25" spans="1:332" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:343" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -45237,7 +45536,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="26" spans="1:332" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:343" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
@@ -45296,7 +45595,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="27" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -45313,7 +45612,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="28" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
@@ -45324,7 +45623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>1058</v>
       </c>
@@ -45332,7 +45631,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="30" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>1112</v>
       </c>
@@ -45340,7 +45639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -45650,8 +45949,20 @@
       <c r="LT31" s="4">
         <v>5</v>
       </c>
+      <c r="LZ31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="MA31" s="4">
+        <v>48000</v>
+      </c>
+      <c r="MC31" s="4">
+        <v>10</v>
+      </c>
+      <c r="MD31" s="4">
+        <v>10</v>
+      </c>
     </row>
-    <row r="32" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -45982,8 +46293,23 @@
       <c r="LT32" s="4" t="s">
         <v>1125</v>
       </c>
+      <c r="LV32" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="LZ32" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="MA32" s="4" t="s">
+        <v>1148</v>
+      </c>
+      <c r="MC32" s="4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="MD32" s="4" t="s">
+        <v>1152</v>
+      </c>
     </row>
-    <row r="33" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>9</v>
       </c>
@@ -46308,8 +46634,23 @@
       <c r="LT33" s="4" t="s">
         <v>1125</v>
       </c>
+      <c r="LV33" s="4" t="s">
+        <v>1129</v>
+      </c>
+      <c r="LZ33" s="4" t="s">
+        <v>1144</v>
+      </c>
+      <c r="MA33" s="4" t="s">
+        <v>1149</v>
+      </c>
+      <c r="MC33" s="4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="MD33" s="4" t="s">
+        <v>1152</v>
+      </c>
     </row>
-    <row r="34" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:342" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
@@ -46320,7 +46661,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="35" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>1060</v>
       </c>
@@ -46328,7 +46669,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="36" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>1120</v>
       </c>
@@ -46336,7 +46677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>26</v>
       </c>
@@ -46344,7 +46685,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>27</v>
       </c>
@@ -46361,7 +46702,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="39" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>28</v>
       </c>
@@ -46378,7 +46719,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="40" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>47</v>
       </c>
@@ -46386,7 +46727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:342" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
@@ -46397,7 +46738,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="42" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>1064</v>
       </c>
@@ -46405,7 +46746,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="43" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>1119</v>
       </c>
@@ -46413,7 +46754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
@@ -46421,7 +46762,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>31</v>
       </c>
@@ -46432,7 +46773,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="46" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>32</v>
       </c>
@@ -46443,7 +46784,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="47" spans="1:332" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:342" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>1065</v>
       </c>
@@ -46451,7 +46792,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="48" spans="1:332" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>1066</v>
       </c>
@@ -46697,7 +47038,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="81" spans="1:331" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>1093</v>
       </c>
@@ -46705,7 +47046,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="82" spans="1:331" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:333" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>1094</v>
       </c>
@@ -46713,7 +47054,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="83" spans="1:331" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:333" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>23</v>
       </c>
@@ -46738,8 +47079,11 @@
       <c r="LR83" s="5" t="s">
         <v>181</v>
       </c>
+      <c r="LU83" s="5" t="s">
+        <v>291</v>
+      </c>
     </row>
-    <row r="84" spans="1:331" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:333" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>24</v>
       </c>
@@ -46764,8 +47108,11 @@
       <c r="LR84" s="5" t="s">
         <v>955</v>
       </c>
+      <c r="LU84" s="5">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="85" spans="1:331" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:333" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>41</v>
       </c>
@@ -46778,8 +47125,11 @@
       <c r="LS85" s="8" t="s">
         <v>735</v>
       </c>
+      <c r="LU85" s="8" t="s">
+        <v>735</v>
+      </c>
     </row>
-    <row r="86" spans="1:331" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>40</v>
       </c>
@@ -46792,8 +47142,11 @@
       <c r="LS86" s="6">
         <v>8</v>
       </c>
+      <c r="LU86" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="87" spans="1:331" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>39</v>
       </c>
@@ -46806,8 +47159,11 @@
       <c r="LS87" s="6" t="s">
         <v>1046</v>
       </c>
+      <c r="LU87" s="6" t="s">
+        <v>1136</v>
+      </c>
     </row>
-    <row r="88" spans="1:331" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:333" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>44</v>
       </c>
@@ -46815,7 +47171,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="89" spans="1:331" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>43</v>
       </c>
@@ -46823,7 +47179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:331" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:333" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>42</v>
       </c>
@@ -46831,7 +47187,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="91" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:333" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>49</v>
       </c>
@@ -46839,7 +47195,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="92" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:333" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>46</v>
       </c>
@@ -46856,7 +47212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:333" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>45</v>
       </c>
@@ -46877,8 +47233,11 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A85:KL93">
     <sortCondition ref="A85:A93"/>
   </sortState>
-  <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="A1:LW1 LY1:XFD1">
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LX1">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tested and bugfixed Druid feats Hardcoded some druid stuff Tested Druid Archetype Fixed Familiar AC Implemented locked languages and improved gaining languages from ancestry and feats Allowed hiding condition choices in spells and activities Added options for hiding higher and unavailable feats Resting now takes 8 hours and not 8 hours plus refocusing Fixed animal companions not getting their specialization damage Fixed level-dependent condition choices not showing up in the active condition Improved text positioning in the general information box Added two more hint checkboxes for particularly greedy hints Changed Forge-Day's Rest from Condition to Hint Changed athletics penalty to athletics modifier in Pest Form Clarified Familiar Focus hint
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="542" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B33F8F07-10D4-4EE8-8D9C-A5C14E909BE6}"/>
+  <xr:revisionPtr revIDLastSave="548" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{46946647-F178-4210-8344-CC854F9CEAD1}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="3465" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="1125" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2779" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5355" uniqueCount="1156">
   <si>
     <t>name</t>
   </si>
@@ -2961,17 +2961,6 @@
   </si>
   <si>
     <t>By moving your clan dagger with rapid precision, you can protect yourself more effectively. Make two clan dagger Strikes against different targets. Your multiple attack penalty applies normally to these Strikes. You then use an Interact action to gain the +1 circumstance bonus to your AC from your clan dagger's parrying trait.</t>
-  </si>
-  <si>
-    <t>Forge-Day's Rest</t>
-  </si>
-  <si>
-    <t>Your unusual rest cycle allows you to recover faster. As long as you rest for 12 hours, you gain the effects of the Fast Recovery general feat and you can go 20 hours without resting before becoming fatigued._x000D_
-_x000D_
-Your body quickly bounces back from afflictions. You regain twice as many Hit Points from resting. Each time you succeed at a Fortitude save against an ongoing disease or poison, you reduce its stage by 2, or by 1 against a virulent disease or poison. Each critical success you achieve against an ongoing disease or poison reduces its stage by 3, or by 2 against a virulent disease or poison. In addition, you reduce the severity of your drained condition by 2 when you rest for a night instead of by 1.</t>
-  </si>
-  <si>
-    <t>As long as this activity is activated, the effects apply. Activate this activity before you rest in order to gain the bonus to hit points recovered. Tick 4 hours after resting to fill up the 12 hours if needed.</t>
   </si>
   <si>
     <t>Vengeful Hatred</t>
@@ -3624,6 +3613,17 @@
   </si>
   <si>
     <t>Once per round you can use a single action, which has the concentrate and manipulate traits, to call down a bolt of lightning, striking any target in range that you can see. You deal 10d6 electricity damage to the target; it must attempt a basic Reflex save. On a failure, it is also deafened for 1 round.</t>
+  </si>
+  <si>
+    <t>Your plant form sprouts hundreds of spines, and your blood causes mild hallucinations in creatures exposed to it. Each time a creature touches you, hits you with an unarmed attack, or hits you with a melee weapon attack while adjacent to you, that creature takes 1d6 piercing damage. Increase the damage to 2d6 if the polymorph spell is 8th level or higher, or to 3d6 if it's 10th level.
+When an adjacent creature damages you with piercing or slashing damage, it must succeed at a Fortitude save against your class DC or become stupefied 1 (or stupefied 2 on a critical failure) until the end of its next turn.
+These benefits last until you're no longer polymorphed into a plant.</t>
+  </si>
+  <si>
+    <t>Restores 1d6 Hit Points per spell level to the target creature when you cast the polymorph spell.</t>
+  </si>
+  <si>
+    <t>Restore 1d6 Hit Points per spell level to the target creature when you cast the polymorph spell.</t>
   </si>
 </sst>
 </file>
@@ -4162,37 +4162,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4565,7 +4535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CO15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -4612,7 +4582,7 @@
         <v>5</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>48</v>
@@ -4657,10 +4627,10 @@
         <v>22</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="AD1" s="4" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="AE1" s="4" t="s">
         <v>7</v>
@@ -4675,10 +4645,10 @@
         <v>29</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="AJ1" s="4" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="AK1" s="4" t="s">
         <v>26</v>
@@ -4696,10 +4666,10 @@
         <v>33</v>
       </c>
       <c r="AP1" s="4" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="AQ1" s="4" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="AR1" s="4" t="s">
         <v>30</v>
@@ -4711,112 +4681,112 @@
         <v>32</v>
       </c>
       <c r="AU1" s="7" t="s">
+        <v>1055</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="AW1" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AX1" s="4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="AY1" s="4" t="s">
         <v>1058</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>1059</v>
       </c>
-      <c r="AW1" s="4" t="s">
-        <v>1110</v>
-      </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BA1" s="7" t="s">
         <v>1060</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>1061</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="BD1" s="4" t="s">
         <v>1062</v>
       </c>
-      <c r="BA1" s="7" t="s">
+      <c r="BE1" s="4" t="s">
         <v>1063</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>1064</v>
       </c>
-      <c r="BC1" s="4" t="s">
-        <v>1109</v>
-      </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BG1" s="7" t="s">
         <v>1065</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>1066</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
         <v>1067</v>
       </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BK1" s="4" t="s">
         <v>1068</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>1069</v>
       </c>
-      <c r="BI1" s="4" t="s">
-        <v>1108</v>
-      </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BM1" s="7" t="s">
         <v>1070</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>1071</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="BP1" s="4" t="s">
         <v>1072</v>
       </c>
-      <c r="BM1" s="7" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>1073</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>1074</v>
       </c>
-      <c r="BO1" s="4" t="s">
-        <v>1107</v>
-      </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BS1" s="7" t="s">
         <v>1075</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>1076</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="BV1" s="4" t="s">
         <v>1077</v>
       </c>
-      <c r="BS1" s="7" t="s">
+      <c r="BW1" s="4" t="s">
         <v>1078</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>1079</v>
       </c>
-      <c r="BU1" s="4" t="s">
-        <v>1106</v>
-      </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BY1" s="7" t="s">
         <v>1080</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>1081</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="CB1" s="4" t="s">
         <v>1082</v>
       </c>
-      <c r="BY1" s="7" t="s">
+      <c r="CC1" s="4" t="s">
         <v>1083</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>1084</v>
-      </c>
-      <c r="CA1" s="4" t="s">
-        <v>1105</v>
-      </c>
-      <c r="CB1" s="4" t="s">
-        <v>1085</v>
-      </c>
-      <c r="CC1" s="4" t="s">
-        <v>1086</v>
-      </c>
-      <c r="CD1" s="4" t="s">
-        <v>1087</v>
       </c>
       <c r="CE1" s="5" t="s">
         <v>23</v>
@@ -4854,7 +4824,7 @@
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>51</v>
@@ -4884,7 +4854,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="3"/>
@@ -4899,10 +4869,10 @@
         <v>5</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="AG2" s="4" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="AH2" s="7"/>
       <c r="AI2" s="4"/>
@@ -4967,7 +4937,7 @@
     </row>
     <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>71</v>
@@ -4983,10 +4953,10 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="1" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -4997,7 +4967,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="3"/>
@@ -5073,7 +5043,7 @@
         <v>0</v>
       </c>
       <c r="CI3" s="6" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="CJ3" s="8"/>
       <c r="CK3" s="6"/>
@@ -5084,14 +5054,14 @@
     </row>
     <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>151</v>
@@ -5118,7 +5088,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="3"/>
@@ -5131,10 +5101,10 @@
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="AH4" s="7"/>
       <c r="AI4" s="4"/>
@@ -5199,7 +5169,7 @@
     </row>
     <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>76</v>
@@ -5225,7 +5195,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="3"/>
@@ -5302,7 +5272,7 @@
     </row>
     <row r="6" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>207</v>
@@ -5326,7 +5296,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="3"/>
@@ -5403,7 +5373,7 @@
     </row>
     <row r="7" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>51</v>
@@ -5431,7 +5401,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="3"/>
@@ -5508,7 +5478,7 @@
     </row>
     <row r="8" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>51</v>
@@ -5521,14 +5491,14 @@
         <v>342</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -5540,7 +5510,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="V8" s="1"/>
       <c r="W8" s="3"/>
@@ -5555,10 +5525,10 @@
         <v>-1</v>
       </c>
       <c r="AF8" s="4" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="AG8" s="4" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="AH8" s="7"/>
       <c r="AI8" s="4"/>
@@ -5623,7 +5593,7 @@
     </row>
     <row r="9" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>51</v>
@@ -5649,7 +5619,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="V9" s="1"/>
       <c r="W9" s="3"/>
@@ -5664,10 +5634,10 @@
         <v>48000</v>
       </c>
       <c r="AF9" s="4" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="AG9" s="4" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="AH9" s="7"/>
       <c r="AI9" s="4"/>
@@ -5732,7 +5702,7 @@
     </row>
     <row r="10" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>51</v>
@@ -5764,7 +5734,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="V10" s="1"/>
       <c r="W10" s="3"/>
@@ -5841,7 +5811,7 @@
     </row>
     <row r="11" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>51</v>
@@ -5877,7 +5847,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="3"/>
@@ -5892,10 +5862,10 @@
         <v>1</v>
       </c>
       <c r="AF11" s="4" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="AG11" s="4" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="AH11" s="7"/>
       <c r="AI11" s="4"/>
@@ -5960,13 +5930,13 @@
     </row>
     <row r="12" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>149</v>
@@ -5990,7 +5960,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="V12" s="1"/>
       <c r="W12" s="3"/>
@@ -6067,7 +6037,7 @@
     </row>
     <row r="13" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>76</v>
@@ -6099,7 +6069,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="3"/>
@@ -6114,10 +6084,10 @@
         <v>100</v>
       </c>
       <c r="AF13" s="4" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="AG13" s="4" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="AH13" s="7"/>
       <c r="AI13" s="4"/>
@@ -6181,12 +6151,12 @@
         <v>10</v>
       </c>
       <c r="CO13" s="1" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="14" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>71</v>
@@ -6218,7 +6188,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="V14" s="1"/>
       <c r="W14" s="3"/>
@@ -6233,10 +6203,10 @@
         <v>144000</v>
       </c>
       <c r="AF14" s="4" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="AG14" s="4" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="AH14" s="7"/>
       <c r="AI14" s="4"/>
@@ -6301,7 +6271,7 @@
     </row>
     <row r="15" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>51</v>
@@ -6333,7 +6303,7 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="V15" s="1"/>
       <c r="W15" s="3"/>
@@ -6424,23 +6394,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:MG93"/>
+  <dimension ref="A1:MF93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="MD65" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="LT2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:MG93"/>
+      <selection pane="bottomRight" activeCell="LX3" sqref="LX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="345" width="27.42578125" style="1" customWidth="1"/>
-    <col min="346" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="344" width="27.42578125" style="1" customWidth="1"/>
+    <col min="345" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:345" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:344" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7333,151 +7303,148 @@
         <v>948</v>
       </c>
       <c r="KL1" t="s">
+        <v>981</v>
+      </c>
+      <c r="KM1" t="s">
         <v>951</v>
       </c>
-      <c r="KM1" t="s">
-        <v>984</v>
-      </c>
       <c r="KN1" t="s">
+        <v>952</v>
+      </c>
+      <c r="KO1" t="s">
+        <v>953</v>
+      </c>
+      <c r="KP1" t="s">
         <v>954</v>
       </c>
-      <c r="KO1" t="s">
+      <c r="KQ1" t="s">
+        <v>987</v>
+      </c>
+      <c r="KR1" t="s">
         <v>955</v>
       </c>
-      <c r="KP1" t="s">
+      <c r="KS1" t="s">
         <v>956</v>
       </c>
-      <c r="KQ1" t="s">
+      <c r="KT1" t="s">
         <v>957</v>
       </c>
-      <c r="KR1" t="s">
-        <v>990</v>
-      </c>
-      <c r="KS1" t="s">
+      <c r="KU1" t="s">
         <v>958</v>
       </c>
-      <c r="KT1" t="s">
+      <c r="KV1" t="s">
         <v>959</v>
       </c>
-      <c r="KU1" t="s">
+      <c r="KW1" t="s">
         <v>960</v>
       </c>
-      <c r="KV1" t="s">
+      <c r="KX1" t="s">
         <v>961</v>
       </c>
-      <c r="KW1" t="s">
+      <c r="KY1" t="s">
         <v>962</v>
       </c>
-      <c r="KX1" t="s">
+      <c r="KZ1" t="s">
         <v>963</v>
       </c>
-      <c r="KY1" t="s">
+      <c r="LA1" t="s">
         <v>964</v>
       </c>
-      <c r="KZ1" t="s">
+      <c r="LB1" t="s">
         <v>965</v>
       </c>
-      <c r="LA1" t="s">
+      <c r="LC1" t="s">
         <v>966</v>
       </c>
-      <c r="LB1" t="s">
+      <c r="LD1" t="s">
         <v>967</v>
       </c>
-      <c r="LC1" t="s">
+      <c r="LE1" t="s">
         <v>968</v>
       </c>
-      <c r="LD1" t="s">
+      <c r="LF1" t="s">
         <v>969</v>
       </c>
-      <c r="LE1" t="s">
+      <c r="LG1" t="s">
         <v>970</v>
       </c>
-      <c r="LF1" t="s">
+      <c r="LH1" t="s">
         <v>971</v>
       </c>
-      <c r="LG1" t="s">
+      <c r="LI1" t="s">
         <v>972</v>
       </c>
-      <c r="LH1" t="s">
+      <c r="LJ1" t="s">
         <v>973</v>
       </c>
-      <c r="LI1" t="s">
+      <c r="LK1" t="s">
         <v>974</v>
       </c>
-      <c r="LJ1" t="s">
+      <c r="LL1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="LM1" t="s">
         <v>975</v>
       </c>
-      <c r="LK1" t="s">
+      <c r="LN1" t="s">
         <v>976</v>
       </c>
-      <c r="LL1" t="s">
+      <c r="LO1" t="s">
         <v>977</v>
       </c>
-      <c r="LM1" t="s">
-        <v>1094</v>
-      </c>
-      <c r="LN1" t="s">
+      <c r="LP1" t="s">
         <v>978</v>
       </c>
-      <c r="LO1" t="s">
+      <c r="LQ1" t="s">
         <v>979</v>
       </c>
-      <c r="LP1" t="s">
+      <c r="LR1" t="s">
         <v>980</v>
       </c>
-      <c r="LQ1" t="s">
-        <v>981</v>
-      </c>
-      <c r="LR1" t="s">
-        <v>982</v>
-      </c>
       <c r="LS1" t="s">
-        <v>983</v>
+        <v>1114</v>
       </c>
       <c r="LT1" t="s">
-        <v>1117</v>
+        <v>1121</v>
       </c>
       <c r="LU1" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="LV1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="LW1" t="s">
-        <v>1123</v>
+        <v>1128</v>
       </c>
       <c r="LX1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="LY1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="LZ1" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="MA1" t="s">
+        <v>1138</v>
+      </c>
+      <c r="MB1" t="s">
         <v>1140</v>
       </c>
-      <c r="MB1" t="s">
+      <c r="MC1" t="s">
         <v>1141</v>
       </c>
-      <c r="MC1" t="s">
+      <c r="MD1" t="s">
         <v>1143</v>
       </c>
-      <c r="MD1" t="s">
-        <v>1144</v>
-      </c>
       <c r="ME1" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="MF1" t="s">
-        <v>1145</v>
-      </c>
-      <c r="MG1" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
     </row>
-    <row r="2" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8360,20 +8327,23 @@
       <c r="KI2" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="KK2" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="KL2" s="1" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="KM2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="KN2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="KO2" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="KP2" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="KQ2" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="KR2" s="1" t="s">
         <v>71</v>
@@ -8382,127 +8352,124 @@
         <v>71</v>
       </c>
       <c r="KT2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="KU2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="KV2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="KW2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="KX2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="KY2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="KZ2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LA2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LB2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="LC2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LD2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LE2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LF2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LG2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LH2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LI2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LJ2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="KU2" s="1" t="s">
+      <c r="LK2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LL2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="KV2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="KW2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="KX2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="KY2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="KZ2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LA2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LB2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LC2" s="1" t="s">
+      <c r="LM2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="LN2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="LO2" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="LD2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LE2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LF2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LG2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LH2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LI2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LJ2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LK2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="LL2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LM2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="LN2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="LO2" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="LP2" s="1" t="s">
         <v>76</v>
       </c>
       <c r="LQ2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="LR2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LS2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LT2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="LU2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LV2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="LR2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="LS2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LT2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LU2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="LV2" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="LW2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="LX2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LY2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="LZ2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MA2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MB2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MC2" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="LX2" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="LY2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="LZ2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="MA2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="MB2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="MC2" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="MD2" s="1" t="s">
         <v>76</v>
       </c>
       <c r="ME2" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="MF2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="MG2" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -8618,7 +8585,7 @@
         <v>480</v>
       </c>
       <c r="EN3" s="1" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="FK3" s="1" t="s">
         <v>562</v>
@@ -8677,29 +8644,29 @@
       <c r="KJ3" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="KK3" s="1" t="s">
-        <v>950</v>
-      </c>
-      <c r="KP3" s="1" t="s">
+      <c r="KO3" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="KR3" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="KY3" s="1" t="s">
         <v>1099</v>
       </c>
-      <c r="KS3" s="1" t="s">
-        <v>994</v>
-      </c>
-      <c r="KZ3" s="1" t="s">
-        <v>1102</v>
-      </c>
-      <c r="LM3" s="1" t="s">
-        <v>1120</v>
-      </c>
-      <c r="LR3" s="1" t="s">
-        <v>1095</v>
-      </c>
-      <c r="MD3" s="1" t="s">
-        <v>1152</v>
+      <c r="LL3" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="LQ3" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="LX3" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="MC3" s="1" t="s">
+        <v>1149</v>
       </c>
     </row>
-    <row r="4" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -9535,13 +9502,13 @@
         <v>941</v>
       </c>
       <c r="KJ4" s="2" t="s">
-        <v>195</v>
+        <v>941</v>
       </c>
       <c r="KK4" s="2" t="s">
         <v>941</v>
       </c>
       <c r="KL4" s="2" t="s">
-        <v>941</v>
+        <v>313</v>
       </c>
       <c r="KM4" s="2" t="s">
         <v>313</v>
@@ -9556,19 +9523,19 @@
         <v>313</v>
       </c>
       <c r="KQ4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="KR4" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="KR4" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="KS4" s="2" t="s">
         <v>313</v>
       </c>
       <c r="KT4" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="KU4" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="KU4" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="KV4" s="2" t="s">
         <v>313</v>
@@ -9580,10 +9547,10 @@
         <v>313</v>
       </c>
       <c r="KY4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="KZ4" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="KZ4" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="LA4" s="2" t="s">
         <v>313</v>
@@ -9595,10 +9562,10 @@
         <v>313</v>
       </c>
       <c r="LD4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="LE4" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="LE4" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="LF4" s="2" t="s">
         <v>313</v>
@@ -9607,10 +9574,10 @@
         <v>313</v>
       </c>
       <c r="LH4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="LI4" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="LI4" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="LJ4" s="2" t="s">
         <v>313</v>
@@ -9619,10 +9586,10 @@
         <v>313</v>
       </c>
       <c r="LL4" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="LM4" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="LM4" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="LN4" s="2" t="s">
         <v>313</v>
@@ -9631,31 +9598,31 @@
         <v>313</v>
       </c>
       <c r="LP4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="LR4" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="LQ4" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="LS4" s="2" t="s">
-        <v>313</v>
+        <v>342</v>
       </c>
       <c r="LT4" s="2" t="s">
         <v>342</v>
       </c>
       <c r="LU4" s="2" t="s">
+        <v>1119</v>
+      </c>
+      <c r="LV4" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="LX4" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="LV4" s="2" t="s">
-        <v>1122</v>
-      </c>
-      <c r="LW4" s="2" t="s">
-        <v>625</v>
-      </c>
       <c r="LY4" s="2" t="s">
-        <v>342</v>
+        <v>195</v>
       </c>
       <c r="LZ4" s="2" t="s">
-        <v>195</v>
+        <v>149</v>
       </c>
       <c r="MA4" s="2" t="s">
         <v>149</v>
@@ -9670,16 +9637,13 @@
         <v>149</v>
       </c>
       <c r="ME4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="MF4" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="MF4" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="MG4" s="2" t="s">
-        <v>149</v>
-      </c>
     </row>
-    <row r="5" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -10229,113 +10193,113 @@
       <c r="KH5" s="2" t="s">
         <v>941</v>
       </c>
-      <c r="KJ5" s="2" t="s">
-        <v>941</v>
+      <c r="KL5" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="KM5" s="2" t="s">
-        <v>149</v>
+        <v>315</v>
       </c>
       <c r="KN5" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="KO5" s="2" t="s">
+      <c r="KP5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="KQ5" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="KS5" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="KQ5" s="2" t="s">
+      <c r="KT5" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="KU5" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="KV5" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="KW5" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="KR5" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="KT5" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="KU5" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="KV5" s="2" t="s">
-        <v>1000</v>
-      </c>
-      <c r="KW5" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="KX5" s="2" t="s">
         <v>149</v>
       </c>
       <c r="KY5" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="KZ5" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="LA5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="KZ5" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="LA5" s="2" t="s">
+      <c r="LB5" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="LB5" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="LC5" s="2" t="s">
         <v>315</v>
       </c>
       <c r="LD5" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="LE5" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="LF5" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="LE5" s="2" t="s">
+      <c r="LG5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="LH5" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="LF5" s="2" t="s">
-        <v>1000</v>
-      </c>
-      <c r="LG5" s="2" t="s">
+      <c r="LI5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="LJ5" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="LH5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="LI5" s="2" t="s">
+      <c r="LK5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="LL5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="LM5" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="LN5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="LO5" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="LP5" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="LJ5" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="LK5" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="LL5" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="LM5" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="LN5" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="LO5" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="LP5" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="LQ5" s="2" t="s">
-        <v>313</v>
+      <c r="LR5" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="LS5" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="LT5" s="2" t="s">
+      <c r="LU5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="LX5" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="LY5" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="MA5" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="LV5" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="LY5" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="LZ5" s="2" t="s">
+      <c r="MB5" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="MB5" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="MC5" s="2" t="s">
         <v>342</v>
@@ -10347,13 +10311,10 @@
         <v>342</v>
       </c>
       <c r="MF5" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="MG5" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -10651,74 +10612,74 @@
       <c r="JU6" s="2" t="s">
         <v>850</v>
       </c>
-      <c r="KM6" s="2" t="s">
+      <c r="KL6" s="2" t="s">
         <v>315</v>
       </c>
+      <c r="KP6" s="2" t="s">
+        <v>315</v>
+      </c>
       <c r="KQ6" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="KT6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="KU6" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="KV6" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="KW6" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="KX6" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="KR6" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="KU6" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="KV6" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="KW6" s="2" t="s">
-        <v>1000</v>
-      </c>
-      <c r="KX6" s="2" t="s">
-        <v>1000</v>
       </c>
       <c r="KY6" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="KZ6" s="2" t="s">
+      <c r="LA6" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="LB6" s="2" t="s">
+      <c r="LD6" s="2" t="s">
         <v>315</v>
       </c>
       <c r="LE6" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="LG6" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="LH6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="LI6" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="LK6" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="LN6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="LR6" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="LF6" s="2" t="s">
-        <v>1021</v>
-      </c>
-      <c r="LH6" s="2" t="s">
-        <v>1000</v>
-      </c>
-      <c r="LI6" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="LJ6" s="2" t="s">
-        <v>1028</v>
-      </c>
-      <c r="LL6" s="2" t="s">
-        <v>1000</v>
-      </c>
-      <c r="LO6" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="LS6" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="LT6" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="LV6" s="2" t="s">
+      <c r="LU6" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="LZ6" s="2" t="s">
-        <v>1021</v>
-      </c>
-      <c r="MC6" s="2" t="s">
+      <c r="LY6" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="MB6" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -10926,50 +10887,50 @@
       <c r="JD7" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="KR7" s="2" t="s">
+      <c r="KQ7" s="2" t="s">
         <v>166</v>
       </c>
+      <c r="KT7" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="KU7" s="2" t="s">
-        <v>151</v>
+        <v>187</v>
       </c>
       <c r="KV7" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="KW7" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="KY7" s="2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="LE7" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="KW7" s="2" t="s">
-        <v>1011</v>
-      </c>
-      <c r="KX7" s="2" t="s">
+      <c r="LG7" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="LH7" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="LI7" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="LK7" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="KZ7" s="2" t="s">
-        <v>1012</v>
-      </c>
-      <c r="LF7" s="2" t="s">
+      <c r="LN7" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="LU7" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="LH7" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="LI7" s="2" t="s">
-        <v>1000</v>
-      </c>
-      <c r="LJ7" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="LL7" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="LO7" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="LV7" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="MC7" s="2" t="s">
+      <c r="MB7" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="8" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -11090,32 +11051,32 @@
       <c r="HW8" s="2" t="s">
         <v>328</v>
       </c>
+      <c r="KT8" s="2" t="s">
+        <v>997</v>
+      </c>
       <c r="KU8" s="2" t="s">
-        <v>1000</v>
+        <v>315</v>
       </c>
       <c r="KV8" s="2" t="s">
         <v>315</v>
       </c>
       <c r="KW8" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="LE8" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="KX8" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="LF8" s="2" t="s">
+      <c r="LG8" s="2" t="s">
         <v>315</v>
       </c>
       <c r="LH8" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="LI8" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="LL8" s="2" t="s">
+      <c r="LK8" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -11125,37 +11086,37 @@
       <c r="CC9" s="2" t="s">
         <v>344</v>
       </c>
+      <c r="KT9" s="2" t="s">
+        <v>315</v>
+      </c>
       <c r="KU9" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="KW9" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="KV9" s="2" t="s">
-        <v>1010</v>
-      </c>
-      <c r="KX9" s="2" t="s">
+      <c r="LE9" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="LK9" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="LF9" s="2" t="s">
-        <v>1010</v>
-      </c>
-      <c r="LL9" s="2" t="s">
-        <v>315</v>
-      </c>
     </row>
-    <row r="10" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="CC10" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="KX10" s="2" t="s">
-        <v>1010</v>
-      </c>
-      <c r="LL10" s="2" t="s">
-        <v>1010</v>
+      <c r="KW10" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="LK10" s="2" t="s">
+        <v>1007</v>
       </c>
     </row>
-    <row r="11" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -11432,41 +11393,41 @@
       <c r="KG11" s="1" t="s">
         <v>937</v>
       </c>
+      <c r="KT11" s="1" t="s">
+        <v>995</v>
+      </c>
       <c r="KU11" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="KV11" s="1" t="s">
-        <v>1001</v>
+      <c r="KY11" s="1" t="s">
+        <v>995</v>
       </c>
       <c r="KZ11" s="1" t="s">
-        <v>998</v>
-      </c>
-      <c r="LA11" s="1" t="s">
-        <v>1013</v>
-      </c>
-      <c r="LD11" s="1" t="s">
-        <v>1017</v>
+        <v>1010</v>
+      </c>
+      <c r="LC11" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="LF11" s="1" t="s">
+        <v>1020</v>
       </c>
       <c r="LG11" s="1" t="s">
-        <v>1023</v>
-      </c>
-      <c r="LH11" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="LK11" s="1" t="s">
-        <v>1097</v>
-      </c>
-      <c r="LN11" s="1" t="s">
-        <v>1032</v>
-      </c>
-      <c r="LU11" s="1" t="s">
-        <v>1126</v>
-      </c>
-      <c r="LZ11" s="1" t="s">
-        <v>1137</v>
+        <v>1021</v>
+      </c>
+      <c r="LJ11" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="LM11" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="LT11" s="1" t="s">
+        <v>1123</v>
+      </c>
+      <c r="LY11" s="1" t="s">
+        <v>1134</v>
       </c>
     </row>
-    <row r="12" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -11656,29 +11617,29 @@
       <c r="KH12" s="1" t="s">
         <v>942</v>
       </c>
-      <c r="KO12" s="1" t="s">
-        <v>986</v>
-      </c>
-      <c r="KR12" s="1" t="s">
-        <v>991</v>
-      </c>
-      <c r="KT12" s="1" t="s">
-        <v>995</v>
-      </c>
-      <c r="LK12" s="1" t="s">
-        <v>1030</v>
-      </c>
-      <c r="LO12" s="1" t="s">
-        <v>1035</v>
-      </c>
-      <c r="LR12" s="1" t="s">
-        <v>1041</v>
-      </c>
-      <c r="LU12" s="1" t="s">
-        <v>1125</v>
+      <c r="KN12" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="KQ12" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="KS12" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="LJ12" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="LN12" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="LQ12" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="LT12" s="1" t="s">
+        <v>1122</v>
       </c>
     </row>
-    <row r="13" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -11829,40 +11790,37 @@
       <c r="KC13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="KJ13" s="1" t="b">
+      <c r="KM13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="KN13" s="1" t="b">
+      <c r="KO13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="KP13" s="1" t="b">
+      <c r="KQ13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="KR13" s="1" t="b">
+      <c r="KW13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="KX13" s="1" t="b">
+      <c r="LK13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="LL13" s="1" t="b">
+      <c r="LN13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="LO13" s="1" t="b">
+      <c r="LU13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="LV13" s="1" t="b">
+    </row>
+    <row r="14" spans="1:344" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="KW14" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:345" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>1103</v>
-      </c>
-      <c r="KX14" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -11873,7 +11831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -11881,7 +11839,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -11978,30 +11936,30 @@
       <c r="KH17" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="KX17"/>
-      <c r="LQ17" s="1" t="s">
+      <c r="KW17"/>
+      <c r="LP17" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="LS17" s="1" t="s">
+      <c r="LR17" s="1" t="s">
         <v>797</v>
       </c>
+      <c r="MA17" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="MB17" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="MD17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="ME17" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="MF17" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="MC17" s="1" t="s">
-        <v>824</v>
-      </c>
-      <c r="ME17" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="MF17" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="MG17" s="1" t="s">
-        <v>125</v>
-      </c>
     </row>
-    <row r="18" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -12107,29 +12065,29 @@
       <c r="KH18" s="1">
         <v>144000</v>
       </c>
-      <c r="LQ18" s="1">
+      <c r="LP18" s="1">
         <v>1000</v>
       </c>
-      <c r="LS18" s="1">
+      <c r="LR18" s="1">
         <v>1000</v>
       </c>
+      <c r="MA18" s="1">
+        <v>10</v>
+      </c>
       <c r="MB18" s="1">
+        <v>100</v>
+      </c>
+      <c r="MD18" s="1">
+        <v>144000</v>
+      </c>
+      <c r="ME18" s="1">
+        <v>6000</v>
+      </c>
+      <c r="MF18" s="1">
         <v>10</v>
       </c>
-      <c r="MC18" s="1">
-        <v>100</v>
-      </c>
-      <c r="ME18" s="1">
-        <v>144000</v>
-      </c>
-      <c r="MF18" s="1">
-        <v>6000</v>
-      </c>
-      <c r="MG18" s="1">
-        <v>10</v>
-      </c>
     </row>
-    <row r="19" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -12140,7 +12098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -12168,20 +12126,20 @@
       <c r="KC20" s="1">
         <v>1</v>
       </c>
-      <c r="KN20" s="1">
+      <c r="KM20" s="1">
         <v>1</v>
       </c>
-      <c r="KR20" s="1">
+      <c r="KQ20" s="1">
         <v>1</v>
       </c>
-      <c r="LL20" s="1">
+      <c r="LK20" s="1">
         <v>100</v>
       </c>
-      <c r="LO20" s="1">
+      <c r="LN20" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -13074,151 +13032,148 @@
         <v>949</v>
       </c>
       <c r="KL21" s="1" t="s">
-        <v>952</v>
+        <v>984</v>
       </c>
       <c r="KM21" s="1" t="s">
-        <v>987</v>
+        <v>982</v>
       </c>
       <c r="KN21" s="1" t="s">
         <v>985</v>
       </c>
       <c r="KO21" s="1" t="s">
-        <v>988</v>
+        <v>996</v>
       </c>
       <c r="KP21" s="1" t="s">
-        <v>999</v>
+        <v>986</v>
       </c>
       <c r="KQ21" s="1" t="s">
         <v>989</v>
       </c>
       <c r="KR21" s="1" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="KS21" s="1" t="s">
         <v>993</v>
       </c>
       <c r="KT21" s="1" t="s">
-        <v>996</v>
+        <v>1030</v>
       </c>
       <c r="KU21" s="1" t="s">
-        <v>1033</v>
+        <v>999</v>
       </c>
       <c r="KV21" s="1" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="KW21" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="KX21" s="1" t="s">
-        <v>1008</v>
+        <v>1001</v>
       </c>
       <c r="KY21" s="1" t="s">
         <v>1004</v>
       </c>
       <c r="KZ21" s="1" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="LA21" s="1" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="LB21" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="LC21" s="1" t="s">
         <v>1015</v>
       </c>
-      <c r="LC21" s="1" t="s">
+      <c r="LD21" s="1" t="s">
         <v>1016</v>
       </c>
-      <c r="LD21" s="1" t="s">
-        <v>1018</v>
-      </c>
       <c r="LE21" s="1" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="LF21" s="1" t="s">
-        <v>1020</v>
+        <v>1023</v>
       </c>
       <c r="LG21" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="LH21" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="LI21" s="1" t="s">
         <v>1026</v>
       </c>
-      <c r="LH21" s="1" t="s">
-        <v>1025</v>
-      </c>
-      <c r="LI21" s="1" t="s">
-        <v>1027</v>
-      </c>
       <c r="LJ21" s="1" t="s">
-        <v>1029</v>
+        <v>1095</v>
       </c>
       <c r="LK21" s="1" t="s">
-        <v>1098</v>
+        <v>1028</v>
       </c>
       <c r="LL21" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="LM21" s="1" t="s">
         <v>1031</v>
       </c>
-      <c r="LM21" s="1" t="s">
-        <v>1119</v>
-      </c>
       <c r="LN21" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="LO21" s="1" t="s">
         <v>1034</v>
       </c>
-      <c r="LO21" s="1" t="s">
+      <c r="LP21" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="LQ21" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="LR21" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="LP21" s="1" t="s">
-        <v>1037</v>
-      </c>
-      <c r="LQ21" s="1" t="s">
-        <v>1038</v>
-      </c>
-      <c r="LR21" s="1" t="s">
-        <v>1042</v>
-      </c>
       <c r="LS21" s="1" t="s">
-        <v>1039</v>
+        <v>1115</v>
       </c>
       <c r="LT21" s="1" t="s">
-        <v>1118</v>
+        <v>1124</v>
       </c>
       <c r="LU21" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="LV21" s="1" t="s">
         <v>1127</v>
       </c>
-      <c r="LV21" s="1" t="s">
+      <c r="LW21" s="1" t="s">
         <v>1129</v>
       </c>
-      <c r="LW21" s="1" t="s">
-        <v>1130</v>
-      </c>
       <c r="LX21" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="LY21" s="1" t="s">
-        <v>1134</v>
+        <v>1153</v>
       </c>
       <c r="LZ21" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="MA21" s="1" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="MB21" s="1" t="s">
-        <v>1142</v>
+        <v>1150</v>
       </c>
       <c r="MC21" s="1" t="s">
-        <v>1153</v>
+        <v>1144</v>
       </c>
       <c r="MD21" s="1" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="ME21" s="1" t="s">
         <v>1148</v>
       </c>
       <c r="MF21" s="1" t="s">
-        <v>1151</v>
-      </c>
-      <c r="MG21" s="1" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
     </row>
-    <row r="22" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:344" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -13235,7 +13190,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="23" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -13294,7 +13249,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="24" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -13362,7 +13317,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="25" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -13436,7 +13391,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="26" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
@@ -13495,7 +13450,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="27" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:344" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -13505,41 +13460,41 @@
       <c r="BB27" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="KX27" s="7" t="s">
-        <v>1056</v>
-      </c>
-      <c r="KZ27" s="7" t="s">
-        <v>1100</v>
+      <c r="KW27" s="7" t="s">
+        <v>1053</v>
+      </c>
+      <c r="KY27" s="7" t="s">
+        <v>1097</v>
       </c>
     </row>
-    <row r="28" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
       <c r="AM28" s="4">
         <v>1</v>
       </c>
-      <c r="LR28" s="4">
+      <c r="LQ28" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>1052</v>
-      </c>
-      <c r="KX29" s="4" t="s">
-        <v>1043</v>
+        <v>1049</v>
+      </c>
+      <c r="KW29" s="4" t="s">
+        <v>1040</v>
       </c>
     </row>
-    <row r="30" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>1104</v>
-      </c>
-      <c r="KX30" s="4" t="b">
+        <v>1101</v>
+      </c>
+      <c r="KW30" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -13799,73 +13754,70 @@
         <v>10</v>
       </c>
       <c r="KJ31" s="4">
+        <v>100</v>
+      </c>
+      <c r="KL31" s="4">
+        <v>5</v>
+      </c>
+      <c r="KM31" s="4">
+        <v>1</v>
+      </c>
+      <c r="KP31" s="4">
+        <v>0</v>
+      </c>
+      <c r="KQ31" s="4">
+        <v>1</v>
+      </c>
+      <c r="KT31" s="4">
+        <v>6000</v>
+      </c>
+      <c r="KU31" s="4">
         <v>-1</v>
-      </c>
-      <c r="KK31" s="4">
-        <v>100</v>
-      </c>
-      <c r="KM31" s="4">
-        <v>5</v>
-      </c>
-      <c r="KN31" s="4">
-        <v>1</v>
-      </c>
-      <c r="KQ31" s="4">
-        <v>0</v>
-      </c>
-      <c r="KR31" s="4">
-        <v>1</v>
-      </c>
-      <c r="KU31" s="4">
-        <v>6000</v>
       </c>
       <c r="KV31" s="4">
         <v>-1</v>
       </c>
-      <c r="KW31" s="4">
+      <c r="LA31" s="4">
         <v>-1</v>
       </c>
-      <c r="LB31" s="4">
+      <c r="LE31" s="4">
         <v>-1</v>
       </c>
-      <c r="LF31" s="4">
+      <c r="LI31" s="4">
         <v>-1</v>
       </c>
-      <c r="LJ31" s="4">
+      <c r="LK31" s="4">
+        <v>100</v>
+      </c>
+      <c r="LL31" s="4">
+        <v>40</v>
+      </c>
+      <c r="LM31" s="4">
         <v>-1</v>
       </c>
-      <c r="LL31" s="4">
+      <c r="LN31" s="4">
+        <v>1</v>
+      </c>
+      <c r="LS31" s="4">
+        <v>5</v>
+      </c>
+      <c r="LY31" s="4">
+        <v>-1</v>
+      </c>
+      <c r="LZ31" s="4">
+        <v>48000</v>
+      </c>
+      <c r="MB31" s="4">
+        <v>1</v>
+      </c>
+      <c r="MD31" s="4">
         <v>100</v>
       </c>
-      <c r="LM31" s="4">
-        <v>40</v>
-      </c>
-      <c r="LN31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="LO31" s="4">
-        <v>1</v>
-      </c>
-      <c r="LT31" s="4">
-        <v>5</v>
-      </c>
-      <c r="LZ31" s="4">
-        <v>-1</v>
-      </c>
-      <c r="MA31" s="4">
-        <v>48000</v>
-      </c>
-      <c r="MC31" s="4">
-        <v>1</v>
-      </c>
       <c r="ME31" s="4">
-        <v>100</v>
-      </c>
-      <c r="MF31" s="4">
         <v>144000</v>
       </c>
     </row>
-    <row r="32" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -13912,7 +13864,7 @@
         <v>178</v>
       </c>
       <c r="AN32" s="4" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="AQ32" s="4" t="s">
         <v>196</v>
@@ -14136,86 +14088,83 @@
       <c r="KJ32" s="4" t="s">
         <v>945</v>
       </c>
-      <c r="KK32" s="4" t="s">
-        <v>948</v>
+      <c r="KL32" s="4" t="s">
+        <v>981</v>
       </c>
       <c r="KM32" s="4" t="s">
-        <v>984</v>
-      </c>
-      <c r="KN32" s="4" t="s">
+        <v>951</v>
+      </c>
+      <c r="KO32" s="4" t="s">
+        <v>953</v>
+      </c>
+      <c r="KP32" s="4" t="s">
         <v>954</v>
       </c>
-      <c r="KP32" s="4" t="s">
-        <v>956</v>
-      </c>
       <c r="KQ32" s="4" t="s">
-        <v>957</v>
-      </c>
-      <c r="KR32" s="4" t="s">
-        <v>990</v>
+        <v>987</v>
+      </c>
+      <c r="KT32" s="4" t="s">
+        <v>994</v>
       </c>
       <c r="KU32" s="4" t="s">
-        <v>997</v>
+        <v>958</v>
       </c>
       <c r="KV32" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="KW32" s="4" t="s">
-        <v>962</v>
-      </c>
-      <c r="KX32" s="4" t="s">
-        <v>963</v>
-      </c>
-      <c r="KZ32" s="4" t="s">
-        <v>1101</v>
-      </c>
-      <c r="LB32" s="4" t="s">
-        <v>967</v>
-      </c>
-      <c r="LF32" s="4" t="s">
-        <v>1022</v>
-      </c>
-      <c r="LJ32" s="4" t="s">
+        <v>960</v>
+      </c>
+      <c r="KY32" s="4" t="s">
+        <v>1098</v>
+      </c>
+      <c r="LA32" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="LE32" s="4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="LI32" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="LK32" s="4" t="s">
+        <v>974</v>
+      </c>
+      <c r="LL32" s="4" t="s">
+        <v>1093</v>
+      </c>
+      <c r="LM32" s="4" t="s">
         <v>975</v>
       </c>
-      <c r="LL32" s="4" t="s">
-        <v>977</v>
-      </c>
-      <c r="LM32" s="4" t="s">
-        <v>1096</v>
-      </c>
       <c r="LN32" s="4" t="s">
-        <v>978</v>
-      </c>
-      <c r="LO32" s="4" t="s">
-        <v>979</v>
-      </c>
-      <c r="LR32" s="4" t="s">
+        <v>976</v>
+      </c>
+      <c r="LQ32" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="LT32" s="4" t="s">
-        <v>1117</v>
-      </c>
-      <c r="LV32" s="4" t="s">
-        <v>1121</v>
+      <c r="LS32" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="LU32" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="LY32" s="4" t="s">
+        <v>1132</v>
       </c>
       <c r="LZ32" s="4" t="s">
-        <v>1135</v>
-      </c>
-      <c r="MA32" s="4" t="s">
-        <v>1139</v>
-      </c>
-      <c r="MC32" s="4" t="s">
-        <v>1143</v>
+        <v>1136</v>
+      </c>
+      <c r="MB32" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="MD32" s="4" t="s">
+        <v>1147</v>
       </c>
       <c r="ME32" s="4" t="s">
-        <v>1150</v>
-      </c>
-      <c r="MF32" s="4" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
-    <row r="33" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>9</v>
       </c>
@@ -14259,7 +14208,7 @@
         <v>175</v>
       </c>
       <c r="AN33" s="4" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="AQ33" s="4" t="s">
         <v>196</v>
@@ -14480,113 +14429,110 @@
       <c r="KJ33" s="4" t="s">
         <v>945</v>
       </c>
-      <c r="KK33" s="4" t="s">
-        <v>948</v>
+      <c r="KL33" s="4" t="s">
+        <v>981</v>
       </c>
       <c r="KM33" s="4" t="s">
-        <v>984</v>
-      </c>
-      <c r="KN33" s="4" t="s">
+        <v>951</v>
+      </c>
+      <c r="KO33" s="4" t="s">
+        <v>953</v>
+      </c>
+      <c r="KP33" s="4" t="s">
         <v>954</v>
       </c>
-      <c r="KP33" s="4" t="s">
-        <v>956</v>
-      </c>
       <c r="KQ33" s="4" t="s">
+        <v>987</v>
+      </c>
+      <c r="KT33" s="4" t="s">
         <v>957</v>
       </c>
-      <c r="KR33" s="4" t="s">
-        <v>990</v>
-      </c>
       <c r="KU33" s="4" t="s">
+        <v>958</v>
+      </c>
+      <c r="KV33" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="KW33" s="4" t="s">
         <v>960</v>
       </c>
-      <c r="KV33" s="4" t="s">
-        <v>961</v>
-      </c>
-      <c r="KW33" s="4" t="s">
+      <c r="KY33" s="4" t="s">
         <v>962</v>
       </c>
-      <c r="KX33" s="4" t="s">
-        <v>963</v>
-      </c>
-      <c r="KZ33" s="4" t="s">
-        <v>965</v>
-      </c>
-      <c r="LB33" s="4" t="s">
-        <v>967</v>
-      </c>
-      <c r="LF33" s="4" t="s">
-        <v>1022</v>
-      </c>
-      <c r="LJ33" s="4" t="s">
+      <c r="LA33" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="LE33" s="4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="LI33" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="LK33" s="4" t="s">
+        <v>974</v>
+      </c>
+      <c r="LL33" s="4" t="s">
+        <v>1091</v>
+      </c>
+      <c r="LM33" s="4" t="s">
         <v>975</v>
       </c>
-      <c r="LL33" s="4" t="s">
-        <v>977</v>
-      </c>
-      <c r="LM33" s="4" t="s">
-        <v>1094</v>
-      </c>
       <c r="LN33" s="4" t="s">
-        <v>978</v>
-      </c>
-      <c r="LO33" s="4" t="s">
+        <v>976</v>
+      </c>
+      <c r="LQ33" s="4" t="s">
         <v>979</v>
       </c>
-      <c r="LR33" s="4" t="s">
-        <v>982</v>
-      </c>
-      <c r="LT33" s="4" t="s">
-        <v>1117</v>
-      </c>
-      <c r="LV33" s="4" t="s">
-        <v>1121</v>
+      <c r="LS33" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="LU33" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="LY33" s="4" t="s">
+        <v>1132</v>
       </c>
       <c r="LZ33" s="4" t="s">
-        <v>1135</v>
-      </c>
-      <c r="MA33" s="4" t="s">
+        <v>1137</v>
+      </c>
+      <c r="MB33" s="4" t="s">
         <v>1140</v>
       </c>
-      <c r="MC33" s="4" t="s">
-        <v>1143</v>
+      <c r="MD33" s="4" t="s">
+        <v>1141</v>
       </c>
       <c r="ME33" s="4" t="s">
-        <v>1144</v>
-      </c>
-      <c r="MF33" s="4" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
-    <row r="34" spans="1:344" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
       <c r="AQ34" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="KX34" s="7" t="s">
-        <v>1055</v>
+      <c r="KW34" s="7" t="s">
+        <v>1052</v>
       </c>
     </row>
-    <row r="35" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>1053</v>
-      </c>
-      <c r="KX35" s="4" t="s">
-        <v>1044</v>
+        <v>1050</v>
+      </c>
+      <c r="KW35" s="4" t="s">
+        <v>1041</v>
       </c>
     </row>
-    <row r="36" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>1112</v>
-      </c>
-      <c r="KX36" s="4" t="b">
+        <v>1109</v>
+      </c>
+      <c r="KW36" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>26</v>
       </c>
@@ -14594,7 +14540,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>27</v>
       </c>
@@ -14604,14 +14550,14 @@
       <c r="JN38" s="4" t="s">
         <v>879</v>
       </c>
-      <c r="KU38" s="4" t="s">
-        <v>1113</v>
-      </c>
-      <c r="KX38" s="4" t="s">
-        <v>963</v>
+      <c r="KT38" s="4" t="s">
+        <v>1110</v>
+      </c>
+      <c r="KW38" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
-    <row r="39" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>28</v>
       </c>
@@ -14621,14 +14567,14 @@
       <c r="JN39" s="4" t="s">
         <v>875</v>
       </c>
-      <c r="KU39" s="4" t="s">
+      <c r="KT39" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="KW39" s="4" t="s">
         <v>960</v>
       </c>
-      <c r="KX39" s="4" t="s">
-        <v>963</v>
-      </c>
     </row>
-    <row r="40" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>47</v>
       </c>
@@ -14636,34 +14582,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:344" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
       <c r="AQ41" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="KX41" s="7" t="s">
+      <c r="KW41" s="7" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="42" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>1054</v>
       </c>
+      <c r="KW42" s="4" t="s">
+        <v>1042</v>
+      </c>
     </row>
-    <row r="42" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>1057</v>
-      </c>
-      <c r="KX42" s="4" t="s">
-        <v>1045</v>
+    <row r="43" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>1108</v>
+      </c>
+      <c r="KW43" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>1111</v>
-      </c>
-      <c r="KX43" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
@@ -14671,299 +14617,299 @@
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>31</v>
       </c>
       <c r="AQ45" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="KX45" s="4" t="s">
-        <v>963</v>
+      <c r="KW45" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
-    <row r="46" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>32</v>
       </c>
       <c r="AQ46" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="KX46" s="4" t="s">
-        <v>963</v>
+      <c r="KW46" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
-    <row r="47" spans="1:344" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
+        <v>1055</v>
+      </c>
+      <c r="KW47" s="7" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="48" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="KW48" s="4" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="49" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="KW49" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="51" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>1058</v>
       </c>
-      <c r="KX47" s="7" t="s">
+      <c r="KW51" s="4" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="52" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="KW52" s="4" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="53" spans="1:309" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>1060</v>
+      </c>
+      <c r="KW53" s="7" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="54" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>1061</v>
+      </c>
+      <c r="KW54" s="4" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="55" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>1106</v>
+      </c>
+      <c r="KW55" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="57" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>1063</v>
+      </c>
+      <c r="KW57" s="4" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="58" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="KW58" s="4" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="59" spans="1:309" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>1065</v>
+      </c>
+      <c r="KW59" s="7" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="60" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="KW60" s="4" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="61" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="KW61" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="63" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="KW63" s="4" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="64" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="KW64" s="4" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="65" spans="1:309" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>1070</v>
+      </c>
+      <c r="KW65" s="7" t="s">
         <v>1088</v>
       </c>
     </row>
-    <row r="48" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>1059</v>
-      </c>
-      <c r="KX48" s="4" t="s">
+    <row r="66" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="KW66" s="4" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="49" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>1110</v>
-      </c>
-      <c r="KX49" s="4" t="b">
+    <row r="67" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>1104</v>
+      </c>
+      <c r="KW67" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>1060</v>
+    <row r="68" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>1072</v>
       </c>
     </row>
-    <row r="51" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>1061</v>
-      </c>
-      <c r="KX51" s="4" t="s">
-        <v>963</v>
+    <row r="69" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="KW69" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
-    <row r="52" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>1062</v>
-      </c>
-      <c r="KX52" s="4" t="s">
-        <v>963</v>
+    <row r="70" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="KW70" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
-    <row r="53" spans="1:310" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>1063</v>
-      </c>
-      <c r="KX53" s="7" t="s">
+    <row r="71" spans="1:309" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>1075</v>
+      </c>
+      <c r="KW71" s="7" t="s">
         <v>1089</v>
       </c>
     </row>
-    <row r="54" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>1064</v>
-      </c>
-      <c r="KX54" s="4" t="s">
+    <row r="72" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="KW72" s="4" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="55" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>1109</v>
-      </c>
-      <c r="KX55" s="4" t="b">
+    <row r="73" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>1103</v>
+      </c>
+      <c r="KW73" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>1065</v>
+    <row r="74" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>1077</v>
       </c>
     </row>
-    <row r="57" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>1066</v>
-      </c>
-      <c r="KX57" s="4" t="s">
-        <v>963</v>
+    <row r="75" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>1078</v>
+      </c>
+      <c r="KW75" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
-    <row r="58" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>1067</v>
-      </c>
-      <c r="KX58" s="4" t="s">
-        <v>963</v>
+    <row r="76" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="KW76" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
-    <row r="59" spans="1:310" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>1068</v>
-      </c>
-      <c r="KX59" s="7" t="s">
+    <row r="77" spans="1:309" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>1080</v>
+      </c>
+      <c r="KW77" s="7" t="s">
         <v>1090</v>
       </c>
     </row>
-    <row r="60" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>1069</v>
-      </c>
-      <c r="KX60" s="4" t="s">
-        <v>1049</v>
+    <row r="78" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="KW78" s="4" t="s">
+        <v>1043</v>
       </c>
     </row>
-    <row r="61" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>1108</v>
-      </c>
-      <c r="KX61" s="4" t="b">
+    <row r="79" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>1102</v>
+      </c>
+      <c r="KW79" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>1070</v>
+    <row r="80" spans="1:309" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>1082</v>
       </c>
     </row>
-    <row r="63" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>1071</v>
-      </c>
-      <c r="KX63" s="4" t="s">
-        <v>963</v>
+    <row r="81" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>1083</v>
+      </c>
+      <c r="KW81" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
-    <row r="64" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>1072</v>
-      </c>
-      <c r="KX64" s="4" t="s">
-        <v>963</v>
+    <row r="82" spans="1:342" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>1084</v>
+      </c>
+      <c r="KW82" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
-    <row r="65" spans="1:310" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
-        <v>1073</v>
-      </c>
-      <c r="KX65" s="7" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="66" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>1074</v>
-      </c>
-      <c r="KX66" s="4" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="67" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>1107</v>
-      </c>
-      <c r="KX67" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="69" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>1076</v>
-      </c>
-      <c r="KX69" s="4" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="70" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>1077</v>
-      </c>
-      <c r="KX70" s="4" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="71" spans="1:310" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>1078</v>
-      </c>
-      <c r="KX71" s="7" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="72" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>1079</v>
-      </c>
-      <c r="KX72" s="4" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="73" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
-        <v>1106</v>
-      </c>
-      <c r="KX73" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="75" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>1081</v>
-      </c>
-      <c r="KX75" s="4" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="76" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>1082</v>
-      </c>
-      <c r="KX76" s="4" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="77" spans="1:310" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>1083</v>
-      </c>
-      <c r="KX77" s="7" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="78" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>1084</v>
-      </c>
-      <c r="KX78" s="4" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="79" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>1105</v>
-      </c>
-      <c r="KX79" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:310" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="81" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>1086</v>
-      </c>
-      <c r="KX81" s="4" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="82" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>1087</v>
-      </c>
-      <c r="KX82" s="4" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="83" spans="1:343" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:342" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>23</v>
       </c>
@@ -14982,22 +14928,22 @@
       <c r="KA83" s="5" t="s">
         <v>919</v>
       </c>
-      <c r="KY83" s="5" t="s">
-        <v>1005</v>
-      </c>
-      <c r="LR83" s="5" t="s">
+      <c r="KX83" s="5" t="s">
+        <v>1002</v>
+      </c>
+      <c r="LQ83" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="LU83" s="5" t="s">
+      <c r="LT83" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="84" spans="1:343" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:342" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>24</v>
       </c>
       <c r="AM84" s="5" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="BL84" s="5">
         <v>1</v>
@@ -15011,17 +14957,17 @@
       <c r="KA84" s="5">
         <v>4</v>
       </c>
-      <c r="KY84" s="5" t="s">
-        <v>1006</v>
-      </c>
-      <c r="LR84" s="5" t="s">
-        <v>953</v>
-      </c>
-      <c r="LU84" s="5">
+      <c r="KX84" s="5" t="s">
+        <v>1003</v>
+      </c>
+      <c r="LQ84" s="5" t="s">
+        <v>950</v>
+      </c>
+      <c r="LT84" s="5">
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="1:343" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:342" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>41</v>
       </c>
@@ -15031,14 +14977,14 @@
       <c r="KB85" s="8" t="s">
         <v>733</v>
       </c>
-      <c r="LS85" s="8" t="s">
+      <c r="LR85" s="8" t="s">
         <v>733</v>
       </c>
-      <c r="LU85" s="8" t="s">
+      <c r="LT85" s="8" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="86" spans="1:343" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:342" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>40</v>
       </c>
@@ -15048,14 +14994,14 @@
       <c r="KB86" s="6">
         <v>2</v>
       </c>
-      <c r="LS86" s="6">
+      <c r="LR86" s="6">
         <v>8</v>
       </c>
-      <c r="LU86" s="6">
+      <c r="LT86" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:343" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:342" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>39</v>
       </c>
@@ -15065,14 +15011,14 @@
       <c r="KB87" s="6" t="s">
         <v>922</v>
       </c>
-      <c r="LS87" s="6" t="s">
-        <v>1040</v>
-      </c>
-      <c r="LU87" s="6" t="s">
-        <v>1128</v>
+      <c r="LR87" s="6" t="s">
+        <v>1037</v>
+      </c>
+      <c r="LT87" s="6" t="s">
+        <v>1125</v>
       </c>
     </row>
-    <row r="88" spans="1:343" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:342" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
         <v>44</v>
       </c>
@@ -15080,7 +15026,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="89" spans="1:343" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:342" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>43</v>
       </c>
@@ -15088,7 +15034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:343" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:342" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>42</v>
       </c>
@@ -15096,7 +15042,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="91" spans="1:343" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:342" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>49</v>
       </c>
@@ -15104,7 +15050,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="92" spans="1:343" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:342" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>46</v>
       </c>
@@ -15114,17 +15060,17 @@
       <c r="JX92" s="1">
         <v>5</v>
       </c>
-      <c r="KX92" s="1">
+      <c r="KW92" s="1">
         <v>3</v>
       </c>
-      <c r="LL92" s="1">
+      <c r="LK92" s="1">
         <v>6</v>
       </c>
-      <c r="ME92" s="1">
+      <c r="MD92" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:343" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:342" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>45</v>
       </c>
@@ -15134,27 +15080,27 @@
       <c r="JX93" s="1" t="s">
         <v>908</v>
       </c>
-      <c r="KX93" s="1" t="s">
-        <v>1009</v>
-      </c>
-      <c r="LL93" s="1" t="s">
-        <v>1114</v>
-      </c>
-      <c r="ME93" s="1" t="s">
-        <v>1149</v>
+      <c r="KW93" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="LK93" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="MD93" s="1" t="s">
+        <v>1146</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A85:KL93">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A85:KK93">
     <sortCondition ref="A85:A93"/>
   </sortState>
-  <conditionalFormatting sqref="A1:LW1 LY1:MB1 MH1:XFD1">
+  <conditionalFormatting sqref="LX1:MA1 A1:LV1 MG1:XFD1">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="LX1">
+  <conditionalFormatting sqref="LW1">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MG1">
+  <conditionalFormatting sqref="MF1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Some hardcoding for Sorcerer feats Sorcerer bloodline spells (Excel only, no conditions) Added spell level to shown spells
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="548" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{46946647-F178-4210-8344-CC854F9CEAD1}"/>
+  <xr:revisionPtr revIDLastSave="562" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{73D28394-ED53-484F-A1AB-0AFE66CA5F1E}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="1125" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5355" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2782" uniqueCount="1160">
   <si>
     <t>name</t>
   </si>
@@ -3620,10 +3620,23 @@
 These benefits last until you're no longer polymorphed into a plant.</t>
   </si>
   <si>
-    <t>Restores 1d6 Hit Points per spell level to the target creature when you cast the polymorph spell.</t>
-  </si>
-  <si>
     <t>Restore 1d6 Hit Points per spell level to the target creature when you cast the polymorph spell.</t>
+  </si>
+  <si>
+    <t>Counterspell (Spontaneous)</t>
+  </si>
+  <si>
+    <t>When a foe Casts a Spell and you can see its manifestations, you can use your own magic to disrupt it. You expend one of your spell slots to counter the triggering creature's casting of a spell that you have in your repertoire. You lose your spell slot as if you had cast the triggering spell. You then attempt to counteract the triggering spell.
+This feat has the trait corresponding to the tradition of spells you cast (arcane, divine, occult, or primal).</t>
+  </si>
+  <si>
+    <t>You have an unexpended spell slot you could use to cast the triggering spell.</t>
+  </si>
+  <si>
+    <t>You can use the triggering spell as a counterspell in your spell list.</t>
+  </si>
+  <si>
+    <t>Use the triggering spell as a counterspell in your spell list.</t>
   </si>
 </sst>
 </file>
@@ -4162,7 +4175,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6380,13 +6403,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A7:A10 A1:A5">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6394,23 +6417,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:MF93"/>
+  <dimension ref="A1:MG93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="LT2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="MD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="LX3" sqref="LX3"/>
+      <selection pane="bottomRight" activeCell="MG12" sqref="MG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="344" width="27.42578125" style="1" customWidth="1"/>
-    <col min="345" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="345" width="27.42578125" style="1" customWidth="1"/>
+    <col min="346" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:344" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:345" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7443,8 +7466,11 @@
       <c r="MF1" t="s">
         <v>1151</v>
       </c>
+      <c r="MG1" t="s">
+        <v>1155</v>
+      </c>
     </row>
-    <row r="2" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8468,8 +8494,11 @@
       <c r="MF2" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="MG2" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="3" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -8617,6 +8646,9 @@
       <c r="GE3" s="1" t="s">
         <v>618</v>
       </c>
+      <c r="HM3" s="1" t="s">
+        <v>1159</v>
+      </c>
       <c r="HU3" s="1" t="s">
         <v>721</v>
       </c>
@@ -8660,13 +8692,16 @@
         <v>1092</v>
       </c>
       <c r="LX3" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="MC3" s="1" t="s">
         <v>1149</v>
       </c>
+      <c r="MG3" s="1" t="s">
+        <v>1158</v>
+      </c>
     </row>
-    <row r="4" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -9642,8 +9677,11 @@
       <c r="MF4" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="MG4" s="2" t="s">
+        <v>696</v>
+      </c>
     </row>
-    <row r="5" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -10313,8 +10351,11 @@
       <c r="MF5" s="2" t="s">
         <v>152</v>
       </c>
+      <c r="MG5" s="2" t="s">
+        <v>344</v>
+      </c>
     </row>
-    <row r="6" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -10679,7 +10720,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -10930,7 +10971,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="8" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -11076,7 +11117,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -11102,7 +11143,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -11116,7 +11157,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="11" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -11426,8 +11467,11 @@
       <c r="LY11" s="1" t="s">
         <v>1134</v>
       </c>
+      <c r="MG11" s="1" t="s">
+        <v>1157</v>
+      </c>
     </row>
-    <row r="12" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -11638,8 +11682,11 @@
       <c r="LT12" s="1" t="s">
         <v>1122</v>
       </c>
+      <c r="MG12" s="1" t="s">
+        <v>697</v>
+      </c>
     </row>
-    <row r="13" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -11812,7 +11859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1100</v>
       </c>
@@ -11820,7 +11867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -11831,7 +11878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -11839,7 +11886,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -11959,7 +12006,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -12087,7 +12134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -12098,7 +12145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -12139,7 +12186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -13172,8 +13219,11 @@
       <c r="MF21" s="1" t="s">
         <v>1152</v>
       </c>
+      <c r="MG21" s="1" t="s">
+        <v>1156</v>
+      </c>
     </row>
-    <row r="22" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:345" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -13190,7 +13240,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="23" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -13249,7 +13299,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="24" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -13317,7 +13367,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="25" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -13391,7 +13441,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="26" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
@@ -13450,7 +13500,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="27" spans="1:344" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -13467,7 +13517,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="28" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
@@ -13478,7 +13528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>1049</v>
       </c>
@@ -13486,7 +13536,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="30" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>1101</v>
       </c>
@@ -13494,7 +13544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -13817,7 +13867,7 @@
         <v>144000</v>
       </c>
     </row>
-    <row r="32" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -15094,13 +15144,16 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A85:KK93">
     <sortCondition ref="A85:A93"/>
   </sortState>
-  <conditionalFormatting sqref="LX1:MA1 A1:LV1 MG1:XFD1">
+  <conditionalFormatting sqref="LX1:MA1 A1:LV1 MH1:XFD1">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="LW1">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="LW1">
+  <conditionalFormatting sqref="MF1">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MF1">
+  <conditionalFormatting sqref="MG1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prepared and converted Sorcerer feats Prepared and converted Sorcerer archetype Gave different durations to blood magic Allowed Skill increases that upgrade but don't provide a basis Allowed condition choices to be fixed depending on a subfeat you have Improved how you gain signature spells, and how many Hardcoded many feats Fixed basic Reach defaulting to 5 instead of 10 Fixed undefined ancestry showing in load character menu Fixed deprecated [className] tags Fixed html in json strings not working Fixed duplicate ID in weapons
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="562" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{73D28394-ED53-484F-A1AB-0AFE66CA5F1E}"/>
+  <xr:revisionPtr revIDLastSave="589" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F53D5BFF-19F4-4B3A-BC39-3CDAAB347A31}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18270" yWindow="1125" windowWidth="36645" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2782" uniqueCount="1160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2740" uniqueCount="1168">
   <si>
     <t>name</t>
   </si>
@@ -3551,11 +3551,6 @@
     <t>Pesh Skin</t>
   </si>
   <si>
-    <t>Your plant form sprouts hundreds of spines, and your blood causes mild hallucinations in creatures exposed to it. Each time a creature touches you, hits you with an unarmed attack, or hits you with a melee weapon attack while adjacent to you, that creature takes 1d6 piercing damage. Increase the damage to 2d6 if the polymorph spell is 8th level or higher, or to 3d6 if it’s 10th level.
-When an adjacent creature damages you with piercing or slashing damage, it must succeed at a Fortitude save against your class DC or become stupefied 1 (or stupefied 2 on a critical failure) until the end of its next turn.
-These benefits last until you’re no longer polymorphed into a plant.</t>
-  </si>
-  <si>
     <t>You are transformed into a plant by a polymorph spell.</t>
   </si>
   <si>
@@ -3637,6 +3632,33 @@
   </si>
   <si>
     <t>Use the triggering spell as a counterspell in your spell list.</t>
+  </si>
+  <si>
+    <t>Interweave Dispel</t>
+  </si>
+  <si>
+    <t>You weave dispelling energy into a spell, sending both effects at a foe. If your next action is to cast a single-target spell against a creature, and you either hit the foe with the spell attack roll or the foe fails its saving throw, you can cast dispel magic on the foe as a free action, expending a spell slot as normal and targeting one spell effect affecting the foe.</t>
+  </si>
+  <si>
+    <t>Cast dispel magic from your spell repertoire as a free action.</t>
+  </si>
+  <si>
+    <t>Bloodline Conduit</t>
+  </si>
+  <si>
+    <t>Your inborn magical nature lets you redirect ambient energies to fuel your spells. If your next action is to Cast a Spell of 5th level or lower that has no duration, you don't expend the spell's slot when you cast it.</t>
+  </si>
+  <si>
+    <t>Tenacious Blood Magic</t>
+  </si>
+  <si>
+    <t>You apply an effect from your blood magic that lasts for 1 round.</t>
+  </si>
+  <si>
+    <t>You have learned how to invest magic more deeply by witnessing Aroden's works. The triggering blood magic effect lasts for 1 minute instead of 1 round.</t>
+  </si>
+  <si>
+    <t>Manually change the duration of the blood magic effect.</t>
   </si>
 </sst>
 </file>
@@ -4175,17 +4197,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4556,11 +4568,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CO15"/>
+  <dimension ref="A1:CO5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4847,27 +4857,31 @@
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1114</v>
+        <v>1154</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1157</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>342</v>
+        <v>696</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>343</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>697</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -4877,7 +4891,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>1115</v>
+        <v>1155</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="3"/>
@@ -4888,15 +4902,9 @@
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
-      <c r="AE2" s="4">
-        <v>5</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>1114</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>1114</v>
-      </c>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
       <c r="AH2" s="7"/>
       <c r="AI2" s="4"/>
       <c r="AJ2" s="4"/>
@@ -4960,27 +4968,27 @@
     </row>
     <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1121</v>
+        <v>1159</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1161</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>343</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>344</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="1" t="s">
-        <v>1123</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>1122</v>
-      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -4990,7 +4998,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1" t="s">
-        <v>1124</v>
+        <v>1160</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="3"/>
@@ -5053,21 +5061,11 @@
       <c r="CB3" s="4"/>
       <c r="CC3" s="4"/>
       <c r="CD3" s="4"/>
-      <c r="CE3" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="CF3" s="5">
-        <v>-1</v>
-      </c>
-      <c r="CG3" s="8" t="s">
-        <v>733</v>
-      </c>
-      <c r="CH3" s="6">
-        <v>0</v>
-      </c>
-      <c r="CI3" s="6" t="s">
-        <v>1125</v>
-      </c>
+      <c r="CE3" s="5"/>
+      <c r="CF3" s="5"/>
+      <c r="CG3" s="8"/>
+      <c r="CH3" s="6"/>
+      <c r="CI3" s="6"/>
       <c r="CJ3" s="8"/>
       <c r="CK3" s="6"/>
       <c r="CL3" s="6"/>
@@ -5077,41 +5075,39 @@
     </row>
     <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1118</v>
+        <v>1162</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
-        <v>1119</v>
+        <v>343</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>187</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1" t="b">
-        <v>1</v>
-      </c>
+      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="Q4" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="R4" s="1">
+        <v>100</v>
+      </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1" t="s">
-        <v>1126</v>
+        <v>1163</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="3"/>
@@ -5122,12 +5118,14 @@
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
+      <c r="AE4" s="4">
+        <v>1</v>
+      </c>
       <c r="AF4" s="4" t="s">
-        <v>1118</v>
+        <v>1162</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>1118</v>
+        <v>1162</v>
       </c>
       <c r="AH4" s="7"/>
       <c r="AI4" s="4"/>
@@ -5192,33 +5190,43 @@
     </row>
     <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1120</v>
+        <v>1164</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1167</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>344</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1" t="s">
+        <v>1165</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="Q5" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="R5" s="1">
+        <v>100</v>
+      </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1" t="s">
-        <v>1127</v>
+        <v>1166</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="3"/>
@@ -5229,9 +5237,15 @@
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
+      <c r="AE5" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>1162</v>
+      </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="4"/>
       <c r="AJ5" s="4"/>
@@ -5293,1122 +5307,11 @@
       <c r="CN5" s="1"/>
       <c r="CO5" s="1"/>
     </row>
-    <row r="6" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1128</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1" t="s">
-        <v>1129</v>
-      </c>
-      <c r="V6" s="1"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="4"/>
-      <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="7"/>
-      <c r="AP6" s="4"/>
-      <c r="AQ6" s="4"/>
-      <c r="AR6" s="4"/>
-      <c r="AS6" s="4"/>
-      <c r="AT6" s="4"/>
-      <c r="AU6" s="7"/>
-      <c r="AV6" s="4"/>
-      <c r="AW6" s="4"/>
-      <c r="AX6" s="4"/>
-      <c r="AY6" s="4"/>
-      <c r="AZ6" s="4"/>
-      <c r="BA6" s="7"/>
-      <c r="BB6" s="4"/>
-      <c r="BC6" s="4"/>
-      <c r="BD6" s="4"/>
-      <c r="BE6" s="4"/>
-      <c r="BF6" s="4"/>
-      <c r="BG6" s="7"/>
-      <c r="BH6" s="4"/>
-      <c r="BI6" s="4"/>
-      <c r="BJ6" s="4"/>
-      <c r="BK6" s="4"/>
-      <c r="BL6" s="4"/>
-      <c r="BM6" s="7"/>
-      <c r="BN6" s="4"/>
-      <c r="BO6" s="4"/>
-      <c r="BP6" s="4"/>
-      <c r="BQ6" s="4"/>
-      <c r="BR6" s="4"/>
-      <c r="BS6" s="7"/>
-      <c r="BT6" s="4"/>
-      <c r="BU6" s="4"/>
-      <c r="BV6" s="4"/>
-      <c r="BW6" s="4"/>
-      <c r="BX6" s="4"/>
-      <c r="BY6" s="7"/>
-      <c r="BZ6" s="4"/>
-      <c r="CA6" s="4"/>
-      <c r="CB6" s="4"/>
-      <c r="CC6" s="4"/>
-      <c r="CD6" s="4"/>
-      <c r="CE6" s="5"/>
-      <c r="CF6" s="5"/>
-      <c r="CG6" s="8"/>
-      <c r="CH6" s="6"/>
-      <c r="CI6" s="6"/>
-      <c r="CJ6" s="8"/>
-      <c r="CK6" s="6"/>
-      <c r="CL6" s="6"/>
-      <c r="CM6" s="1"/>
-      <c r="CN6" s="1"/>
-      <c r="CO6" s="1"/>
-    </row>
-    <row r="7" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1" t="s">
-        <v>1131</v>
-      </c>
-      <c r="V7" s="1"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="4"/>
-      <c r="AF7" s="4"/>
-      <c r="AG7" s="4"/>
-      <c r="AH7" s="7"/>
-      <c r="AI7" s="4"/>
-      <c r="AJ7" s="4"/>
-      <c r="AK7" s="4"/>
-      <c r="AL7" s="4"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="4"/>
-      <c r="AO7" s="7"/>
-      <c r="AP7" s="4"/>
-      <c r="AQ7" s="4"/>
-      <c r="AR7" s="4"/>
-      <c r="AS7" s="4"/>
-      <c r="AT7" s="4"/>
-      <c r="AU7" s="7"/>
-      <c r="AV7" s="4"/>
-      <c r="AW7" s="4"/>
-      <c r="AX7" s="4"/>
-      <c r="AY7" s="4"/>
-      <c r="AZ7" s="4"/>
-      <c r="BA7" s="7"/>
-      <c r="BB7" s="4"/>
-      <c r="BC7" s="4"/>
-      <c r="BD7" s="4"/>
-      <c r="BE7" s="4"/>
-      <c r="BF7" s="4"/>
-      <c r="BG7" s="7"/>
-      <c r="BH7" s="4"/>
-      <c r="BI7" s="4"/>
-      <c r="BJ7" s="4"/>
-      <c r="BK7" s="4"/>
-      <c r="BL7" s="4"/>
-      <c r="BM7" s="7"/>
-      <c r="BN7" s="4"/>
-      <c r="BO7" s="4"/>
-      <c r="BP7" s="4"/>
-      <c r="BQ7" s="4"/>
-      <c r="BR7" s="4"/>
-      <c r="BS7" s="7"/>
-      <c r="BT7" s="4"/>
-      <c r="BU7" s="4"/>
-      <c r="BV7" s="4"/>
-      <c r="BW7" s="4"/>
-      <c r="BX7" s="4"/>
-      <c r="BY7" s="7"/>
-      <c r="BZ7" s="4"/>
-      <c r="CA7" s="4"/>
-      <c r="CB7" s="4"/>
-      <c r="CC7" s="4"/>
-      <c r="CD7" s="4"/>
-      <c r="CE7" s="5"/>
-      <c r="CF7" s="5"/>
-      <c r="CG7" s="8"/>
-      <c r="CH7" s="6"/>
-      <c r="CI7" s="6"/>
-      <c r="CJ7" s="8"/>
-      <c r="CK7" s="6"/>
-      <c r="CL7" s="6"/>
-      <c r="CM7" s="1"/>
-      <c r="CN7" s="1"/>
-      <c r="CO7" s="1"/>
-    </row>
-    <row r="8" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>1018</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="1" t="s">
-        <v>1134</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1" t="s">
-        <v>1133</v>
-      </c>
-      <c r="V8" s="1"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="4">
-        <v>-1</v>
-      </c>
-      <c r="AF8" s="4" t="s">
-        <v>1132</v>
-      </c>
-      <c r="AG8" s="4" t="s">
-        <v>1132</v>
-      </c>
-      <c r="AH8" s="7"/>
-      <c r="AI8" s="4"/>
-      <c r="AJ8" s="4"/>
-      <c r="AK8" s="4"/>
-      <c r="AL8" s="4"/>
-      <c r="AM8" s="4"/>
-      <c r="AN8" s="4"/>
-      <c r="AO8" s="7"/>
-      <c r="AP8" s="4"/>
-      <c r="AQ8" s="4"/>
-      <c r="AR8" s="4"/>
-      <c r="AS8" s="4"/>
-      <c r="AT8" s="4"/>
-      <c r="AU8" s="7"/>
-      <c r="AV8" s="4"/>
-      <c r="AW8" s="4"/>
-      <c r="AX8" s="4"/>
-      <c r="AY8" s="4"/>
-      <c r="AZ8" s="4"/>
-      <c r="BA8" s="7"/>
-      <c r="BB8" s="4"/>
-      <c r="BC8" s="4"/>
-      <c r="BD8" s="4"/>
-      <c r="BE8" s="4"/>
-      <c r="BF8" s="4"/>
-      <c r="BG8" s="7"/>
-      <c r="BH8" s="4"/>
-      <c r="BI8" s="4"/>
-      <c r="BJ8" s="4"/>
-      <c r="BK8" s="4"/>
-      <c r="BL8" s="4"/>
-      <c r="BM8" s="7"/>
-      <c r="BN8" s="4"/>
-      <c r="BO8" s="4"/>
-      <c r="BP8" s="4"/>
-      <c r="BQ8" s="4"/>
-      <c r="BR8" s="4"/>
-      <c r="BS8" s="7"/>
-      <c r="BT8" s="4"/>
-      <c r="BU8" s="4"/>
-      <c r="BV8" s="4"/>
-      <c r="BW8" s="4"/>
-      <c r="BX8" s="4"/>
-      <c r="BY8" s="7"/>
-      <c r="BZ8" s="4"/>
-      <c r="CA8" s="4"/>
-      <c r="CB8" s="4"/>
-      <c r="CC8" s="4"/>
-      <c r="CD8" s="4"/>
-      <c r="CE8" s="5"/>
-      <c r="CF8" s="5"/>
-      <c r="CG8" s="8"/>
-      <c r="CH8" s="6"/>
-      <c r="CI8" s="6"/>
-      <c r="CJ8" s="8"/>
-      <c r="CK8" s="6"/>
-      <c r="CL8" s="6"/>
-      <c r="CM8" s="1"/>
-      <c r="CN8" s="1"/>
-      <c r="CO8" s="1"/>
-    </row>
-    <row r="9" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1137</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1" t="s">
-        <v>1135</v>
-      </c>
-      <c r="V9" s="1"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="4">
-        <v>48000</v>
-      </c>
-      <c r="AF9" s="4" t="s">
-        <v>1136</v>
-      </c>
-      <c r="AG9" s="4" t="s">
-        <v>1137</v>
-      </c>
-      <c r="AH9" s="7"/>
-      <c r="AI9" s="4"/>
-      <c r="AJ9" s="4"/>
-      <c r="AK9" s="4"/>
-      <c r="AL9" s="4"/>
-      <c r="AM9" s="4"/>
-      <c r="AN9" s="4"/>
-      <c r="AO9" s="7"/>
-      <c r="AP9" s="4"/>
-      <c r="AQ9" s="4"/>
-      <c r="AR9" s="4"/>
-      <c r="AS9" s="4"/>
-      <c r="AT9" s="4"/>
-      <c r="AU9" s="7"/>
-      <c r="AV9" s="4"/>
-      <c r="AW9" s="4"/>
-      <c r="AX9" s="4"/>
-      <c r="AY9" s="4"/>
-      <c r="AZ9" s="4"/>
-      <c r="BA9" s="7"/>
-      <c r="BB9" s="4"/>
-      <c r="BC9" s="4"/>
-      <c r="BD9" s="4"/>
-      <c r="BE9" s="4"/>
-      <c r="BF9" s="4"/>
-      <c r="BG9" s="7"/>
-      <c r="BH9" s="4"/>
-      <c r="BI9" s="4"/>
-      <c r="BJ9" s="4"/>
-      <c r="BK9" s="4"/>
-      <c r="BL9" s="4"/>
-      <c r="BM9" s="7"/>
-      <c r="BN9" s="4"/>
-      <c r="BO9" s="4"/>
-      <c r="BP9" s="4"/>
-      <c r="BQ9" s="4"/>
-      <c r="BR9" s="4"/>
-      <c r="BS9" s="7"/>
-      <c r="BT9" s="4"/>
-      <c r="BU9" s="4"/>
-      <c r="BV9" s="4"/>
-      <c r="BW9" s="4"/>
-      <c r="BX9" s="4"/>
-      <c r="BY9" s="7"/>
-      <c r="BZ9" s="4"/>
-      <c r="CA9" s="4"/>
-      <c r="CB9" s="4"/>
-      <c r="CC9" s="4"/>
-      <c r="CD9" s="4"/>
-      <c r="CE9" s="5"/>
-      <c r="CF9" s="5"/>
-      <c r="CG9" s="8"/>
-      <c r="CH9" s="6"/>
-      <c r="CI9" s="6"/>
-      <c r="CJ9" s="8"/>
-      <c r="CK9" s="6"/>
-      <c r="CL9" s="6"/>
-      <c r="CM9" s="1"/>
-      <c r="CN9" s="1"/>
-      <c r="CO9" s="1"/>
-    </row>
-    <row r="10" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1138</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="R10" s="1">
-        <v>10</v>
-      </c>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1" t="s">
-        <v>1139</v>
-      </c>
-      <c r="V10" s="1"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="4"/>
-      <c r="AC10" s="4"/>
-      <c r="AD10" s="4"/>
-      <c r="AE10" s="4"/>
-      <c r="AF10" s="4"/>
-      <c r="AG10" s="4"/>
-      <c r="AH10" s="7"/>
-      <c r="AI10" s="4"/>
-      <c r="AJ10" s="4"/>
-      <c r="AK10" s="4"/>
-      <c r="AL10" s="4"/>
-      <c r="AM10" s="4"/>
-      <c r="AN10" s="4"/>
-      <c r="AO10" s="7"/>
-      <c r="AP10" s="4"/>
-      <c r="AQ10" s="4"/>
-      <c r="AR10" s="4"/>
-      <c r="AS10" s="4"/>
-      <c r="AT10" s="4"/>
-      <c r="AU10" s="7"/>
-      <c r="AV10" s="4"/>
-      <c r="AW10" s="4"/>
-      <c r="AX10" s="4"/>
-      <c r="AY10" s="4"/>
-      <c r="AZ10" s="4"/>
-      <c r="BA10" s="7"/>
-      <c r="BB10" s="4"/>
-      <c r="BC10" s="4"/>
-      <c r="BD10" s="4"/>
-      <c r="BE10" s="4"/>
-      <c r="BF10" s="4"/>
-      <c r="BG10" s="7"/>
-      <c r="BH10" s="4"/>
-      <c r="BI10" s="4"/>
-      <c r="BJ10" s="4"/>
-      <c r="BK10" s="4"/>
-      <c r="BL10" s="4"/>
-      <c r="BM10" s="7"/>
-      <c r="BN10" s="4"/>
-      <c r="BO10" s="4"/>
-      <c r="BP10" s="4"/>
-      <c r="BQ10" s="4"/>
-      <c r="BR10" s="4"/>
-      <c r="BS10" s="7"/>
-      <c r="BT10" s="4"/>
-      <c r="BU10" s="4"/>
-      <c r="BV10" s="4"/>
-      <c r="BW10" s="4"/>
-      <c r="BX10" s="4"/>
-      <c r="BY10" s="7"/>
-      <c r="BZ10" s="4"/>
-      <c r="CA10" s="4"/>
-      <c r="CB10" s="4"/>
-      <c r="CC10" s="4"/>
-      <c r="CD10" s="4"/>
-      <c r="CE10" s="5"/>
-      <c r="CF10" s="5"/>
-      <c r="CG10" s="8"/>
-      <c r="CH10" s="6"/>
-      <c r="CI10" s="6"/>
-      <c r="CJ10" s="8"/>
-      <c r="CK10" s="6"/>
-      <c r="CL10" s="6"/>
-      <c r="CM10" s="1"/>
-      <c r="CN10" s="1"/>
-      <c r="CO10" s="1"/>
-    </row>
-    <row r="11" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1140</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1" t="s">
-        <v>824</v>
-      </c>
-      <c r="R11" s="1">
-        <v>100</v>
-      </c>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1" t="s">
-        <v>1150</v>
-      </c>
-      <c r="V11" s="1"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="4"/>
-      <c r="AC11" s="4"/>
-      <c r="AD11" s="4"/>
-      <c r="AE11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AF11" s="4" t="s">
-        <v>1140</v>
-      </c>
-      <c r="AG11" s="4" t="s">
-        <v>1140</v>
-      </c>
-      <c r="AH11" s="7"/>
-      <c r="AI11" s="4"/>
-      <c r="AJ11" s="4"/>
-      <c r="AK11" s="4"/>
-      <c r="AL11" s="4"/>
-      <c r="AM11" s="4"/>
-      <c r="AN11" s="4"/>
-      <c r="AO11" s="7"/>
-      <c r="AP11" s="4"/>
-      <c r="AQ11" s="4"/>
-      <c r="AR11" s="4"/>
-      <c r="AS11" s="4"/>
-      <c r="AT11" s="4"/>
-      <c r="AU11" s="7"/>
-      <c r="AV11" s="4"/>
-      <c r="AW11" s="4"/>
-      <c r="AX11" s="4"/>
-      <c r="AY11" s="4"/>
-      <c r="AZ11" s="4"/>
-      <c r="BA11" s="7"/>
-      <c r="BB11" s="4"/>
-      <c r="BC11" s="4"/>
-      <c r="BD11" s="4"/>
-      <c r="BE11" s="4"/>
-      <c r="BF11" s="4"/>
-      <c r="BG11" s="7"/>
-      <c r="BH11" s="4"/>
-      <c r="BI11" s="4"/>
-      <c r="BJ11" s="4"/>
-      <c r="BK11" s="4"/>
-      <c r="BL11" s="4"/>
-      <c r="BM11" s="7"/>
-      <c r="BN11" s="4"/>
-      <c r="BO11" s="4"/>
-      <c r="BP11" s="4"/>
-      <c r="BQ11" s="4"/>
-      <c r="BR11" s="4"/>
-      <c r="BS11" s="7"/>
-      <c r="BT11" s="4"/>
-      <c r="BU11" s="4"/>
-      <c r="BV11" s="4"/>
-      <c r="BW11" s="4"/>
-      <c r="BX11" s="4"/>
-      <c r="BY11" s="7"/>
-      <c r="BZ11" s="4"/>
-      <c r="CA11" s="4"/>
-      <c r="CB11" s="4"/>
-      <c r="CC11" s="4"/>
-      <c r="CD11" s="4"/>
-      <c r="CE11" s="5"/>
-      <c r="CF11" s="5"/>
-      <c r="CG11" s="8"/>
-      <c r="CH11" s="6"/>
-      <c r="CI11" s="6"/>
-      <c r="CJ11" s="8"/>
-      <c r="CK11" s="6"/>
-      <c r="CL11" s="6"/>
-      <c r="CM11" s="1"/>
-      <c r="CN11" s="1"/>
-      <c r="CO11" s="1"/>
-    </row>
-    <row r="12" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>1149</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1" t="s">
-        <v>1144</v>
-      </c>
-      <c r="V12" s="1"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="4"/>
-      <c r="AC12" s="4"/>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="4"/>
-      <c r="AF12" s="4"/>
-      <c r="AG12" s="4"/>
-      <c r="AH12" s="7"/>
-      <c r="AI12" s="4"/>
-      <c r="AJ12" s="4"/>
-      <c r="AK12" s="4"/>
-      <c r="AL12" s="4"/>
-      <c r="AM12" s="4"/>
-      <c r="AN12" s="4"/>
-      <c r="AO12" s="7"/>
-      <c r="AP12" s="4"/>
-      <c r="AQ12" s="4"/>
-      <c r="AR12" s="4"/>
-      <c r="AS12" s="4"/>
-      <c r="AT12" s="4"/>
-      <c r="AU12" s="7"/>
-      <c r="AV12" s="4"/>
-      <c r="AW12" s="4"/>
-      <c r="AX12" s="4"/>
-      <c r="AY12" s="4"/>
-      <c r="AZ12" s="4"/>
-      <c r="BA12" s="7"/>
-      <c r="BB12" s="4"/>
-      <c r="BC12" s="4"/>
-      <c r="BD12" s="4"/>
-      <c r="BE12" s="4"/>
-      <c r="BF12" s="4"/>
-      <c r="BG12" s="7"/>
-      <c r="BH12" s="4"/>
-      <c r="BI12" s="4"/>
-      <c r="BJ12" s="4"/>
-      <c r="BK12" s="4"/>
-      <c r="BL12" s="4"/>
-      <c r="BM12" s="7"/>
-      <c r="BN12" s="4"/>
-      <c r="BO12" s="4"/>
-      <c r="BP12" s="4"/>
-      <c r="BQ12" s="4"/>
-      <c r="BR12" s="4"/>
-      <c r="BS12" s="7"/>
-      <c r="BT12" s="4"/>
-      <c r="BU12" s="4"/>
-      <c r="BV12" s="4"/>
-      <c r="BW12" s="4"/>
-      <c r="BX12" s="4"/>
-      <c r="BY12" s="7"/>
-      <c r="BZ12" s="4"/>
-      <c r="CA12" s="4"/>
-      <c r="CB12" s="4"/>
-      <c r="CC12" s="4"/>
-      <c r="CD12" s="4"/>
-      <c r="CE12" s="5"/>
-      <c r="CF12" s="5"/>
-      <c r="CG12" s="8"/>
-      <c r="CH12" s="6"/>
-      <c r="CI12" s="6"/>
-      <c r="CJ12" s="8"/>
-      <c r="CK12" s="6"/>
-      <c r="CL12" s="6"/>
-      <c r="CM12" s="1"/>
-      <c r="CN12" s="1"/>
-      <c r="CO12" s="1"/>
-    </row>
-    <row r="13" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1143</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="R13" s="1">
-        <v>144000</v>
-      </c>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1" t="s">
-        <v>1145</v>
-      </c>
-      <c r="V13" s="1"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4">
-        <v>100</v>
-      </c>
-      <c r="AF13" s="4" t="s">
-        <v>1147</v>
-      </c>
-      <c r="AG13" s="4" t="s">
-        <v>1141</v>
-      </c>
-      <c r="AH13" s="7"/>
-      <c r="AI13" s="4"/>
-      <c r="AJ13" s="4"/>
-      <c r="AK13" s="4"/>
-      <c r="AL13" s="4"/>
-      <c r="AM13" s="4"/>
-      <c r="AN13" s="4"/>
-      <c r="AO13" s="7"/>
-      <c r="AP13" s="4"/>
-      <c r="AQ13" s="4"/>
-      <c r="AR13" s="4"/>
-      <c r="AS13" s="4"/>
-      <c r="AT13" s="4"/>
-      <c r="AU13" s="7"/>
-      <c r="AV13" s="4"/>
-      <c r="AW13" s="4"/>
-      <c r="AX13" s="4"/>
-      <c r="AY13" s="4"/>
-      <c r="AZ13" s="4"/>
-      <c r="BA13" s="7"/>
-      <c r="BB13" s="4"/>
-      <c r="BC13" s="4"/>
-      <c r="BD13" s="4"/>
-      <c r="BE13" s="4"/>
-      <c r="BF13" s="4"/>
-      <c r="BG13" s="7"/>
-      <c r="BH13" s="4"/>
-      <c r="BI13" s="4"/>
-      <c r="BJ13" s="4"/>
-      <c r="BK13" s="4"/>
-      <c r="BL13" s="4"/>
-      <c r="BM13" s="7"/>
-      <c r="BN13" s="4"/>
-      <c r="BO13" s="4"/>
-      <c r="BP13" s="4"/>
-      <c r="BQ13" s="4"/>
-      <c r="BR13" s="4"/>
-      <c r="BS13" s="7"/>
-      <c r="BT13" s="4"/>
-      <c r="BU13" s="4"/>
-      <c r="BV13" s="4"/>
-      <c r="BW13" s="4"/>
-      <c r="BX13" s="4"/>
-      <c r="BY13" s="7"/>
-      <c r="BZ13" s="4"/>
-      <c r="CA13" s="4"/>
-      <c r="CB13" s="4"/>
-      <c r="CC13" s="4"/>
-      <c r="CD13" s="4"/>
-      <c r="CE13" s="5"/>
-      <c r="CF13" s="5"/>
-      <c r="CG13" s="8"/>
-      <c r="CH13" s="6"/>
-      <c r="CI13" s="6"/>
-      <c r="CJ13" s="8"/>
-      <c r="CK13" s="6"/>
-      <c r="CL13" s="6"/>
-      <c r="CM13" s="1"/>
-      <c r="CN13" s="1">
-        <v>10</v>
-      </c>
-      <c r="CO13" s="1" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1142</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="R14" s="1">
-        <v>6000</v>
-      </c>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1" t="s">
-        <v>1148</v>
-      </c>
-      <c r="V14" s="1"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AA14" s="7"/>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="4">
-        <v>144000</v>
-      </c>
-      <c r="AF14" s="4" t="s">
-        <v>1142</v>
-      </c>
-      <c r="AG14" s="4" t="s">
-        <v>1142</v>
-      </c>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="4"/>
-      <c r="AJ14" s="4"/>
-      <c r="AK14" s="4"/>
-      <c r="AL14" s="4"/>
-      <c r="AM14" s="4"/>
-      <c r="AN14" s="4"/>
-      <c r="AO14" s="7"/>
-      <c r="AP14" s="4"/>
-      <c r="AQ14" s="4"/>
-      <c r="AR14" s="4"/>
-      <c r="AS14" s="4"/>
-      <c r="AT14" s="4"/>
-      <c r="AU14" s="7"/>
-      <c r="AV14" s="4"/>
-      <c r="AW14" s="4"/>
-      <c r="AX14" s="4"/>
-      <c r="AY14" s="4"/>
-      <c r="AZ14" s="4"/>
-      <c r="BA14" s="7"/>
-      <c r="BB14" s="4"/>
-      <c r="BC14" s="4"/>
-      <c r="BD14" s="4"/>
-      <c r="BE14" s="4"/>
-      <c r="BF14" s="4"/>
-      <c r="BG14" s="7"/>
-      <c r="BH14" s="4"/>
-      <c r="BI14" s="4"/>
-      <c r="BJ14" s="4"/>
-      <c r="BK14" s="4"/>
-      <c r="BL14" s="4"/>
-      <c r="BM14" s="7"/>
-      <c r="BN14" s="4"/>
-      <c r="BO14" s="4"/>
-      <c r="BP14" s="4"/>
-      <c r="BQ14" s="4"/>
-      <c r="BR14" s="4"/>
-      <c r="BS14" s="7"/>
-      <c r="BT14" s="4"/>
-      <c r="BU14" s="4"/>
-      <c r="BV14" s="4"/>
-      <c r="BW14" s="4"/>
-      <c r="BX14" s="4"/>
-      <c r="BY14" s="7"/>
-      <c r="BZ14" s="4"/>
-      <c r="CA14" s="4"/>
-      <c r="CB14" s="4"/>
-      <c r="CC14" s="4"/>
-      <c r="CD14" s="4"/>
-      <c r="CE14" s="5"/>
-      <c r="CF14" s="5"/>
-      <c r="CG14" s="8"/>
-      <c r="CH14" s="6"/>
-      <c r="CI14" s="6"/>
-      <c r="CJ14" s="8"/>
-      <c r="CK14" s="6"/>
-      <c r="CL14" s="6"/>
-      <c r="CM14" s="1"/>
-      <c r="CN14" s="1"/>
-      <c r="CO14" s="1"/>
-    </row>
-    <row r="15" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1151</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="R15" s="1">
-        <v>10</v>
-      </c>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1" t="s">
-        <v>1152</v>
-      </c>
-      <c r="V15" s="1"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
-      <c r="AG15" s="4"/>
-      <c r="AH15" s="7"/>
-      <c r="AI15" s="4"/>
-      <c r="AJ15" s="4"/>
-      <c r="AK15" s="4"/>
-      <c r="AL15" s="4"/>
-      <c r="AM15" s="4"/>
-      <c r="AN15" s="4"/>
-      <c r="AO15" s="7"/>
-      <c r="AP15" s="4"/>
-      <c r="AQ15" s="4"/>
-      <c r="AR15" s="4"/>
-      <c r="AS15" s="4"/>
-      <c r="AT15" s="4"/>
-      <c r="AU15" s="7"/>
-      <c r="AV15" s="4"/>
-      <c r="AW15" s="4"/>
-      <c r="AX15" s="4"/>
-      <c r="AY15" s="4"/>
-      <c r="AZ15" s="4"/>
-      <c r="BA15" s="7"/>
-      <c r="BB15" s="4"/>
-      <c r="BC15" s="4"/>
-      <c r="BD15" s="4"/>
-      <c r="BE15" s="4"/>
-      <c r="BF15" s="4"/>
-      <c r="BG15" s="7"/>
-      <c r="BH15" s="4"/>
-      <c r="BI15" s="4"/>
-      <c r="BJ15" s="4"/>
-      <c r="BK15" s="4"/>
-      <c r="BL15" s="4"/>
-      <c r="BM15" s="7"/>
-      <c r="BN15" s="4"/>
-      <c r="BO15" s="4"/>
-      <c r="BP15" s="4"/>
-      <c r="BQ15" s="4"/>
-      <c r="BR15" s="4"/>
-      <c r="BS15" s="7"/>
-      <c r="BT15" s="4"/>
-      <c r="BU15" s="4"/>
-      <c r="BV15" s="4"/>
-      <c r="BW15" s="4"/>
-      <c r="BX15" s="4"/>
-      <c r="BY15" s="7"/>
-      <c r="BZ15" s="4"/>
-      <c r="CA15" s="4"/>
-      <c r="CB15" s="4"/>
-      <c r="CC15" s="4"/>
-      <c r="CD15" s="4"/>
-      <c r="CE15" s="5"/>
-      <c r="CF15" s="5"/>
-      <c r="CG15" s="8"/>
-      <c r="CH15" s="6"/>
-      <c r="CI15" s="6"/>
-      <c r="CJ15" s="8"/>
-      <c r="CK15" s="6"/>
-      <c r="CL15" s="6"/>
-      <c r="CM15" s="1"/>
-      <c r="CN15" s="1"/>
-      <c r="CO15" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A7:A10 A1:A5">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+  <conditionalFormatting sqref="A3 A1">
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
+  <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6417,23 +5320,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:MG93"/>
+  <dimension ref="A1:MJ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="MD2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="MD65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="MG12" sqref="MG12"/>
+      <selection pane="bottomRight" sqref="A1:MJ93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="345" width="27.42578125" style="1" customWidth="1"/>
-    <col min="346" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="348" width="27.42578125" style="1" customWidth="1"/>
+    <col min="349" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:345" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:348" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7446,31 +6349,40 @@
         <v>1132</v>
       </c>
       <c r="LZ1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="MA1" t="s">
         <v>1137</v>
       </c>
-      <c r="MA1" t="s">
-        <v>1138</v>
-      </c>
       <c r="MB1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="MC1" t="s">
         <v>1140</v>
       </c>
-      <c r="MC1" t="s">
+      <c r="MD1" t="s">
+        <v>1142</v>
+      </c>
+      <c r="ME1" t="s">
         <v>1141</v>
       </c>
-      <c r="MD1" t="s">
-        <v>1143</v>
-      </c>
-      <c r="ME1" t="s">
-        <v>1142</v>
-      </c>
       <c r="MF1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="MG1" t="s">
-        <v>1155</v>
+        <v>1154</v>
+      </c>
+      <c r="MH1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="MI1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="MJ1" t="s">
+        <v>1164</v>
       </c>
     </row>
-    <row r="2" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8497,8 +7409,17 @@
       <c r="MG2" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="MH2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MI2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="MJ2" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="3" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -8647,7 +7568,7 @@
         <v>618</v>
       </c>
       <c r="HM3" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="HU3" s="1" t="s">
         <v>721</v>
@@ -8692,16 +7613,22 @@
         <v>1092</v>
       </c>
       <c r="LX3" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="MC3" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="MG3" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
+      </c>
+      <c r="MH3" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="MJ3" s="1" t="s">
+        <v>1167</v>
       </c>
     </row>
-    <row r="4" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:348" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -9680,8 +8607,17 @@
       <c r="MG4" s="2" t="s">
         <v>696</v>
       </c>
+      <c r="MH4" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="MI4" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="MJ4" s="2" t="s">
+        <v>195</v>
+      </c>
     </row>
-    <row r="5" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:348" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -10354,8 +9290,17 @@
       <c r="MG5" s="2" t="s">
         <v>344</v>
       </c>
+      <c r="MH5" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="MI5" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="MJ5" s="2" t="s">
+        <v>344</v>
+      </c>
     </row>
-    <row r="6" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:348" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -10720,7 +9665,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:348" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -10971,7 +9916,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="8" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:348" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -11117,7 +10062,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:348" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -11143,7 +10088,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:348" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -11157,7 +10102,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="11" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -11465,13 +10410,13 @@
         <v>1123</v>
       </c>
       <c r="LY11" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="MG11" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
-    <row r="12" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -11685,8 +10630,11 @@
       <c r="MG12" s="1" t="s">
         <v>697</v>
       </c>
+      <c r="MJ12" s="1" t="s">
+        <v>1165</v>
+      </c>
     </row>
-    <row r="13" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -11859,7 +10807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1100</v>
       </c>
@@ -11867,7 +10815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -11878,7 +10826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -11886,7 +10834,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -12005,8 +10953,14 @@
       <c r="MF17" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="MI17" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="MJ17" s="1" t="s">
+        <v>824</v>
+      </c>
     </row>
-    <row r="18" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -12133,8 +11087,14 @@
       <c r="MF18" s="1">
         <v>10</v>
       </c>
+      <c r="MI18" s="1">
+        <v>100</v>
+      </c>
+      <c r="MJ18" s="1">
+        <v>100</v>
+      </c>
     </row>
-    <row r="19" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -12145,7 +11105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -12186,7 +11146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -13196,34 +12156,43 @@
         <v>1131</v>
       </c>
       <c r="LY21" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="LZ21" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="MA21" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="MB21" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="MC21" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="MD21" s="1" t="s">
         <v>1144</v>
       </c>
-      <c r="MD21" s="1" t="s">
-        <v>1145</v>
-      </c>
       <c r="ME21" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="MF21" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="MG21" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
+      </c>
+      <c r="MH21" s="1" t="s">
+        <v>1160</v>
+      </c>
+      <c r="MI21" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="MJ21" s="1" t="s">
+        <v>1166</v>
       </c>
     </row>
-    <row r="22" spans="1:345" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:348" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -13240,7 +12209,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="23" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:348" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -13299,7 +12268,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="24" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:348" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -13367,7 +12336,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="25" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:348" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -13441,7 +12410,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="26" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:348" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
@@ -13500,7 +12469,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="27" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:348" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -13517,7 +12486,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="28" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
@@ -13528,7 +12497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>1049</v>
       </c>
@@ -13536,7 +12505,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="30" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>1101</v>
       </c>
@@ -13544,7 +12513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -13866,8 +12835,14 @@
       <c r="ME31" s="4">
         <v>144000</v>
       </c>
+      <c r="MI31" s="4">
+        <v>1</v>
+      </c>
+      <c r="MJ31" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -14202,19 +13177,25 @@
         <v>1132</v>
       </c>
       <c r="LZ32" s="4" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="MB32" s="4" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="MD32" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="ME32" s="4" t="s">
-        <v>1142</v>
+        <v>1141</v>
+      </c>
+      <c r="MI32" s="4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="MJ32" s="4" t="s">
+        <v>1162</v>
       </c>
     </row>
-    <row r="33" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>9</v>
       </c>
@@ -14543,19 +13524,25 @@
         <v>1132</v>
       </c>
       <c r="LZ33" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="MB33" s="4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="MD33" s="4" t="s">
         <v>1140</v>
       </c>
-      <c r="MD33" s="4" t="s">
+      <c r="ME33" s="4" t="s">
         <v>1141</v>
       </c>
-      <c r="ME33" s="4" t="s">
-        <v>1142</v>
+      <c r="MI33" s="4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="MJ33" s="4" t="s">
+        <v>1162</v>
       </c>
     </row>
-    <row r="34" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:348" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>29</v>
       </c>
@@ -14566,7 +13553,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="35" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>1050</v>
       </c>
@@ -14574,7 +13561,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="36" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>1109</v>
       </c>
@@ -14582,7 +13569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>26</v>
       </c>
@@ -14590,7 +13577,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>27</v>
       </c>
@@ -14607,7 +13594,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="39" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>28</v>
       </c>
@@ -14624,7 +13611,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="40" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>47</v>
       </c>
@@ -14632,7 +13619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:348" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
@@ -14643,7 +13630,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="42" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>1054</v>
       </c>
@@ -14651,7 +13638,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="43" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>1108</v>
       </c>
@@ -14659,7 +13646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
@@ -14667,7 +13654,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>31</v>
       </c>
@@ -14678,7 +13665,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="46" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>32</v>
       </c>
@@ -14689,7 +13676,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="47" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:348" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>1055</v>
       </c>
@@ -14697,7 +13684,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="48" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:348" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>1056</v>
       </c>
@@ -15137,14 +14124,14 @@
         <v>1111</v>
       </c>
       <c r="MD93" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A85:KK93">
     <sortCondition ref="A85:A93"/>
   </sortState>
-  <conditionalFormatting sqref="LX1:MA1 A1:LV1 MH1:XFD1">
+  <conditionalFormatting sqref="LX1:MA1 A1:LV1 MH1 MK1:XFD1">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="LW1">

</xml_diff>

<commit_message>
Implemented tile mode and choice area content for spell choices Tested more level 5 spells
</commit_message>
<xml_diff>
--- a/activities.xlsx
+++ b/activities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb76e5660c890129/Personal/Projects/Design/Patherpoint/patherpoint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="603" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{32EF4236-F062-4347-BEA6-82CDA700B047}"/>
+  <xr:revisionPtr revIDLastSave="617" documentId="13_ncr:40009_{E3EB266C-7612-416D-8781-7A2BED99FA57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AED4E7A3-AA7A-4967-AB5B-EDB7452BC0EC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="368" yWindow="968" windowWidth="19050" windowHeight="11512" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activities" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2702" uniqueCount="1156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2707" uniqueCount="1161">
   <si>
     <t>name</t>
   </si>
@@ -3628,6 +3628,21 @@
   </si>
   <si>
     <t>Your most recent action was to cast a non-cantrip spell.</t>
+  </si>
+  <si>
+    <t>Crushing Despair: Fail Save</t>
+  </si>
+  <si>
+    <t>While crushing despair is active, you must attempt another save against the spell at the start of your turn; on a failure, you are slowed 1 for that turn as you sob uncontrollably.</t>
+  </si>
+  <si>
+    <t>Slowed</t>
+  </si>
+  <si>
+    <t>Crushing Despair: Failed Save</t>
+  </si>
+  <si>
+    <t>gainConditions/0/value</t>
   </si>
 </sst>
 </file>
@@ -4541,9 +4556,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:93" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4824,7 +4839,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:93" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1139</v>
       </c>
@@ -4935,7 +4950,7 @@
       <c r="CN2" s="1"/>
       <c r="CO2" s="1"/>
     </row>
-    <row r="3" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:93" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1144</v>
       </c>
@@ -5042,7 +5057,7 @@
       <c r="CN3" s="1"/>
       <c r="CO3" s="1"/>
     </row>
-    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1147</v>
       </c>
@@ -5157,7 +5172,7 @@
       <c r="CN4" s="1"/>
       <c r="CO4" s="1"/>
     </row>
-    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:93" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1149</v>
       </c>
@@ -5289,23 +5304,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:MF93"/>
+  <dimension ref="A1:MG94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="LV5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="ME2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="LX20" sqref="LX20"/>
+      <selection pane="bottomRight" activeCell="MG17" sqref="MG17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="344" width="27.42578125" style="1" customWidth="1"/>
-    <col min="345" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="37.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="345" width="27.3984375" style="1" customWidth="1"/>
+    <col min="346" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:344" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:345" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6338,8 +6353,11 @@
       <c r="MF1" t="s">
         <v>1149</v>
       </c>
+      <c r="MG1" t="s">
+        <v>1156</v>
+      </c>
     </row>
-    <row r="2" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7364,7 +7382,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -7573,7 +7591,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="4" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -8550,7 +8568,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -9221,7 +9239,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -9586,7 +9604,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -9837,7 +9855,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="8" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -9983,7 +10001,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -10009,7 +10027,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:344" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:345" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -10023,7 +10041,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="11" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -10325,7 +10343,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="12" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -10543,7 +10561,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="13" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -10722,7 +10740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>1085</v>
       </c>
@@ -10730,7 +10748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -10741,7 +10759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -10749,7 +10767,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -10863,7 +10881,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="18" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -10985,7 +11003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -10996,7 +11014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -11043,7 +11061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -12076,8 +12094,11 @@
       <c r="MF21" s="1" t="s">
         <v>1151</v>
       </c>
+      <c r="MG21" s="1" t="s">
+        <v>1157</v>
+      </c>
     </row>
-    <row r="22" spans="1:344" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:345" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -12094,7 +12115,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="23" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -12153,7 +12174,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="24" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
@@ -12221,7 +12242,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="25" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -12295,7 +12316,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="26" spans="1:344" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:345" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
@@ -12354,7 +12375,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="27" spans="1:344" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -12371,7 +12392,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="28" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
@@ -12382,7 +12403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>1034</v>
       </c>
@@ -12390,7 +12411,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="30" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>1086</v>
       </c>
@@ -12398,7 +12419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -12711,8 +12732,11 @@
       <c r="ME31" s="4">
         <v>1</v>
       </c>
+      <c r="MG31" s="4">
+        <v>5</v>
+      </c>
     </row>
-    <row r="32" spans="1:344" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -13049,8 +13073,11 @@
       <c r="ME32" s="4" t="s">
         <v>1147</v>
       </c>
+      <c r="MG32" s="4" t="s">
+        <v>1158</v>
+      </c>
     </row>
-    <row r="33" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
         <v>9</v>
       </c>
@@ -13381,133 +13408,133 @@
       <c r="ME33" s="4" t="s">
         <v>1147</v>
       </c>
+      <c r="MG33" s="4" t="s">
+        <v>1159</v>
+      </c>
     </row>
-    <row r="34" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="4" t="s">
+        <v>1160</v>
+      </c>
+      <c r="MG34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AQ34" s="7" t="s">
+      <c r="AQ35" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="KS34" s="7" t="s">
+      <c r="KS35" s="7" t="s">
         <v>1037</v>
       </c>
     </row>
-    <row r="35" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="36" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="4" t="s">
         <v>1035</v>
       </c>
-      <c r="KS35" s="4" t="s">
+      <c r="KS36" s="4" t="s">
         <v>1026</v>
       </c>
     </row>
-    <row r="36" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="37" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="4" t="s">
         <v>1094</v>
       </c>
-      <c r="KS36" s="4" t="b">
+      <c r="KS37" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="38" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AQ37" s="4">
+      <c r="AQ38" s="4">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="AQ38" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="JJ38" s="4" t="s">
-        <v>864</v>
-      </c>
-      <c r="KP38" s="4" t="s">
-        <v>1095</v>
-      </c>
-      <c r="KS38" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="39" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="AQ39" s="4" t="s">
         <v>196</v>
       </c>
       <c r="JJ39" s="4" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="KP39" s="4" t="s">
-        <v>942</v>
+        <v>1095</v>
       </c>
       <c r="KS39" s="4" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="40" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ40" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="JJ40" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="KP40" s="4" t="s">
+        <v>942</v>
+      </c>
+      <c r="KS40" s="4" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="41" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="JJ40" s="4">
+      <c r="JJ41" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AQ41" s="7" t="s">
+      <c r="AQ42" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="KS41" s="7" t="s">
+      <c r="KS42" s="7" t="s">
         <v>1036</v>
       </c>
     </row>
-    <row r="42" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="4" t="s">
         <v>1039</v>
       </c>
-      <c r="KS42" s="4" t="s">
+      <c r="KS43" s="4" t="s">
         <v>1027</v>
       </c>
     </row>
-    <row r="43" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+    <row r="44" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="4" t="s">
         <v>1093</v>
       </c>
-      <c r="KS43" s="4" t="b">
+      <c r="KS44" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="45" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AQ44" s="4">
+      <c r="AQ45" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="45" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+    <row r="46" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="AQ45" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="KS45" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="46" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="AQ46" s="4" t="s">
         <v>196</v>
@@ -13516,460 +13543,471 @@
         <v>945</v>
       </c>
     </row>
-    <row r="47" spans="1:343" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:345" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ47" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="KS47" s="4" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="48" spans="1:345" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="7" t="s">
         <v>1040</v>
       </c>
-      <c r="KS47" s="7" t="s">
+      <c r="KS48" s="7" t="s">
         <v>1070</v>
       </c>
     </row>
-    <row r="48" spans="1:343" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="49" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="4" t="s">
         <v>1041</v>
       </c>
-      <c r="KS48" s="4" t="s">
+      <c r="KS49" s="4" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="49" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+    <row r="50" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="4" t="s">
         <v>1092</v>
       </c>
-      <c r="KS49" s="4" t="b">
+      <c r="KS50" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="51" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="4" t="s">
         <v>1042</v>
       </c>
     </row>
-    <row r="51" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="52" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="4" t="s">
         <v>1043</v>
-      </c>
-      <c r="KS51" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="52" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>1044</v>
       </c>
       <c r="KS52" s="4" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="53" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+    <row r="53" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="4" t="s">
+        <v>1044</v>
+      </c>
+      <c r="KS53" s="4" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="54" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="7" t="s">
         <v>1045</v>
       </c>
-      <c r="KS53" s="7" t="s">
+      <c r="KS54" s="7" t="s">
         <v>1071</v>
       </c>
     </row>
-    <row r="54" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    <row r="55" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="4" t="s">
         <v>1046</v>
       </c>
-      <c r="KS54" s="4" t="s">
+      <c r="KS55" s="4" t="s">
         <v>1030</v>
       </c>
     </row>
-    <row r="55" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+    <row r="56" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="4" t="s">
         <v>1091</v>
       </c>
-      <c r="KS55" s="4" t="b">
+      <c r="KS56" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+    <row r="57" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="4" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="57" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="58" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="4" t="s">
         <v>1048</v>
-      </c>
-      <c r="KS57" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="58" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>1049</v>
       </c>
       <c r="KS58" s="4" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="59" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+    <row r="59" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="KS59" s="4" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="60" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="7" t="s">
         <v>1050</v>
       </c>
-      <c r="KS59" s="7" t="s">
+      <c r="KS60" s="7" t="s">
         <v>1072</v>
       </c>
     </row>
-    <row r="60" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+    <row r="61" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="4" t="s">
         <v>1051</v>
       </c>
-      <c r="KS60" s="4" t="s">
+      <c r="KS61" s="4" t="s">
         <v>1031</v>
       </c>
     </row>
-    <row r="61" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+    <row r="62" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="4" t="s">
         <v>1090</v>
       </c>
-      <c r="KS61" s="4" t="b">
+      <c r="KS62" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="63" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="4" t="s">
         <v>1052</v>
       </c>
     </row>
-    <row r="63" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+    <row r="64" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="4" t="s">
         <v>1053</v>
-      </c>
-      <c r="KS63" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="64" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>1054</v>
       </c>
       <c r="KS64" s="4" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="65" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
+    <row r="65" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="4" t="s">
+        <v>1054</v>
+      </c>
+      <c r="KS65" s="4" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="66" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="7" t="s">
         <v>1055</v>
       </c>
-      <c r="KS65" s="7" t="s">
+      <c r="KS66" s="7" t="s">
         <v>1073</v>
       </c>
     </row>
-    <row r="66" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+    <row r="67" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="4" t="s">
         <v>1056</v>
       </c>
-      <c r="KS66" s="4" t="s">
+      <c r="KS67" s="4" t="s">
         <v>1032</v>
       </c>
     </row>
-    <row r="67" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+    <row r="68" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A68" s="4" t="s">
         <v>1089</v>
       </c>
-      <c r="KS67" s="4" t="b">
+      <c r="KS68" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+    <row r="69" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="4" t="s">
         <v>1057</v>
       </c>
     </row>
-    <row r="69" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+    <row r="70" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="4" t="s">
         <v>1058</v>
-      </c>
-      <c r="KS69" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="70" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>1059</v>
       </c>
       <c r="KS70" s="4" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="71" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
+    <row r="71" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A71" s="4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="KS71" s="4" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="72" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A72" s="7" t="s">
         <v>1060</v>
       </c>
-      <c r="KS71" s="7" t="s">
+      <c r="KS72" s="7" t="s">
         <v>1074</v>
       </c>
     </row>
-    <row r="72" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+    <row r="73" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A73" s="4" t="s">
         <v>1061</v>
       </c>
-      <c r="KS72" s="4" t="s">
+      <c r="KS73" s="4" t="s">
         <v>1033</v>
       </c>
     </row>
-    <row r="73" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+    <row r="74" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A74" s="4" t="s">
         <v>1088</v>
       </c>
-      <c r="KS73" s="4" t="b">
+      <c r="KS74" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+    <row r="75" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A75" s="4" t="s">
         <v>1062</v>
       </c>
     </row>
-    <row r="75" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+    <row r="76" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="4" t="s">
         <v>1063</v>
-      </c>
-      <c r="KS75" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="76" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>1064</v>
       </c>
       <c r="KS76" s="4" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="77" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+    <row r="77" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A77" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="KS77" s="4" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="78" spans="1:305" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A78" s="7" t="s">
         <v>1065</v>
       </c>
-      <c r="KS77" s="7" t="s">
+      <c r="KS78" s="7" t="s">
         <v>1075</v>
       </c>
     </row>
-    <row r="78" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+    <row r="79" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="4" t="s">
         <v>1066</v>
       </c>
-      <c r="KS78" s="4" t="s">
+      <c r="KS79" s="4" t="s">
         <v>1028</v>
       </c>
     </row>
-    <row r="79" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
+    <row r="80" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A80" s="4" t="s">
         <v>1087</v>
       </c>
-      <c r="KS79" s="4" t="b">
+      <c r="KS80" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:305" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="4" t="s">
+    <row r="81" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A81" s="4" t="s">
         <v>1067</v>
       </c>
     </row>
-    <row r="81" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+    <row r="82" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A82" s="4" t="s">
         <v>1068</v>
-      </c>
-      <c r="KS81" s="4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="82" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>1069</v>
       </c>
       <c r="KS82" s="4" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="83" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+    <row r="83" spans="1:338" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A83" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="KS83" s="4" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="84" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A84" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AM83" s="5" t="s">
+      <c r="AM84" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="BL83" s="5" t="s">
+      <c r="BL84" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="DU83" s="5" t="s">
+      <c r="DU84" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="FH83" s="5" t="s">
+      <c r="FH84" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="JW83" s="5" t="s">
+      <c r="JW84" s="5" t="s">
         <v>904</v>
       </c>
-      <c r="KT83" s="5" t="s">
+      <c r="KT84" s="5" t="s">
         <v>987</v>
       </c>
-      <c r="LM83" s="5" t="s">
+      <c r="LM84" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="LP83" s="5" t="s">
+      <c r="LP84" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="84" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+    <row r="85" spans="1:338" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A85" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AM84" s="5" t="s">
+      <c r="AM85" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="BL84" s="5">
+      <c r="BL85" s="5">
         <v>1</v>
       </c>
-      <c r="DU84" s="5">
+      <c r="DU85" s="5">
         <v>1</v>
       </c>
-      <c r="FH84" s="5">
+      <c r="FH85" s="5">
         <v>1</v>
       </c>
-      <c r="JW84" s="5">
+      <c r="JW85" s="5">
         <v>4</v>
       </c>
-      <c r="KT84" s="5" t="s">
+      <c r="KT85" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="LM84" s="5" t="s">
+      <c r="LM85" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="LP84" s="5">
+      <c r="LP85" s="5">
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="8" t="s">
+    <row r="86" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A86" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="HT85" s="8" t="s">
+      <c r="HT86" s="8" t="s">
         <v>718</v>
       </c>
-      <c r="JX85" s="8" t="s">
+      <c r="JX86" s="8" t="s">
         <v>718</v>
       </c>
-      <c r="LN85" s="8" t="s">
+      <c r="LN86" s="8" t="s">
         <v>718</v>
       </c>
-      <c r="LP85" s="8" t="s">
+      <c r="LP86" s="8" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="86" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
+    <row r="87" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A87" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="HT86" s="6">
+      <c r="HT87" s="6">
         <v>1</v>
       </c>
-      <c r="JX86" s="6">
+      <c r="JX87" s="6">
         <v>2</v>
       </c>
-      <c r="LN86" s="6">
+      <c r="LN87" s="6">
         <v>8</v>
       </c>
-      <c r="LP86" s="6">
+      <c r="LP87" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
+    <row r="88" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A88" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="HT87" s="6" t="s">
+      <c r="HT88" s="6" t="s">
         <v>717</v>
       </c>
-      <c r="JX87" s="6" t="s">
+      <c r="JX88" s="6" t="s">
         <v>907</v>
       </c>
-      <c r="LN87" s="6" t="s">
+      <c r="LN88" s="6" t="s">
         <v>1022</v>
       </c>
-      <c r="LP87" s="6" t="s">
+      <c r="LP88" s="6" t="s">
         <v>1110</v>
       </c>
     </row>
-    <row r="88" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
+    <row r="89" spans="1:338" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A89" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="HT88" s="8" t="s">
+      <c r="HT89" s="8" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="89" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
+    <row r="90" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A90" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="HT89" s="6">
+      <c r="HT90" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
+    <row r="91" spans="1:338" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A91" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="HT90" s="6" t="s">
+      <c r="HT91" s="6" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="91" spans="1:338" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:338" x14ac:dyDescent="0.45">
+      <c r="A92" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="JX91" s="1" t="s">
+      <c r="JX92" s="1" t="s">
         <v>908</v>
       </c>
     </row>
-    <row r="92" spans="1:338" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:338" x14ac:dyDescent="0.45">
+      <c r="A93" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="IP92" s="1">
+      <c r="IP93" s="1">
         <v>6</v>
       </c>
-      <c r="JT92" s="1">
+      <c r="JT93" s="1">
         <v>5</v>
       </c>
-      <c r="KS92" s="1">
+      <c r="KS93" s="1">
         <v>3</v>
       </c>
-      <c r="LG92" s="1">
+      <c r="LG93" s="1">
         <v>6</v>
       </c>
-      <c r="LZ92" s="1">
+      <c r="LZ93" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:338" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="94" spans="1:338" x14ac:dyDescent="0.45">
+      <c r="A94" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="IP93" s="1" t="s">
+      <c r="IP94" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="JT93" s="1" t="s">
+      <c r="JT94" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="KS93" s="1" t="s">
+      <c r="KS94" s="1" t="s">
         <v>991</v>
       </c>
-      <c r="LG93" s="1" t="s">
+      <c r="LG94" s="1" t="s">
         <v>1096</v>
       </c>
-      <c r="LZ93" s="1" t="s">
+      <c r="LZ94" s="1" t="s">
         <v>1130</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A85:KG93">
-    <sortCondition ref="A85:A93"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A86:KG94">
+    <sortCondition ref="A86:A94"/>
   </sortState>
   <conditionalFormatting sqref="LT1:LW1 A1:LR1 MD1 MG1:XFD1">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>

</xml_diff>